<commit_message>
Added tutorial lines and removed test convo
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{000DFE13-AF50-4FA3-8EF4-9A892935BAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2112F4-3CCC-4D9E-A00A-EBC2F0DA9326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
   <si>
     <t>Context</t>
   </si>
@@ -44,15 +44,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>brrrt</t>
-  </si>
-  <si>
-    <t>zazaza</t>
-  </si>
-  <si>
-    <t>yoink</t>
-  </si>
-  <si>
     <t>Placeholder</t>
   </si>
   <si>
@@ -80,66 +71,9 @@
     <t>ExtraData</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
-    <t>Start of test conversation</t>
-  </si>
-  <si>
-    <t>Reply to Jessica</t>
-  </si>
-  <si>
-    <t>2nd line of convo</t>
-  </si>
-  <si>
-    <t>Hey Jessica, knock knock?</t>
-  </si>
-  <si>
-    <t>... Who's there?</t>
-  </si>
-  <si>
-    <t>bob_start_joke</t>
-  </si>
-  <si>
-    <t>bob_joke_question</t>
-  </si>
-  <si>
-    <t>bob_punchline</t>
-  </si>
-  <si>
-    <t>Old lady.</t>
-  </si>
-  <si>
-    <t>Old lady who?</t>
-  </si>
-  <si>
-    <t>Didn't know there was a yodeller!</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Can we kill this guy?</t>
-  </si>
-  <si>
-    <t>jessica_reply1</t>
-  </si>
-  <si>
-    <t>jessica_reply2</t>
-  </si>
-  <si>
-    <t>jessica_silent</t>
-  </si>
-  <si>
-    <t>jessica_player_question</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -155,13 +89,187 @@
     <t>CharacterID</t>
   </si>
   <si>
-    <t>Ah, alright.</t>
-  </si>
-  <si>
-    <t>After player says no</t>
-  </si>
-  <si>
-    <t>jessica_cant_kill_bob</t>
+    <t>First line of tutorial</t>
+  </si>
+  <si>
+    <t>Wake up sunshine… you fell asleep while playing games.</t>
+  </si>
+  <si>
+    <t>Me and your Dad are going to get some ice cream.</t>
+  </si>
+  <si>
+    <t>What flavour of ice cream do you want?</t>
+  </si>
+  <si>
+    <t>First question</t>
+  </si>
+  <si>
+    <t>Vanilla</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Strawberry</t>
+  </si>
+  <si>
+    <t>Player choices</t>
+  </si>
+  <si>
+    <t>Tutorial_Mom</t>
+  </si>
+  <si>
+    <t>Tutorial_Dad</t>
+  </si>
+  <si>
+    <t>p_0_vanilla</t>
+  </si>
+  <si>
+    <t>p_0_chocolate</t>
+  </si>
+  <si>
+    <t>p_0_strawberry</t>
+  </si>
+  <si>
+    <t>tutmom_0_wake_up</t>
+  </si>
+  <si>
+    <t>tutmom_0_going_ice_cream</t>
+  </si>
+  <si>
+    <t>tutdad_0_q_ice_cream</t>
+  </si>
+  <si>
+    <t>Okay, we don't take long.</t>
+  </si>
+  <si>
+    <t>Response to player choice</t>
+  </si>
+  <si>
+    <t>tutdad_0_question_response</t>
+  </si>
+  <si>
+    <t>(To Mom) Have you seen where the car keys are?</t>
+  </si>
+  <si>
+    <t>tutdad_0_where_are_keys</t>
+  </si>
+  <si>
+    <t>Being sent out to scavenge</t>
+  </si>
+  <si>
+    <t>tutdad_0_scavenge_response</t>
+  </si>
+  <si>
+    <t>We're back!</t>
+  </si>
+  <si>
+    <t>At door</t>
+  </si>
+  <si>
+    <t>tutmom_0_q_open_door</t>
+  </si>
+  <si>
+    <t>tutmom_0_at_door</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>These lines show some formatting stuff</t>
+  </si>
+  <si>
+    <t>Heres some useful internal notes</t>
+  </si>
+  <si>
+    <t>test_0_dont_use_caps_in_ids</t>
+  </si>
+  <si>
+    <t>test_0_use_name_then_day</t>
+  </si>
+  <si>
+    <t>Did I ever tell you the definition... Of insanity?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let me ask you something... </t>
+  </si>
+  <si>
+    <t>Thank you kiddo...  see you soon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hey kiddo, can you open the door please? It's raining out here... </t>
+  </si>
+  <si>
+    <t>idk something can go here</t>
+  </si>
+  <si>
+    <t>Export as TSV (tab seperated values)</t>
+  </si>
+  <si>
+    <t>test_0_main_chars_only_use_one_letter</t>
+  </si>
+  <si>
+    <t>Dialogue is so cool.</t>
+  </si>
+  <si>
+    <t>I got nothin</t>
+  </si>
+  <si>
+    <t>test_0_q_questions_have_a_q_first</t>
+  </si>
+  <si>
+    <t>Extra stuff</t>
+  </si>
+  <si>
+    <t>Can</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>Open Door</t>
+  </si>
+  <si>
+    <t>Keep Door Closed</t>
+  </si>
+  <si>
+    <t>Basic prompts that are used often</t>
+  </si>
+  <si>
+    <t>player_open_door</t>
+  </si>
+  <si>
+    <t>player_keep_door_closed</t>
+  </si>
+  <si>
+    <t>Hehe, nice one... Really though, it is quite cold.</t>
+  </si>
+  <si>
+    <t>Player keeps door closed</t>
+  </si>
+  <si>
+    <t>tutmom_0_q_open_door_second</t>
+  </si>
+  <si>
+    <t>Kiddo?</t>
+  </si>
+  <si>
+    <t>Player keeps door closed again</t>
+  </si>
+  <si>
+    <t>tutmom_0_door_closed_twice</t>
+  </si>
+  <si>
+    <t>Thanks kiddo, now let's eat some ice cream!</t>
+  </si>
+  <si>
+    <t>Player lets them in</t>
+  </si>
+  <si>
+    <t>tutdad_0_lets_eat</t>
   </si>
 </sst>
 </file>
@@ -297,10 +405,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -600,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,10 +724,10 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -632,231 +736,516 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
         <v>40</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -884,6 +1273,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -1122,24 +1528,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1156,29 +1570,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed "Tab Seperated Values" to "Tab Delimited"
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2112F4-3CCC-4D9E-A00A-EBC2F0DA9326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7477DFC6-C737-484E-9276-7ED2607915DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -203,9 +203,6 @@
     <t>idk something can go here</t>
   </si>
   <si>
-    <t>Export as TSV (tab seperated values)</t>
-  </si>
-  <si>
     <t>test_0_main_chars_only_use_one_letter</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>tutdad_0_lets_eat</t>
+  </si>
+  <si>
+    <t>Export as TSV (tab delimited)</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -797,7 +797,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,13 +808,13 @@
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -823,7 +823,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -831,16 +831,16 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -849,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -900,13 +900,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -920,13 +920,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -1184,16 +1184,16 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
         <v>69</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
         <v>70</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -1207,16 +1207,16 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
         <v>73</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>74</v>
       </c>
       <c r="F25" t="s">
         <v>2</v>
@@ -1230,16 +1230,16 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
         <v>75</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>76</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>77</v>
       </c>
       <c r="F26" t="s">
         <v>2</v>
@@ -1273,20 +1273,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1529,6 +1529,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1541,14 +1549,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed one spelling error
Replaced "Don't" with "Won't"
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7477DFC6-C737-484E-9276-7ED2607915DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4035E36C-9372-49FC-9015-8710FFEC7776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -140,9 +140,6 @@
     <t>tutdad_0_q_ice_cream</t>
   </si>
   <si>
-    <t>Okay, we don't take long.</t>
-  </si>
-  <si>
     <t>Response to player choice</t>
   </si>
   <si>
@@ -269,7 +266,10 @@
     <t>tutdad_0_lets_eat</t>
   </si>
   <si>
-    <t>Export as TSV (tab delimited)</t>
+    <t>Okay, we won't take long.</t>
+  </si>
+  <si>
+    <t>Export: Save as Text (tab delimited)</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,19 +750,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -771,24 +771,24 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -797,15 +797,15 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>77</v>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -823,24 +823,24 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -849,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -900,13 +900,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -920,13 +920,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -1075,16 +1075,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
         <v>35</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>36</v>
       </c>
       <c r="F19" t="s">
         <v>2</v>
@@ -1098,13 +1098,13 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
         <v>37</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>38</v>
       </c>
       <c r="F20" t="s">
         <v>2</v>
@@ -1118,16 +1118,16 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
         <v>39</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>40</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
@@ -1141,16 +1141,16 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
         <v>2</v>
@@ -1164,13 +1164,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
         <v>2</v>
@@ -1184,16 +1184,16 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
         <v>69</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>70</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -1207,16 +1207,16 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
         <v>72</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>73</v>
       </c>
       <c r="F25" t="s">
         <v>2</v>
@@ -1230,16 +1230,16 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
         <v>74</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>75</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>76</v>
       </c>
       <c r="F26" t="s">
         <v>2</v>
@@ -1273,20 +1273,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1529,14 +1529,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1549,6 +1541,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Created conversations and added support for callbacks when convos are finished
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4035E36C-9372-49FC-9015-8710FFEC7776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52BB685-6075-41E3-8707-B799F22C31B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>First line of tutorial</t>
   </si>
   <si>
-    <t>Wake up sunshine… you fell asleep while playing games.</t>
-  </si>
-  <si>
     <t>Me and your Dad are going to get some ice cream.</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>Export: Save as Text (tab delimited)</t>
+  </si>
+  <si>
+    <t>Wake up sunshine...  you fell asleep while playing games.</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,19 +750,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -771,24 +771,24 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -797,24 +797,24 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -823,24 +823,24 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -849,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -900,13 +900,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -920,13 +920,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -937,10 +937,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -949,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
         <v>2</v>
@@ -960,16 +960,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
         <v>2</v>
@@ -980,19 +980,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
         <v>2</v>
@@ -1006,16 +1006,16 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
         <v>2</v>
@@ -1029,16 +1029,16 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
         <v>2</v>
@@ -1052,16 +1052,16 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -1072,19 +1072,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
         <v>34</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
       </c>
       <c r="F19" t="s">
         <v>2</v>
@@ -1095,16 +1095,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
         <v>36</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>37</v>
       </c>
       <c r="F20" t="s">
         <v>2</v>
@@ -1115,19 +1115,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
         <v>38</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
@@ -1138,19 +1138,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
         <v>2</v>
@@ -1161,16 +1161,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" t="s">
         <v>2</v>
@@ -1181,19 +1181,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
         <v>68</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -1204,19 +1204,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
         <v>71</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
       </c>
       <c r="F25" t="s">
         <v>2</v>
@@ -1227,19 +1227,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>74</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>75</v>
       </c>
       <c r="F26" t="s">
         <v>2</v>
@@ -1273,20 +1273,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1529,6 +1529,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1541,14 +1549,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added lines to auto-generate character IDs
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Tech\Github Repos\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52BB685-6075-41E3-8707-B799F22C31B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9985ABE-855E-4F1A-97AC-0CFBC4B0C7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
+    <workbookView xWindow="4740" yWindow="2955" windowWidth="28800" windowHeight="15885" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="105">
   <si>
     <t>Context</t>
   </si>
@@ -119,15 +119,6 @@
     <t>Tutorial_Dad</t>
   </si>
   <si>
-    <t>p_0_vanilla</t>
-  </si>
-  <si>
-    <t>p_0_chocolate</t>
-  </si>
-  <si>
-    <t>p_0_strawberry</t>
-  </si>
-  <si>
     <t>tutmom_0_wake_up</t>
   </si>
   <si>
@@ -270,6 +261,96 @@
   </si>
   <si>
     <t>Wake up sunshine...  you fell asleep while playing games.</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Violet</t>
+  </si>
+  <si>
+    <t>Hal</t>
+  </si>
+  <si>
+    <t>Sal</t>
+  </si>
+  <si>
+    <t>Dad</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>Neighbour</t>
+  </si>
+  <si>
+    <t>Journalist</t>
+  </si>
+  <si>
+    <t>Character Define</t>
+  </si>
+  <si>
+    <t>Used to generate Character IDs</t>
+  </si>
+  <si>
+    <t>^^^ before they have any lines</t>
+  </si>
+  <si>
+    <t>player_0_vanilla</t>
+  </si>
+  <si>
+    <t>player_0_chocolate</t>
+  </si>
+  <si>
+    <t>player_0_strawberry</t>
+  </si>
+  <si>
+    <t>none_chardefine</t>
+  </si>
+  <si>
+    <t>player_chardefine</t>
+  </si>
+  <si>
+    <t>tutmom_chardefine</t>
+  </si>
+  <si>
+    <t>tutdad_chardefine</t>
+  </si>
+  <si>
+    <t>j_chardefine</t>
+  </si>
+  <si>
+    <t>b_chardefine</t>
+  </si>
+  <si>
+    <t>v_chardefine</t>
+  </si>
+  <si>
+    <t>h_chardefine</t>
+  </si>
+  <si>
+    <t>s_chardefine</t>
+  </si>
+  <si>
+    <t>bear_chardefine</t>
+  </si>
+  <si>
+    <t>raiders_chardefine</t>
+  </si>
+  <si>
+    <t>neighbour_chardefine</t>
+  </si>
+  <si>
+    <t>journalist_chardefine</t>
+  </si>
+  <si>
+    <t>dad_chardefine</t>
   </si>
 </sst>
 </file>
@@ -327,7 +408,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
     <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
@@ -393,6 +474,98 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -704,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,19 +923,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -771,24 +944,24 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -797,24 +970,24 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -823,24 +996,24 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -849,47 +1022,27 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -900,16 +1053,19 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
@@ -917,42 +1073,91 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="F13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
@@ -960,19 +1165,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="F14" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -980,22 +1188,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
@@ -1003,22 +1211,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
@@ -1026,22 +1234,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="F17" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
@@ -1049,22 +1257,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
@@ -1072,22 +1280,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="F19" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
@@ -1095,19 +1303,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="F20" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
@@ -1115,157 +1326,465 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s">
         <v>37</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
         <v>38</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F45" t="s">
         <v>2</v>
       </c>
-      <c r="G21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" t="s">
         <v>2</v>
       </c>
-      <c r="G22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="G46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" t="s">
         <v>2</v>
       </c>
-      <c r="G23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" t="s">
         <v>2</v>
       </c>
-      <c r="G24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" t="s">
-        <v>2</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="G48" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H1048576">
+  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 A40:H1048576 H7:H39 A29:G48 E8:E21 A8:C21">
+    <cfRule type="expression" dxfId="6" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G6 F29:G1048576">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D21">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:G21">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1048576">
+  <conditionalFormatting sqref="F8:G21">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Final">
-      <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Final",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Draft">
-      <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Draft",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("None",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1273,20 +1792,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1529,14 +2048,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1549,6 +2060,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added lines for looking for keys
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Tech\Github Repos\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9985ABE-855E-4F1A-97AC-0CFBC4B0C7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCCDA9F-FC3E-41DC-A375-EA43C2A7CAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="2955" windowWidth="28800" windowHeight="15885" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
+    <workbookView xWindow="2250" yWindow="2430" windowWidth="28800" windowHeight="15885" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="110">
   <si>
     <t>Context</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>dad_chardefine</t>
+  </si>
+  <si>
+    <t>I don't know where we left them...</t>
+  </si>
+  <si>
+    <t>I could've swore they were around here somewhere!</t>
+  </si>
+  <si>
+    <t>If you try to talk to them before finding keys</t>
+  </si>
+  <si>
+    <t>tutdad_0_looking_for_keys</t>
+  </si>
+  <si>
+    <t>tutmom_0_looking_for_keys</t>
   </si>
 </sst>
 </file>
@@ -408,7 +423,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
@@ -501,72 +556,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -581,9 +570,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -621,7 +610,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -727,7 +716,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -869,7 +858,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -877,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,16 +1602,16 @@
         <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="F43" t="s">
         <v>2</v>
@@ -1636,16 +1625,16 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="F44" t="s">
         <v>2</v>
@@ -1656,16 +1645,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
+        <v>34</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F45" t="s">
         <v>2</v>
@@ -1679,16 +1671,16 @@
         <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="F46" t="s">
         <v>2</v>
@@ -1702,16 +1694,13 @@
         <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="F47" t="s">
         <v>2</v>
@@ -1722,19 +1711,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F48" t="s">
         <v>2</v>
@@ -1743,34 +1732,75 @@
         <v>5</v>
       </c>
     </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>68</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" t="s">
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 A40:H1048576 H7:H39 A29:G48 E8:E21 A8:C21">
-    <cfRule type="expression" dxfId="6" priority="11">
+  <conditionalFormatting sqref="A8:G21">
+    <cfRule type="expression" dxfId="9" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 H7:H39 A29:G48 A40:H1048576">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G6 F29:G1048576">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D21">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8:G21">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:G21">
@@ -1792,20 +1822,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2048,6 +2078,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2060,14 +2098,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added scavenge responses, improved line importer
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Tech\Github Repos\BeyondTheDoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCCDA9F-FC3E-41DC-A375-EA43C2A7CAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164DE663-F606-49B2-8045-87ED5C0BE7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2430" windowWidth="28800" windowHeight="15885" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="118">
   <si>
     <t>Context</t>
   </si>
@@ -80,12 +80,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>player_yes</t>
-  </si>
-  <si>
-    <t>player_no</t>
-  </si>
-  <si>
     <t>CharacterID</t>
   </si>
   <si>
@@ -212,21 +206,6 @@
     <t>Here</t>
   </si>
   <si>
-    <t>Open Door</t>
-  </si>
-  <si>
-    <t>Keep Door Closed</t>
-  </si>
-  <si>
-    <t>Basic prompts that are used often</t>
-  </si>
-  <si>
-    <t>player_open_door</t>
-  </si>
-  <si>
-    <t>player_keep_door_closed</t>
-  </si>
-  <si>
     <t>Hehe, nice one... Really though, it is quite cold.</t>
   </si>
   <si>
@@ -296,12 +275,6 @@
     <t>Character Define</t>
   </si>
   <si>
-    <t>Used to generate Character IDs</t>
-  </si>
-  <si>
-    <t>^^^ before they have any lines</t>
-  </si>
-  <si>
     <t>player_0_vanilla</t>
   </si>
   <si>
@@ -366,6 +339,57 @@
   </si>
   <si>
     <t>tutmom_0_looking_for_keys</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>These just make sure that all characters are "defined" even if they have no lines yet</t>
+  </si>
+  <si>
+    <t>Tutorial/day 0</t>
+  </si>
+  <si>
+    <t>Lines with no character</t>
+  </si>
+  <si>
+    <t>open_door</t>
+  </si>
+  <si>
+    <t>keep_door_closed</t>
+  </si>
+  <si>
+    <t>Send {character} to scavenge</t>
+  </si>
+  <si>
+    <t>Open door</t>
+  </si>
+  <si>
+    <t>Keep door closed</t>
+  </si>
+  <si>
+    <t>send_to_scavenge</t>
+  </si>
+  <si>
+    <t>Stay silent</t>
+  </si>
+  <si>
+    <t>These are basic prompts that are used repeatedly (as choices)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>stay_silent</t>
+  </si>
+  <si>
+    <t>Go back</t>
+  </si>
+  <si>
+    <t>go_back</t>
   </si>
 </sst>
 </file>
@@ -423,7 +447,73 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
@@ -868,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +976,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -912,19 +1002,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -933,24 +1023,24 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -959,24 +1049,24 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -985,24 +1075,24 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1011,7 +1101,15 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,16 +1117,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
@@ -1042,16 +1140,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -1062,19 +1157,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
@@ -1085,19 +1177,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>85</v>
-      </c>
-      <c r="C11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>94</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
@@ -1108,19 +1197,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
         <v>86</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>95</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
@@ -1131,19 +1217,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
         <v>87</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>96</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -1154,19 +1237,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -1177,19 +1257,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="B15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" t="s">
-        <v>87</v>
-      </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -1200,19 +1277,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -1223,19 +1297,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -1246,19 +1317,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
@@ -1269,19 +1337,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -1292,19 +1357,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
@@ -1315,24 +1377,109 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
       </c>
       <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1341,16 +1488,13 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -1364,13 +1508,13 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
@@ -1384,13 +1528,13 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="F31" t="s">
         <v>4</v>
@@ -1399,41 +1543,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" t="s">
-        <v>5</v>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
         <v>25</v>
-      </c>
-      <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>27</v>
       </c>
       <c r="F35" t="s">
         <v>2</v>
@@ -1444,16 +1576,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F36" t="s">
         <v>2</v>
@@ -1464,19 +1596,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
         <v>2</v>
@@ -1490,16 +1622,16 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F38" t="s">
         <v>2</v>
@@ -1513,16 +1645,16 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
         <v>22</v>
       </c>
-      <c r="C39" t="s">
-        <v>24</v>
-      </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F39" t="s">
         <v>2</v>
@@ -1536,16 +1668,16 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F40" t="s">
         <v>2</v>
@@ -1556,19 +1688,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F41" t="s">
         <v>2</v>
@@ -1579,16 +1711,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F42" t="s">
         <v>2</v>
@@ -1599,19 +1731,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
         <v>2</v>
@@ -1622,19 +1754,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F44" t="s">
         <v>2</v>
@@ -1645,19 +1777,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F45" t="s">
         <v>2</v>
@@ -1668,19 +1800,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
         <v>37</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>39</v>
       </c>
       <c r="F46" t="s">
         <v>2</v>
@@ -1691,16 +1823,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>35</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F47" t="s">
         <v>2</v>
@@ -1711,19 +1846,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F48" t="s">
         <v>2</v>
@@ -1734,19 +1869,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F49" t="s">
         <v>2</v>
@@ -1757,19 +1892,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F50" t="s">
         <v>2</v>
@@ -1779,42 +1914,62 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <conditionalFormatting sqref="A8:G21">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="14" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 H7:H39 A29:G48 A40:H1048576">
-    <cfRule type="expression" dxfId="8" priority="11">
+  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 H7:H39 A30:G48 A7:B7 B29:G29 A27:A29 A40:H1048576">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G6 F29:G1048576">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:G21">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F8)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:G26 B27:G28">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:G28">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F25)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("None",F25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1822,20 +1977,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2078,14 +2233,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2098,6 +2245,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Stored the current speaking character
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164DE663-F606-49B2-8045-87ED5C0BE7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0D91D-8DC4-48D8-AAEF-EC4D4C13CDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -489,32 +489,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
       </font>
@@ -593,6 +567,32 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -959,7 +959,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,45 +1920,45 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 H7:H39 A30:G48 A7:B7 B29:G29 A27:A29 A40:H1048576">
-    <cfRule type="expression" dxfId="13" priority="16">
+  <conditionalFormatting sqref="A25:G48">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G6 F29:G1048576">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Final">
+  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 A7:B7 H7:H39 A40:H1048576">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G6">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:G21">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25:G26 B27:G28">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25:G28">
+  <conditionalFormatting sqref="F25:G1048576">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F25)))</formula>
     </cfRule>
@@ -1977,20 +1977,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2233,6 +2233,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2245,14 +2253,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Created improved excel pipeline
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Tech\Github Repos\BeyondTheDoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCCDA9F-FC3E-41DC-A375-EA43C2A7CAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A443099-4C7F-4C0D-802C-AB76685AC94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2430" windowWidth="28800" windowHeight="15885" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
+    <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="144">
   <si>
     <t>Context</t>
   </si>
@@ -80,12 +80,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>player_yes</t>
-  </si>
-  <si>
-    <t>player_no</t>
-  </si>
-  <si>
     <t>CharacterID</t>
   </si>
   <si>
@@ -191,9 +185,6 @@
     <t>test_0_main_chars_only_use_one_letter</t>
   </si>
   <si>
-    <t>Dialogue is so cool.</t>
-  </si>
-  <si>
     <t>I got nothin</t>
   </si>
   <si>
@@ -212,21 +203,6 @@
     <t>Here</t>
   </si>
   <si>
-    <t>Open Door</t>
-  </si>
-  <si>
-    <t>Keep Door Closed</t>
-  </si>
-  <si>
-    <t>Basic prompts that are used often</t>
-  </si>
-  <si>
-    <t>player_open_door</t>
-  </si>
-  <si>
-    <t>player_keep_door_closed</t>
-  </si>
-  <si>
     <t>Hehe, nice one... Really though, it is quite cold.</t>
   </si>
   <si>
@@ -296,12 +272,6 @@
     <t>Character Define</t>
   </si>
   <si>
-    <t>Used to generate Character IDs</t>
-  </si>
-  <si>
-    <t>^^^ before they have any lines</t>
-  </si>
-  <si>
     <t>player_0_vanilla</t>
   </si>
   <si>
@@ -366,6 +336,138 @@
   </si>
   <si>
     <t>tutmom_0_looking_for_keys</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>These just make sure that all characters are "defined" even if they have no lines yet</t>
+  </si>
+  <si>
+    <t>Tutorial/day 0</t>
+  </si>
+  <si>
+    <t>Lines with no character</t>
+  </si>
+  <si>
+    <t>open_door</t>
+  </si>
+  <si>
+    <t>keep_door_closed</t>
+  </si>
+  <si>
+    <t>Send {character} to scavenge</t>
+  </si>
+  <si>
+    <t>Open door</t>
+  </si>
+  <si>
+    <t>Keep door closed</t>
+  </si>
+  <si>
+    <t>send_to_scavenge</t>
+  </si>
+  <si>
+    <t>Stay silent</t>
+  </si>
+  <si>
+    <t>These are basic prompts that are used repeatedly (as choices)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>stay_silent</t>
+  </si>
+  <si>
+    <t>Go back</t>
+  </si>
+  <si>
+    <t>go_back</t>
+  </si>
+  <si>
+    <t>Look through peephole</t>
+  </si>
+  <si>
+    <t>Make decision</t>
+  </si>
+  <si>
+    <t>Ask questions</t>
+  </si>
+  <si>
+    <t>"Who are you?"</t>
+  </si>
+  <si>
+    <t>"What do you want?"</t>
+  </si>
+  <si>
+    <t>"Why should I let you in?"</t>
+  </si>
+  <si>
+    <t>"How can you be helpful to me?"</t>
+  </si>
+  <si>
+    <t>look_through_peephole</t>
+  </si>
+  <si>
+    <t>make_decision</t>
+  </si>
+  <si>
+    <t>ask_questions</t>
+  </si>
+  <si>
+    <t>who_are_you</t>
+  </si>
+  <si>
+    <t>what_do_you_want</t>
+  </si>
+  <si>
+    <t>why_should_i_let_you_in</t>
+  </si>
+  <si>
+    <t>how_can_you_be_helpful</t>
+  </si>
+  <si>
+    <t>This is where the spoken text goes (or the conversation name - see below)</t>
+  </si>
+  <si>
+    <t>For internal use</t>
+  </si>
+  <si>
+    <t>That left column is for characters (case sensitive) and special markers</t>
+  </si>
+  <si>
+    <t>CONVERSATION</t>
+  </si>
+  <si>
+    <t>CHOICE</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>WakeUp</t>
+  </si>
+  <si>
+    <t>LookForKeys</t>
+  </si>
+  <si>
+    <t>GoScavenge</t>
+  </si>
+  <si>
+    <t>AtDoor</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>AtDoor2</t>
+  </si>
+  <si>
+    <t>JokeEnding</t>
   </si>
 </sst>
 </file>
@@ -423,87 +525,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <fill>
         <gradientFill degree="90">
@@ -531,6 +553,190 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <gradientFill degree="90">
           <stop position="0">
@@ -540,6 +746,540 @@
             <color theme="2"/>
           </stop>
         </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
       </fill>
       <border>
         <left style="dotted">
@@ -866,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +1626,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -912,91 +1652,76 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1005,53 +1730,64 @@
         <v>50</v>
       </c>
       <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
-        <v>57</v>
+      <c r="H6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -1062,19 +1798,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
@@ -1085,19 +1818,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
@@ -1108,19 +1838,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
@@ -1131,19 +1858,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
         <v>85</v>
-      </c>
-      <c r="C13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>96</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -1154,19 +1878,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
         <v>86</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>97</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -1177,19 +1898,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>87</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>98</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -1200,19 +1918,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -1223,19 +1938,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -1246,19 +1958,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
@@ -1269,19 +1978,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -1292,19 +1998,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
@@ -1315,24 +2018,109 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
       </c>
       <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1341,16 +2129,13 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -1364,13 +2149,13 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
@@ -1384,13 +2169,13 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="F31" t="s">
         <v>4</v>
@@ -1404,13 +2189,13 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
@@ -1419,24 +2204,64 @@
         <v>5</v>
       </c>
     </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="F35" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
@@ -1444,19 +2269,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="F36" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
@@ -1464,22 +2289,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="F37" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
@@ -1490,19 +2312,16 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="F38" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
@@ -1513,217 +2332,55 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="F39" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>90</v>
-      </c>
-      <c r="F40" t="s">
-        <v>2</v>
-      </c>
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>31</v>
-      </c>
-      <c r="F41" t="s">
-        <v>2</v>
-      </c>
-      <c r="G41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>33</v>
-      </c>
-      <c r="F42" t="s">
-        <v>2</v>
-      </c>
-      <c r="G42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" t="s">
-        <v>107</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>108</v>
-      </c>
-      <c r="F43" t="s">
-        <v>2</v>
-      </c>
-      <c r="G43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F44" t="s">
-        <v>2</v>
-      </c>
-      <c r="G44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" t="s">
-        <v>2</v>
-      </c>
-      <c r="G45" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F46" t="s">
-        <v>2</v>
-      </c>
-      <c r="G46" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="D47">
         <v>0</v>
-      </c>
-      <c r="E47" t="s">
-        <v>38</v>
-      </c>
-      <c r="F47" t="s">
-        <v>2</v>
-      </c>
-      <c r="G47" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
         <v>25</v>
-      </c>
-      <c r="B48" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>65</v>
       </c>
       <c r="F48" t="s">
         <v>2</v>
@@ -1734,19 +2391,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="F49" t="s">
         <v>2</v>
@@ -1757,19 +2411,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="F50" t="s">
         <v>2</v>
@@ -1778,43 +2432,510 @@
         <v>5</v>
       </c>
     </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" t="s">
+        <v>2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" t="s">
+        <v>2</v>
+      </c>
+      <c r="G62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" t="s">
+        <v>2</v>
+      </c>
+      <c r="G63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>99</v>
+      </c>
+      <c r="F64" t="s">
+        <v>2</v>
+      </c>
+      <c r="G64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>33</v>
+      </c>
+      <c r="F70" t="s">
+        <v>2</v>
+      </c>
+      <c r="G70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>37</v>
+      </c>
+      <c r="F75" t="s">
+        <v>2</v>
+      </c>
+      <c r="G75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>36</v>
+      </c>
+      <c r="F76" t="s">
+        <v>2</v>
+      </c>
+      <c r="G76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>135</v>
+      </c>
+      <c r="B77" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" t="s">
+        <v>142</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" t="s">
+        <v>56</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>57</v>
+      </c>
+      <c r="F85" t="s">
+        <v>2</v>
+      </c>
+      <c r="G85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>135</v>
+      </c>
+      <c r="B86" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>135</v>
+      </c>
+      <c r="B88" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>134</v>
+      </c>
+      <c r="B93" t="s">
+        <v>143</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" t="s">
+        <v>58</v>
+      </c>
+      <c r="C94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>60</v>
+      </c>
+      <c r="F94" t="s">
+        <v>2</v>
+      </c>
+      <c r="G94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>134</v>
+      </c>
+      <c r="B98" t="s">
+        <v>141</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" t="s">
+        <v>61</v>
+      </c>
+      <c r="C99" t="s">
+        <v>62</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>63</v>
+      </c>
+      <c r="F99" t="s">
+        <v>2</v>
+      </c>
+      <c r="G99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A8:G21">
-    <cfRule type="expression" dxfId="9" priority="5">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H3 A4 C4:H4 A5:H6 H7:H39 A29:G48 A40:H1048576">
-    <cfRule type="expression" dxfId="8" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G6 F29:G1048576">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Final">
+  <dataConsolidate/>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:G21">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Final">
-      <formula>NOT(ISERROR(SEARCH("Final",F8)))</formula>
+  <conditionalFormatting sqref="A1:H1048576">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Draft">
-      <formula>NOT(ISERROR(SEARCH("Draft",F8)))</formula>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F8)))</formula>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F8)))</formula>
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$A1="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1822,20 +2943,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2078,14 +3199,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2098,6 +3211,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added 2 first lines for day 1
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A443099-4C7F-4C0D-802C-AB76685AC94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D3C85F-DFF7-4B3F-8210-81C04F74FF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="152">
   <si>
     <t>Context</t>
   </si>
@@ -468,6 +468,30 @@
   </si>
   <si>
     <t>JokeEnding</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Uuuuugh. If the sound continues I will have to hide again under the bed</t>
+  </si>
+  <si>
+    <t>player woke up</t>
+  </si>
+  <si>
+    <t>Wake_up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player </t>
+  </si>
+  <si>
+    <t>p1_wakeup</t>
+  </si>
+  <si>
+    <t>Another dream huh, what can I do for today</t>
+  </si>
+  <si>
+    <t>p1_choosing</t>
   </si>
 </sst>
 </file>
@@ -490,7 +514,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -500,6 +524,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,616 +546,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
@@ -1606,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2905,37 +2336,93 @@
         <v>136</v>
       </c>
     </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>134</v>
+      </c>
+      <c r="B106" t="s">
+        <v>147</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>11</v>
+      </c>
+      <c r="B107" t="s">
+        <v>145</v>
+      </c>
+      <c r="C107" t="s">
+        <v>146</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>149</v>
+      </c>
+      <c r="F107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>148</v>
+      </c>
+      <c r="B108" t="s">
+        <v>150</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108" t="s">
+        <v>151</v>
+      </c>
+      <c r="F108" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
+  <conditionalFormatting sqref="A1:H106 A109:H1048576 A107:A108 C107:H108">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>LEFT($A1, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>$A1="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>$A1="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$A1="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
-      <formula>LEFT($A1, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>$A1="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$A1="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$A1="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
-      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2943,20 +2430,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3199,6 +2686,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -3211,14 +2706,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
day 1 fully ported into excel
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D3C85F-DFF7-4B3F-8210-81C04F74FF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524D51B8-176A-49B0-B1BF-477D56216F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="168">
   <si>
     <t>Context</t>
   </si>
@@ -476,9 +476,6 @@
     <t>Uuuuugh. If the sound continues I will have to hide again under the bed</t>
   </si>
   <si>
-    <t>player woke up</t>
-  </si>
-  <si>
     <t>Wake_up</t>
   </si>
   <si>
@@ -492,6 +489,57 @@
   </si>
   <si>
     <t>p1_choosing</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>The war continues on Brasnia Republic, it has been one week since the war started, United States send more weapons to revolutionaries, multiple industries are leaving the country, afraid of being involved with any side of the war. So far the only hope for some is leaving for Canada as they are the only ones accepting refugees.</t>
+  </si>
+  <si>
+    <t>I only see snow and ash outside, I hope the heater doesnt give up on me, that would be my downfall</t>
+  </si>
+  <si>
+    <t>Player checks radio in day 1</t>
+  </si>
+  <si>
+    <t>Player goes outside to check situation</t>
+  </si>
+  <si>
+    <t>Player just woke up</t>
+  </si>
+  <si>
+    <t>player just woke up</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>p1_outside</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>LOOK FOR SHELTER, DONT LEAVE YOUR HOUSES. IF OUTSIDE SEEK THE NEAREST OUTPOST FOR HELP OR VOLUNTEERING.</t>
+  </si>
+  <si>
+    <t>Player checks television in day 1</t>
+  </si>
+  <si>
+    <t>tv1</t>
+  </si>
+  <si>
+    <t>I think I have enough food for the next days if, I hope the war doesn't reach this are of the city</t>
+  </si>
+  <si>
+    <t>Player checks food supplies</t>
+  </si>
+  <si>
+    <t>p1_supply</t>
+  </si>
+  <si>
+    <t>Day 2</t>
   </si>
 </sst>
 </file>
@@ -556,46 +604,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+  <dxfs count="107">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -625,14 +659,2448 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
       </fill>
       <border>
         <left style="dotted">
@@ -1037,10 +3505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +4817,7 @@
         <v>134</v>
       </c>
       <c r="B106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -2363,13 +4831,13 @@
         <v>145</v>
       </c>
       <c r="C107" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="D107">
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F107" t="s">
         <v>2</v>
@@ -2377,52 +4845,539 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B108" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="C108" t="s">
+        <v>156</v>
       </c>
       <c r="D108">
         <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F108" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>136</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>134</v>
+      </c>
+      <c r="B111" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>151</v>
+      </c>
+      <c r="B112" t="s">
+        <v>152</v>
+      </c>
+      <c r="C112" t="s">
+        <v>154</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>158</v>
+      </c>
+      <c r="F112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>136</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>134</v>
+      </c>
+      <c r="B115" t="s">
+        <v>146</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>11</v>
+      </c>
+      <c r="B116" t="s">
+        <v>153</v>
+      </c>
+      <c r="C116" t="s">
+        <v>155</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>159</v>
+      </c>
+      <c r="F116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>136</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>134</v>
+      </c>
+      <c r="B119" t="s">
+        <v>146</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>160</v>
+      </c>
+      <c r="B120" t="s">
+        <v>161</v>
+      </c>
+      <c r="C120" t="s">
+        <v>162</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" t="s">
+        <v>163</v>
+      </c>
+      <c r="F120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>136</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>134</v>
+      </c>
+      <c r="B123" t="s">
+        <v>146</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>11</v>
+      </c>
+      <c r="B124" t="s">
+        <v>164</v>
+      </c>
+      <c r="C124" t="s">
+        <v>165</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" t="s">
+        <v>166</v>
+      </c>
+      <c r="F124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>136</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>100</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H106 A109:H1048576 A107:A108 C107:H108">
-    <cfRule type="expression" dxfId="8" priority="1">
+  <conditionalFormatting sqref="A1:H106 G128 A107:A108 C107:H108 A116 A120:E121 F120:G120 G129:H1048576 A128:E1048576 A111:H111 A109:H109 A115:H115 A119:H119 A117:H117 A123:H123 A113:H113 C116:G116 A112:G112 A124:F125 A127:H127">
+    <cfRule type="expression" dxfId="106" priority="79">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="105" priority="80">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="104" priority="81">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="103" priority="87">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:H106 G128 A107:A108 C107:H108 A116 A120:E121 F120:G120 G129:H1048576 A128:E1048576 A111:H111 A109:H109 A115:H115 A119:H119 A117:H117 A123:H123 A113:H113 C116:G116 A112:G112 A124:F125 A127:H127">
+    <cfRule type="expression" dxfId="102" priority="83">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G108 F120:G120 F124:G124 F116:G116 F112:G112 G122 G126 F127:G1048576">
+    <cfRule type="containsText" dxfId="101" priority="82" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="84" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="85" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="86" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F130:F1048576">
+    <cfRule type="expression" dxfId="97" priority="92">
+      <formula>LEFT($A129, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="93">
+      <formula>$A129="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="94">
+      <formula>$A129="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Final">
-      <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Draft">
-      <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+  <conditionalFormatting sqref="F130:F1048576">
+    <cfRule type="expression" dxfId="93" priority="97">
+      <formula>$A129="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H120 H118 H114 H124 H122 G126:H126 H128">
+    <cfRule type="expression" dxfId="92" priority="106">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="107">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="108">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="109">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H120 H118 H114 H124 H122 G126:H126 H128">
+    <cfRule type="expression" dxfId="88" priority="128">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F128:F129">
+    <cfRule type="expression" dxfId="87" priority="137">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="138">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="139">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="140">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F128:F129">
+    <cfRule type="expression" dxfId="83" priority="142">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G122">
+    <cfRule type="expression" dxfId="82" priority="159">
+      <formula>LEFT($A125, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="160">
+      <formula>$A125="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="161">
+      <formula>$A125="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="162">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G122">
+    <cfRule type="expression" dxfId="78" priority="175">
+      <formula>$A125="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G124">
+    <cfRule type="expression" dxfId="72" priority="404">
+      <formula>LEFT($A121, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="405">
+      <formula>$A121="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="406">
+      <formula>$A121="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="407">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G124">
+    <cfRule type="expression" dxfId="68" priority="408">
+      <formula>$A121="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H110">
+    <cfRule type="expression" dxfId="67" priority="409">
+      <formula>LEFT($A116, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="410">
+      <formula>$A116="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="411">
+      <formula>$A116="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="412">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H110">
+    <cfRule type="expression" dxfId="63" priority="413">
+      <formula>$A116="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H116">
+    <cfRule type="expression" dxfId="57" priority="529">
+      <formula>LEFT($A123, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="530">
+      <formula>$A123="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="531">
+      <formula>$A123="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="532">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H116">
+    <cfRule type="expression" dxfId="53" priority="533">
+      <formula>$A123="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H112">
+    <cfRule type="expression" dxfId="52" priority="534">
+      <formula>LEFT($A124, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="535">
+      <formula>$A124="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="536">
+      <formula>$A124="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="537">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H112">
+    <cfRule type="expression" dxfId="48" priority="538">
+      <formula>$A124="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G114">
+    <cfRule type="expression" dxfId="42" priority="35">
+      <formula>LEFT($A114, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="36">
+      <formula>$A114="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="37">
+      <formula>$A114="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="43">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G114">
+    <cfRule type="expression" dxfId="38" priority="39">
+      <formula>$A114="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G114">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",G114)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",G114)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",G114)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="42" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",G114)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G110">
+    <cfRule type="expression" dxfId="33" priority="26">
+      <formula>LEFT($A110, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="27">
+      <formula>$A110="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="28">
+      <formula>$A110="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="34">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G110">
+    <cfRule type="expression" dxfId="29" priority="30">
+      <formula>$A110="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G110">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",G110)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",G110)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",G110)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",G110)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H121">
+    <cfRule type="expression" dxfId="24" priority="21">
+      <formula>LEFT($A121, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="22">
+      <formula>$A121="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>$A121="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="25">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H121">
+    <cfRule type="expression" dxfId="20" priority="24">
+      <formula>$A121="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F121">
+    <cfRule type="expression" dxfId="19" priority="16">
+      <formula>LEFT($A121, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="17">
+      <formula>$A121="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>$A121="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="20">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F121">
+    <cfRule type="expression" dxfId="15" priority="19">
+      <formula>$A121="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G121">
+    <cfRule type="expression" dxfId="14" priority="11">
+      <formula>LEFT($A121, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="12">
+      <formula>$A121="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>$A121="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G121">
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>$A121="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G125">
+    <cfRule type="expression" dxfId="9" priority="6">
+      <formula>LEFT($A125, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>$A125="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$A125="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G125">
+    <cfRule type="expression" dxfId="5" priority="9">
+      <formula>$A125="END"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H125">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>LEFT($A125, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$A125="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$A125="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H125">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>$A125="END"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2430,20 +5385,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2686,14 +5641,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2706,6 +5653,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
More day 7 lines
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C17ACFB-715E-4A06-A0F7-4A6003F5176A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526AB355-8CF2-4C72-9BC1-F579174624D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="742">
   <si>
     <t>Context</t>
   </si>
@@ -2260,6 +2260,9 @@
   </si>
   <si>
     <t>p_7_speechless</t>
+  </si>
+  <si>
+    <t>BOB</t>
   </si>
 </sst>
 </file>
@@ -3469,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H900"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A871" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A901" sqref="A901"/>
+    <sheetView tabSelected="1" topLeftCell="A869" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C878" sqref="C878"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9619,12 +9622,12 @@
     </row>
     <row r="590" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>478</v>
+        <v>683</v>
       </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="B591" t="s">
         <v>67</v>
@@ -9660,12 +9663,12 @@
     </row>
     <row r="594" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>485</v>
+        <v>683</v>
       </c>
     </row>
     <row r="595" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="B595" t="s">
         <v>519</v>
@@ -10293,7 +10296,10 @@
     </row>
     <row r="659" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>489</v>
+        <v>477</v>
+      </c>
+      <c r="B659" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="660" spans="1:6" x14ac:dyDescent="0.25">
@@ -10315,7 +10321,7 @@
     </row>
     <row r="661" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>478</v>
+        <v>683</v>
       </c>
     </row>
     <row r="662" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added begining of day 5
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A443BA90-1942-48A0-842E-597276C3E278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF3FC7C-89F2-4AC8-A28E-CEC298D7C2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="832">
   <si>
     <t>Context</t>
   </si>
@@ -2479,6 +2479,60 @@
   </si>
   <si>
     <t>p_4_sleep</t>
+  </si>
+  <si>
+    <t>DAY 5</t>
+  </si>
+  <si>
+    <t>We are certainly going to make a bigger expedition today to search for supplies</t>
+  </si>
+  <si>
+    <t>Nothing new in the front of the war. The republic palace was raided yesterday, the building has been completely ran over</t>
+  </si>
+  <si>
+    <t>Yesterday the broadcast was hacked, the government now will shoot any revolutionary in sight without questions asked. Join the military, make Brasnia great again. Make Brasnia safe again.</t>
+  </si>
+  <si>
+    <t>Visibility has increased, we can scavenge further now</t>
+  </si>
+  <si>
+    <t>Jessica commements on the radio</t>
+  </si>
+  <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>p5_outside</t>
+  </si>
+  <si>
+    <t>tv5</t>
+  </si>
+  <si>
+    <t>p5_supply</t>
+  </si>
+  <si>
+    <t>I hope they are alright</t>
+  </si>
+  <si>
+    <t>Oh you already woke up. But why do you care about it? It doesn't affect us in any way</t>
+  </si>
+  <si>
+    <t>My dad used to work there</t>
+  </si>
+  <si>
+    <t>Oh, what was his job</t>
+  </si>
+  <si>
+    <t>He was one of Judiciaries</t>
+  </si>
+  <si>
+    <t>Wait, whats your full name?</t>
+  </si>
+  <si>
+    <t>*loud music</t>
+  </si>
+  <si>
+    <t>I will turn that off</t>
   </si>
 </sst>
 </file>
@@ -2834,6 +2888,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2884,11 +2958,57 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD9EBCD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2901,6 +3021,488 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD9EBCD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3028,7 +3630,59 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border>
@@ -3100,65 +3754,39 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor rgb="FFD9EBCD"/>
         </patternFill>
       </fill>
       <border>
@@ -3183,26 +3811,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3244,344 +3852,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD9EBCD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD9EBCD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -3602,52 +3872,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i/>
       </font>
@@ -3725,15 +3949,15 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
       <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
       </fill>
       <border>
         <left style="dotted">
@@ -3752,13 +3976,81 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="2" tint="-0.749961851863155"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3918,6 +4210,58 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
       </font>
@@ -3944,33 +4288,55 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <b val="0"/>
+        <i/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3980,7 +4346,33 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -4130,13 +4522,91 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD9EBCD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -4188,7 +4658,111 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
       <border>
@@ -4234,6 +4808,162 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD9EBCD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
       </font>
@@ -4292,7 +5022,33 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border>
@@ -4344,7 +5100,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -4468,6 +5224,32 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
       </font>
@@ -4475,6 +5257,344 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD9EBCD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD9EBCD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -4520,13 +5640,13 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
+        <b val="0"/>
+        <i/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
       <border>
@@ -4571,6 +5691,32 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i/>
@@ -4579,6 +5725,110 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FFD9EBCD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -4630,266 +5880,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD9EBCD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -4917,942 +5907,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD9EBCD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD9EBCD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD9EBCD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD9EBCD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="2"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -6188,8 +6242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H900"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A768" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G791" sqref="G791"/>
+    <sheetView tabSelected="1" topLeftCell="A795" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D824" sqref="D824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14322,6 +14376,286 @@
         <v>136</v>
       </c>
     </row>
+    <row r="799" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A799" t="s">
+        <v>100</v>
+      </c>
+      <c r="B799" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="800" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A800" t="s">
+        <v>134</v>
+      </c>
+      <c r="B800" t="s">
+        <v>560</v>
+      </c>
+      <c r="D800">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="801" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A801" t="s">
+        <v>147</v>
+      </c>
+      <c r="B801" t="s">
+        <v>816</v>
+      </c>
+      <c r="C801" t="s">
+        <v>351</v>
+      </c>
+      <c r="D801">
+        <v>5</v>
+      </c>
+      <c r="E801" t="s">
+        <v>820</v>
+      </c>
+      <c r="F801" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="802" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A802" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="804" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A804" t="s">
+        <v>134</v>
+      </c>
+      <c r="B804" t="s">
+        <v>561</v>
+      </c>
+      <c r="D804">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="805" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A805" t="s">
+        <v>11</v>
+      </c>
+      <c r="B805" t="s">
+        <v>818</v>
+      </c>
+      <c r="C805" t="s">
+        <v>151</v>
+      </c>
+      <c r="D805">
+        <v>5</v>
+      </c>
+      <c r="E805" t="s">
+        <v>821</v>
+      </c>
+      <c r="F805" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="806" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A806" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="808" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A808" t="s">
+        <v>134</v>
+      </c>
+      <c r="B808" t="s">
+        <v>562</v>
+      </c>
+      <c r="D808">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="809" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A809" t="s">
+        <v>156</v>
+      </c>
+      <c r="B809" t="s">
+        <v>817</v>
+      </c>
+      <c r="C809" t="s">
+        <v>350</v>
+      </c>
+      <c r="D809">
+        <v>5</v>
+      </c>
+      <c r="E809" t="s">
+        <v>822</v>
+      </c>
+      <c r="F809" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="810" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A810" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="812" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A812" t="s">
+        <v>134</v>
+      </c>
+      <c r="B812" t="s">
+        <v>563</v>
+      </c>
+      <c r="D812">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="813" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A813" t="s">
+        <v>11</v>
+      </c>
+      <c r="B813" t="s">
+        <v>815</v>
+      </c>
+      <c r="C813" t="s">
+        <v>161</v>
+      </c>
+      <c r="D813">
+        <v>5</v>
+      </c>
+      <c r="E813" t="s">
+        <v>823</v>
+      </c>
+      <c r="F813" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="814" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A814" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="816" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A816" t="s">
+        <v>134</v>
+      </c>
+      <c r="B816" t="s">
+        <v>819</v>
+      </c>
+      <c r="D816">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="817" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>67</v>
+      </c>
+      <c r="B817" t="s">
+        <v>824</v>
+      </c>
+      <c r="D817">
+        <v>5</v>
+      </c>
+      <c r="F817" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="818" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>11</v>
+      </c>
+      <c r="B818" t="s">
+        <v>825</v>
+      </c>
+      <c r="D818">
+        <v>5</v>
+      </c>
+      <c r="F818" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="819" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
+        <v>67</v>
+      </c>
+      <c r="B819" t="s">
+        <v>826</v>
+      </c>
+      <c r="D819">
+        <v>5</v>
+      </c>
+      <c r="F819" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="820" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>11</v>
+      </c>
+      <c r="B820" t="s">
+        <v>827</v>
+      </c>
+      <c r="D820">
+        <v>5</v>
+      </c>
+      <c r="F820" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="821" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
+        <v>67</v>
+      </c>
+      <c r="B821" t="s">
+        <v>828</v>
+      </c>
+      <c r="D821">
+        <v>5</v>
+      </c>
+      <c r="F821" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="822" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A822" t="s">
+        <v>11</v>
+      </c>
+      <c r="B822" t="s">
+        <v>829</v>
+      </c>
+      <c r="D822">
+        <v>5</v>
+      </c>
+      <c r="F822" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="823" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A823" t="s">
+        <v>147</v>
+      </c>
+      <c r="B823" t="s">
+        <v>830</v>
+      </c>
+      <c r="D823">
+        <v>5</v>
+      </c>
+      <c r="F823" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="824" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A824" t="s">
+        <v>67</v>
+      </c>
+      <c r="B824" t="s">
+        <v>831</v>
+      </c>
+      <c r="D824">
+        <v>5</v>
+      </c>
+      <c r="F824" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="825" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A825" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="853" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
         <v>100</v>
@@ -14827,234 +15161,234 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A713:A718">
-    <cfRule type="expression" dxfId="144" priority="98">
+    <cfRule type="expression" dxfId="144" priority="94">
+      <formula>$A713="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="95">
+      <formula>$A713="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="96">
+      <formula>$A713="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="97">
+      <formula>$A713="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="98">
       <formula>$A713="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="101">
-      <formula>MOD(ROW(),2)=0</formula>
+    <cfRule type="expression" dxfId="139" priority="93">
+      <formula>LEFT($A713, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="95">
-      <formula>$A713="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="96">
-      <formula>$A713="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="99">
+    <cfRule type="expression" dxfId="138" priority="99">
       <formula>$A713="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="100">
+    <cfRule type="expression" dxfId="137" priority="100">
       <formula>$A713="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="97">
-      <formula>$A713="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="93">
-      <formula>LEFT($A713, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="94">
-      <formula>$A713="CHOICE"</formula>
+    <cfRule type="expression" dxfId="136" priority="101">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A758:B758">
-    <cfRule type="expression" dxfId="135" priority="64">
+    <cfRule type="expression" dxfId="135" priority="70">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="62">
+      <formula>LEFT($A758, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="63">
+      <formula>$A758="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="64">
       <formula>$A758="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="65">
+    <cfRule type="expression" dxfId="131" priority="65">
       <formula>$A758="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="66">
+    <cfRule type="expression" dxfId="130" priority="66">
       <formula>$A758="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="67">
+    <cfRule type="expression" dxfId="129" priority="68">
+      <formula>$A758="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="67">
       <formula>$A758="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="68">
-      <formula>$A758="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="69">
+    <cfRule type="expression" dxfId="127" priority="69">
       <formula>$A758="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="70">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="128" priority="63">
-      <formula>$A758="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="62">
-      <formula>LEFT($A758, 2)="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A763:B763">
-    <cfRule type="expression" dxfId="126" priority="56">
+    <cfRule type="expression" dxfId="126" priority="55">
+      <formula>$A763="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="56">
       <formula>$A763="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="59">
+    <cfRule type="expression" dxfId="124" priority="57">
+      <formula>$A763="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="58">
+      <formula>$A763="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="59">
       <formula>$A763="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="58">
-      <formula>$A763="ELIF"</formula>
+    <cfRule type="expression" dxfId="121" priority="60">
+      <formula>$A763="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="57">
-      <formula>$A763="IF"</formula>
+    <cfRule type="expression" dxfId="120" priority="61">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="54">
+    <cfRule type="expression" dxfId="119" priority="53">
+      <formula>LEFT($A763, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="54">
       <formula>$A763="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="55">
-      <formula>$A763="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="53">
-      <formula>LEFT($A763, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="60">
-      <formula>$A763="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="61">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:H700 F700:F701 A701 C701:H701 A702:H708 A709 C709:H709 A710:H712 A719:H719 A722:H722 A723 C723:H723 A724:H724 A725 C725:H725 A726:H729 A730 C730:H730 A731:H733 A734 C734:H734 A735:H737 A738 C738:H738 A739:H741 A742 C742:H742 A743:H757 A759:H762 A764:H774 A775:C775 E775:H775 A776:B776 A777:H780 A781 C781:H781 A782:H793 A794 C794:H794 A795:H795 A796 C796:H796 A797:H800 A814:H816 A813 C813:H813 A802:H804 A801 C801:H801 A810:H812 A809 C809:H809 A806:H808 A805 C805:H805 A821:H821 A817:A819 C817:H820 A823:H1048576 B822:H822 F817:F824">
+    <cfRule type="expression" dxfId="117" priority="141">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H700 F700:F701 A701 C701:H701 A702:H708 A709 C709:H709 A710:H712 A719:H719 A722:H722 A723 C723:H723 A724:H724 A725 C725:H725 A726:H729 A730 C730:H730 A731:H733 A734 C734:H734 A735:H737 A738 C738:H738 A739:H741 A742 C742:H742 A743:H757 A759:H762 A764:H774 A775:C775 E775:H775 A776:B776 A777:H780 A781 C781:H781 A782:H793 A794 C794:H794 A795:H795 A796 C796:H796 A797:H1048576">
-    <cfRule type="expression" dxfId="117" priority="132">
+    <cfRule type="expression" dxfId="116" priority="136">
+      <formula>$A1="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="135">
+      <formula>$A1="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="134">
+      <formula>$A1="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="130">
+      <formula>$A1="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="131">
+      <formula>$A1="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="132">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="131">
-      <formula>$A1="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="130">
-      <formula>$A1="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="133">
+    <cfRule type="expression" dxfId="110" priority="133">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="141">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="136">
-      <formula>$A1="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="135">
-      <formula>$A1="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="134">
-      <formula>$A1="ELIF"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A719:H719 A1:H700 F700:F701 A701 C701:H701 A702:H708 A709 C709:H709 A710:H712 A722:H722 A723 C723:H723 A724:H724 A725 C725:H725 A726:H729 A730 C730:H730 A731:H733 A734 C734:H734 A735:H737 A738 C738:H738 A739:H741 A742 C742:H742 A743:H757 A759:H762 A764:H774 A775:C775 E775:H775 A776:B776 A777:H780 A781 C781:H781 A782:H793 A794 C794:H794 A795:H795 A796 C796:H796 A797:H1048576">
+  <conditionalFormatting sqref="A719:H719 A1:H700 F700:F701 A701 C701:H701 A702:H708 A709 C709:H709 A710:H712 A722:H722 A723 C723:H723 A724:H724 A725 C725:H725 A726:H729 A730 C730:H730 A731:H733 A734 C734:H734 A735:H737 A738 C738:H738 A739:H741 A742 C742:H742 A743:H757 A759:H762 A764:H774 A775:C775 E775:H775 A776:B776 A777:H780 A781 C781:H781 A782:H793 A794 C794:H794 A795:H795 A796 C796:H796 A797:H800 A814:H816 A813 C813:H813 A802:H804 A801 C801:H801 A810:H812 A809 C809:H809 A806:H808 A805 C805:H805 A821:H821 A817:A819 C817:H820 A823:H1048576 B822:H822 F817:F824">
     <cfRule type="expression" dxfId="109" priority="129">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B713:H713">
-    <cfRule type="expression" dxfId="108" priority="121">
+    <cfRule type="expression" dxfId="108" priority="123">
+      <formula>$A713="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="124">
+      <formula>$A713="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="125">
+      <formula>$A713="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="126">
+      <formula>$A713="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="127">
+      <formula>$A713="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="128">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="122">
+      <formula>$A713="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="121">
       <formula>$A713="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="122">
-      <formula>$A713="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="123">
-      <formula>$A713="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="124">
-      <formula>$A713="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="125">
-      <formula>$A713="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="126">
-      <formula>$A713="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="120">
+    <cfRule type="expression" dxfId="100" priority="120">
       <formula>LEFT($A713, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="127">
-      <formula>$A713="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="128">
-      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B715:H716">
-    <cfRule type="expression" dxfId="99" priority="106">
+    <cfRule type="expression" dxfId="99" priority="110">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="108">
+      <formula>$A715="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="107">
+      <formula>$A715="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="106">
       <formula>$A715="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="107">
-      <formula>$A715="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="108">
-      <formula>$A715="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="105">
+    <cfRule type="expression" dxfId="95" priority="105">
       <formula>$A715="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="109">
-      <formula>$A715="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="110">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="93" priority="104">
+    <cfRule type="expression" dxfId="94" priority="104">
       <formula>$A715="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="103">
+    <cfRule type="expression" dxfId="93" priority="103">
       <formula>$A715="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="102">
+    <cfRule type="expression" dxfId="92" priority="102">
       <formula>LEFT($A715, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="109">
+      <formula>$A715="ENDIF"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B718:H718">
-    <cfRule type="expression" dxfId="90" priority="92">
+    <cfRule type="expression" dxfId="90" priority="89">
+      <formula>$A718="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="90">
+      <formula>$A718="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="91">
+      <formula>$A718="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="91">
-      <formula>$A718="ENDIF"</formula>
+    <cfRule type="expression" dxfId="86" priority="84">
+      <formula>LEFT($A718, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="90">
-      <formula>$A718="ELSE"</formula>
+    <cfRule type="expression" dxfId="85" priority="85">
+      <formula>$A718="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="89">
-      <formula>$A718="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="88">
-      <formula>$A718="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="86">
+    <cfRule type="expression" dxfId="84" priority="86">
       <formula>$A718="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="85">
-      <formula>$A718="CHOICE"</formula>
+    <cfRule type="expression" dxfId="83" priority="87">
+      <formula>$A718="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="84">
-      <formula>LEFT($A718, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="87">
-      <formula>$A718="END"</formula>
+    <cfRule type="expression" dxfId="82" priority="88">
+      <formula>$A718="IF"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C776">
-    <cfRule type="expression" dxfId="81" priority="161">
-      <formula>$A775="CHOICE"</formula>
+    <cfRule type="expression" dxfId="81" priority="167">
+      <formula>$A775="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="162">
+    <cfRule type="expression" dxfId="80" priority="168">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="166">
+      <formula>$A775="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="165">
+      <formula>$A775="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="164">
+      <formula>$A775="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="163">
+      <formula>$A775="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="162">
       <formula>$A775="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="163">
-      <formula>$A775="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="164">
-      <formula>$A775="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="165">
-      <formula>$A775="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="166">
-      <formula>$A775="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="167">
-      <formula>$A775="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="168">
-      <formula>MOD(ROW(),2)=0</formula>
+    <cfRule type="expression" dxfId="74" priority="161">
+      <formula>$A775="CHOICE"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="73" priority="160">
       <formula>LEFT($A775, 2)="//"</formula>
@@ -15064,189 +15398,189 @@
     <cfRule type="expression" dxfId="72" priority="46">
       <formula>$A714="ELSE"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="48" operator="containsText" text="Final">
+    <cfRule type="expression" dxfId="71" priority="45">
+      <formula>$A714="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="44">
+      <formula>$A714="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="43">
+      <formula>$A714="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="42">
+      <formula>$A714="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="41">
+      <formula>$A714="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="40">
+      <formula>LEFT($A714, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="50" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F714)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="49" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F714)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="52">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="51" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F714)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="48" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F714)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="49" operator="containsText" text="Draft">
-      <formula>NOT(ISERROR(SEARCH("Draft",F714)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="50" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F714)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="47">
+    <cfRule type="expression" dxfId="60" priority="47">
       <formula>$A714="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="45">
-      <formula>$A714="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="44">
-      <formula>$A714="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="43">
-      <formula>$A714="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="42">
-      <formula>$A714="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="41">
-      <formula>$A714="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="40">
-      <formula>LEFT($A714, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="51" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F714)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52">
-      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F717">
-    <cfRule type="expression" dxfId="59" priority="29">
+    <cfRule type="expression" dxfId="59" priority="33">
+      <formula>$A717="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="32">
+      <formula>$A717="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="31">
+      <formula>$A717="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="30">
+      <formula>$A717="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="29">
       <formula>$A717="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="28">
+    <cfRule type="expression" dxfId="54" priority="28">
       <formula>$A717="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="27">
+    <cfRule type="expression" dxfId="53" priority="27">
       <formula>LEFT($A717, 2)="//"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="35" operator="containsText" text="Final">
+    <cfRule type="expression" dxfId="52" priority="39">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="38" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F717)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="37" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F717)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="36" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F717)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="35" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F717)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="39">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="38" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F717)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="37" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F717)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="36" operator="containsText" text="Draft">
-      <formula>NOT(ISERROR(SEARCH("Draft",F717)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="34">
+    <cfRule type="expression" dxfId="47" priority="34">
       <formula>$A717="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="33">
-      <formula>$A717="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="32">
-      <formula>$A717="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="31">
-      <formula>$A717="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="30">
-      <formula>$A717="END"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F763">
-    <cfRule type="expression" dxfId="46" priority="21">
+    <cfRule type="expression" dxfId="46" priority="17">
+      <formula>$A763="END"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="22" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F763)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="21">
       <formula>$A763="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="20">
+    <cfRule type="expression" dxfId="43" priority="20">
       <formula>$A763="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="19">
+    <cfRule type="expression" dxfId="42" priority="19">
       <formula>$A763="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="17">
-      <formula>$A763="END"</formula>
+    <cfRule type="expression" dxfId="41" priority="18">
+      <formula>$A763="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="16">
+    <cfRule type="expression" dxfId="40" priority="16">
       <formula>$A763="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="15">
+    <cfRule type="expression" dxfId="39" priority="26">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="25" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F763)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="24" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F763)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="23" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F763)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="15">
       <formula>$A763="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="14">
+    <cfRule type="expression" dxfId="34" priority="14">
       <formula>LEFT($A763, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="18">
-      <formula>$A763="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="26">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="25" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F763)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="24" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F763)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="23" operator="containsText" text="Draft">
-      <formula>NOT(ISERROR(SEARCH("Draft",F763)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="22" operator="containsText" text="Final">
-      <formula>NOT(ISERROR(SEARCH("Final",F763)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F776">
-    <cfRule type="expression" dxfId="33" priority="2">
+    <cfRule type="expression" dxfId="33" priority="5">
+      <formula>$A776="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="6">
+      <formula>$A776="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="7">
+      <formula>$A776="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="1">
+      <formula>LEFT($A776, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>$A776="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>$A776="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="4">
+    <cfRule type="expression" dxfId="27" priority="4">
       <formula>$A776="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="5">
-      <formula>$A776="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6">
-      <formula>$A776="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="7">
-      <formula>$A776="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="1">
-      <formula>LEFT($A776, 2)="//"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F776)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F776)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="11" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="23" priority="11" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F776)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="22" priority="10" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F776)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="Final">
-      <formula>NOT(ISERROR(SEARCH("Final",F776)))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="8">
       <formula>$A776="ENDIF"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G711 F722:G757 F759:G759 F761:G762 F764:G775 F777:G1048576">
-    <cfRule type="containsText" dxfId="20" priority="137" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="20" priority="139" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="140" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="137" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="138" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="17" priority="138" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="139" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="140" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F719:G719">
-    <cfRule type="containsText" dxfId="16" priority="79" operator="containsText" text="Final">
-      <formula>NOT(ISERROR(SEARCH("Final",F719)))</formula>
+    <cfRule type="containsText" dxfId="16" priority="81" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F719)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="80" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F719)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="81" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F719)))</formula>
+    <cfRule type="containsText" dxfId="14" priority="79" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F719)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="82" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F719)))</formula>

</xml_diff>

<commit_message>
Fixed up remaining lines
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C589EE55-8ABF-427C-9A2B-29565E36BB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1ECA8E-6DFB-4C67-9DEB-BDDC8B24329D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2899" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="1090">
   <si>
     <t>Context</t>
   </si>
@@ -2469,9 +2469,6 @@
     <t>I should stay here, I cannot do much</t>
   </si>
   <si>
-    <t>Making choice to who to send</t>
-  </si>
-  <si>
     <t>*Thumbs up*</t>
   </si>
   <si>
@@ -2484,15 +2481,6 @@
     <t>Scavenging comment</t>
   </si>
   <si>
-    <t>Violet scavenging day 5</t>
-  </si>
-  <si>
-    <t>Jessica scavenging day 5</t>
-  </si>
-  <si>
-    <t>Bob scavenging day 5</t>
-  </si>
-  <si>
     <t>You're sending her alone to the gas station? Are you dumb? How can she help us by scavenging around the gas station?</t>
   </si>
   <si>
@@ -2502,9 +2490,6 @@
     <t>I cant go alone!</t>
   </si>
   <si>
-    <t>Makign choice to who to send</t>
-  </si>
-  <si>
     <t>Ok, let me think a bit more</t>
   </si>
   <si>
@@ -2514,18 +2499,9 @@
     <t>*I want to go scavenge, there might be something useful that I can fix there*</t>
   </si>
   <si>
-    <t>Send bob day 5</t>
-  </si>
-  <si>
-    <t>Send Jessica day 5</t>
-  </si>
-  <si>
     <t>Bob should go, It's better this way</t>
   </si>
   <si>
-    <t>Violet scavenge day 4</t>
-  </si>
-  <si>
     <t>Fine by me, it seems she can handle well on her own</t>
   </si>
   <si>
@@ -2637,12 +2613,6 @@
     <t>v_5_thumbs</t>
   </si>
   <si>
-    <t>violet should go, It's better this way</t>
-  </si>
-  <si>
-    <t>Send violet day 5</t>
-  </si>
-  <si>
     <t>b_5_violet</t>
   </si>
   <si>
@@ -3325,6 +3295,18 @@
   </si>
   <si>
     <t>b_4_scavenge_no_gun</t>
+  </si>
+  <si>
+    <t>Bob scavenge day 5</t>
+  </si>
+  <si>
+    <t>Violet scavenge day 5</t>
+  </si>
+  <si>
+    <t>Jessica scavenge day 5</t>
+  </si>
+  <si>
+    <t>Violet should go, It's better this way</t>
   </si>
 </sst>
 </file>
@@ -3382,46 +3364,786 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="78">
     <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -4863,8 +5585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A691" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C709" sqref="C709"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C217" sqref="C217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5667,13 +6389,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>1071</v>
+        <v>1061</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>1073</v>
+        <v>1063</v>
       </c>
       <c r="F43" t="s">
         <v>4</v>
@@ -5687,13 +6409,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>1072</v>
+        <v>1062</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>1074</v>
+        <v>1064</v>
       </c>
       <c r="F44" t="s">
         <v>4</v>
@@ -5710,7 +6432,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>1061</v>
+        <v>1051</v>
       </c>
       <c r="F45" t="s">
         <v>4</v>
@@ -5724,13 +6446,13 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>1076</v>
+        <v>1066</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>1077</v>
+        <v>1067</v>
       </c>
       <c r="F46" t="s">
         <v>4</v>
@@ -5744,7 +6466,7 @@
         <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>1062</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -5752,7 +6474,7 @@
         <v>133</v>
       </c>
       <c r="B49" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -5791,7 +6513,7 @@
         <v>133</v>
       </c>
       <c r="B56" t="s">
-        <v>1064</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -5830,7 +6552,7 @@
         <v>99</v>
       </c>
       <c r="B63" t="s">
-        <v>1066</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -5838,7 +6560,7 @@
         <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>1065</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -5846,7 +6568,7 @@
         <v>99</v>
       </c>
       <c r="B65" t="s">
-        <v>1081</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -5854,15 +6576,15 @@
         <v>466</v>
       </c>
       <c r="B66" t="s">
-        <v>1075</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B67" t="s">
-        <v>1080</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -5870,15 +6592,15 @@
         <v>134</v>
       </c>
       <c r="B68" t="s">
-        <v>1079</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>1071</v>
+        <v>1061</v>
       </c>
       <c r="E69" t="s">
-        <v>1073</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -5886,15 +6608,15 @@
         <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>1080</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>1072</v>
+        <v>1062</v>
       </c>
       <c r="E71" t="s">
-        <v>1074</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -5907,7 +6629,7 @@
         <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>1088</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -5915,7 +6637,7 @@
         <v>133</v>
       </c>
       <c r="B75" t="s">
-        <v>1079</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -5928,7 +6650,7 @@
         <v>133</v>
       </c>
       <c r="B77" t="s">
-        <v>1080</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -5941,7 +6663,7 @@
         <v>133</v>
       </c>
       <c r="B88" t="s">
-        <v>1078</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -5951,10 +6673,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>1076</v>
+        <v>1066</v>
       </c>
       <c r="E90" t="s">
-        <v>1077</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -6279,7 +7001,7 @@
         <v>24</v>
       </c>
       <c r="B117" t="s">
-        <v>1084</v>
+        <v>1074</v>
       </c>
       <c r="C117" t="s">
         <v>32</v>
@@ -6346,7 +7068,7 @@
         <v>133</v>
       </c>
       <c r="B124" t="s">
-        <v>1082</v>
+        <v>1072</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -6357,16 +7079,16 @@
         <v>24</v>
       </c>
       <c r="B125" t="s">
-        <v>1083</v>
+        <v>1073</v>
       </c>
       <c r="C125" t="s">
-        <v>1085</v>
+        <v>1075</v>
       </c>
       <c r="D125">
         <v>0</v>
       </c>
       <c r="E125" t="s">
-        <v>1086</v>
+        <v>1076</v>
       </c>
       <c r="F125" t="s">
         <v>3</v>
@@ -6442,7 +7164,7 @@
         <v>134</v>
       </c>
       <c r="B131" t="s">
-        <v>1087</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -6507,7 +7229,7 @@
         <v>134</v>
       </c>
       <c r="B139" t="s">
-        <v>1087</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -6577,7 +7299,7 @@
         <v>133</v>
       </c>
       <c r="B151" t="s">
-        <v>1087</v>
+        <v>1077</v>
       </c>
       <c r="D151">
         <v>0</v>
@@ -7032,6 +7754,9 @@
       <c r="B196" t="s">
         <v>485</v>
       </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
@@ -7101,6 +7826,9 @@
       <c r="B204" t="s">
         <v>486</v>
       </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
@@ -9250,7 +9978,10 @@
         <v>133</v>
       </c>
       <c r="B397" t="s">
-        <v>1067</v>
+        <v>1057</v>
+      </c>
+      <c r="D397">
+        <v>3</v>
       </c>
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.25">
@@ -9283,7 +10014,7 @@
         <v>67</v>
       </c>
       <c r="B400" t="s">
-        <v>1068</v>
+        <v>1058</v>
       </c>
       <c r="D400">
         <v>3</v>
@@ -9319,10 +10050,10 @@
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B403" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.25">
@@ -9337,6 +10068,9 @@
       <c r="B406" t="s">
         <v>395</v>
       </c>
+      <c r="D406">
+        <v>3</v>
+      </c>
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
@@ -9387,10 +10121,10 @@
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B411" t="s">
-        <v>1065</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.25">
@@ -9442,7 +10176,7 @@
         <v>134</v>
       </c>
       <c r="B419" t="s">
-        <v>1060</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.25">
@@ -9684,7 +10418,7 @@
         <v>3</v>
       </c>
       <c r="E440" t="s">
-        <v>876</v>
+        <v>866</v>
       </c>
       <c r="F440" t="s">
         <v>2</v>
@@ -9992,7 +10726,7 @@
         <v>11</v>
       </c>
       <c r="B468" t="s">
-        <v>1089</v>
+        <v>1079</v>
       </c>
       <c r="D468">
         <v>3</v>
@@ -10092,7 +10826,7 @@
         <v>11</v>
       </c>
       <c r="B477" t="s">
-        <v>1090</v>
+        <v>1080</v>
       </c>
       <c r="D477">
         <v>3</v>
@@ -10266,7 +11000,7 @@
         <v>133</v>
       </c>
       <c r="B494" t="s">
-        <v>1091</v>
+        <v>1081</v>
       </c>
       <c r="D494">
         <v>3</v>
@@ -10918,6 +11652,9 @@
       <c r="B567" t="s">
         <v>510</v>
       </c>
+      <c r="D567">
+        <v>3</v>
+      </c>
     </row>
     <row r="568" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
@@ -11314,7 +12051,7 @@
         <v>4</v>
       </c>
       <c r="E606" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="F606" t="s">
         <v>2</v>
@@ -11606,10 +12343,10 @@
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B637" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.25">
@@ -11633,15 +12370,15 @@
         <v>466</v>
       </c>
       <c r="B641" t="s">
-        <v>1075</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="642" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B642" t="s">
-        <v>1092</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="643" spans="1:6" x14ac:dyDescent="0.25">
@@ -11696,7 +12433,7 @@
         <v>134</v>
       </c>
       <c r="B647" t="s">
-        <v>1079</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="648" spans="1:6" x14ac:dyDescent="0.25">
@@ -11721,7 +12458,7 @@
         <v>134</v>
       </c>
       <c r="B649" t="s">
-        <v>1080</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="650" spans="1:6" x14ac:dyDescent="0.25">
@@ -11751,7 +12488,7 @@
         <v>133</v>
       </c>
       <c r="B654" t="s">
-        <v>1092</v>
+        <v>1082</v>
       </c>
       <c r="D654">
         <v>4</v>
@@ -11762,7 +12499,7 @@
         <v>66</v>
       </c>
       <c r="B655" t="s">
-        <v>1094</v>
+        <v>1084</v>
       </c>
       <c r="D655">
         <v>4</v>
@@ -11787,7 +12524,7 @@
         <v>67</v>
       </c>
       <c r="B657" t="s">
-        <v>1093</v>
+        <v>1083</v>
       </c>
       <c r="D657">
         <v>4</v>
@@ -11806,10 +12543,10 @@
     </row>
     <row r="659" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B659" t="s">
-        <v>1065</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="660" spans="1:6" x14ac:dyDescent="0.25">
@@ -11927,10 +12664,10 @@
     </row>
     <row r="672" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B672" t="s">
         <v>1069</v>
-      </c>
-      <c r="B672" t="s">
-        <v>1079</v>
       </c>
     </row>
     <row r="673" spans="1:6" x14ac:dyDescent="0.25">
@@ -11968,10 +12705,10 @@
     </row>
     <row r="677" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B677" t="s">
-        <v>1080</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="678" spans="1:6" x14ac:dyDescent="0.25">
@@ -12097,7 +12834,7 @@
         <v>4</v>
       </c>
       <c r="E692" t="s">
-        <v>1095</v>
+        <v>1085</v>
       </c>
       <c r="F692" t="s">
         <v>2</v>
@@ -12303,10 +13040,10 @@
     </row>
     <row r="715" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B715" t="s">
-        <v>1065</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="716" spans="1:6" x14ac:dyDescent="0.25">
@@ -12314,37 +13051,54 @@
         <v>135</v>
       </c>
     </row>
+    <row r="720" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A720" t="s">
+        <v>133</v>
+      </c>
+      <c r="B720" t="s">
+        <v>709</v>
+      </c>
+      <c r="D720">
+        <v>4</v>
+      </c>
+    </row>
     <row r="721" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>133</v>
+        <v>466</v>
       </c>
       <c r="B721" t="s">
-        <v>709</v>
-      </c>
-      <c r="D721">
-        <v>4</v>
+        <v>503</v>
       </c>
     </row>
     <row r="722" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>466</v>
+        <v>66</v>
       </c>
       <c r="B722" t="s">
-        <v>503</v>
+        <v>710</v>
+      </c>
+      <c r="D722">
+        <v>4</v>
+      </c>
+      <c r="E722" t="s">
+        <v>754</v>
+      </c>
+      <c r="F722" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="723" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B723" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D723">
         <v>4</v>
       </c>
       <c r="E723" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F723" t="s">
         <v>2</v>
@@ -12352,19 +13106,7 @@
     </row>
     <row r="724" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>67</v>
-      </c>
-      <c r="B724" t="s">
-        <v>711</v>
-      </c>
-      <c r="D724">
-        <v>4</v>
-      </c>
-      <c r="E724" t="s">
-        <v>755</v>
-      </c>
-      <c r="F724" t="s">
-        <v>2</v>
+        <v>650</v>
       </c>
     </row>
     <row r="725" spans="1:6" x14ac:dyDescent="0.25">
@@ -12462,6 +13204,9 @@
       <c r="B735" t="s">
         <v>724</v>
       </c>
+      <c r="D735">
+        <v>4</v>
+      </c>
     </row>
     <row r="736" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
@@ -12999,6 +13744,9 @@
       <c r="B796" t="s">
         <v>729</v>
       </c>
+      <c r="D796">
+        <v>4</v>
+      </c>
     </row>
     <row r="797" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
@@ -13167,6 +13915,9 @@
       <c r="B812" t="s">
         <v>748</v>
       </c>
+      <c r="D812">
+        <v>4</v>
+      </c>
     </row>
     <row r="813" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
@@ -13263,7 +14014,7 @@
         <v>133</v>
       </c>
       <c r="B823" t="s">
-        <v>962</v>
+        <v>952</v>
       </c>
       <c r="D823">
         <v>5</v>
@@ -13299,7 +14050,7 @@
         <v>133</v>
       </c>
       <c r="B827" t="s">
-        <v>961</v>
+        <v>951</v>
       </c>
       <c r="D827">
         <v>5</v>
@@ -13335,7 +14086,7 @@
         <v>133</v>
       </c>
       <c r="B831" t="s">
-        <v>960</v>
+        <v>950</v>
       </c>
       <c r="D831">
         <v>5</v>
@@ -13371,7 +14122,7 @@
         <v>133</v>
       </c>
       <c r="B835" t="s">
-        <v>959</v>
+        <v>949</v>
       </c>
       <c r="D835">
         <v>5</v>
@@ -13424,7 +14175,7 @@
         <v>5</v>
       </c>
       <c r="E840" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="F840" t="s">
         <v>2</v>
@@ -13441,7 +14192,7 @@
         <v>5</v>
       </c>
       <c r="E841" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="F841" t="s">
         <v>2</v>
@@ -13458,7 +14209,7 @@
         <v>5</v>
       </c>
       <c r="E842" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="F842" t="s">
         <v>2</v>
@@ -13475,7 +14226,7 @@
         <v>5</v>
       </c>
       <c r="E843" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="F843" t="s">
         <v>2</v>
@@ -13492,7 +14243,7 @@
         <v>5</v>
       </c>
       <c r="E844" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="F844" t="s">
         <v>2</v>
@@ -13509,7 +14260,7 @@
         <v>5</v>
       </c>
       <c r="E845" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="F845" t="s">
         <v>2</v>
@@ -13526,7 +14277,7 @@
         <v>5</v>
       </c>
       <c r="E846" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="F846" t="s">
         <v>2</v>
@@ -13543,7 +14294,7 @@
         <v>5</v>
       </c>
       <c r="E847" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="F847" t="s">
         <v>2</v>
@@ -13576,7 +14327,7 @@
         <v>5</v>
       </c>
       <c r="E851" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="F851" t="s">
         <v>2</v>
@@ -13593,7 +14344,7 @@
         <v>5</v>
       </c>
       <c r="E852" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="F852" t="s">
         <v>2</v>
@@ -13610,7 +14361,7 @@
         <v>5</v>
       </c>
       <c r="E853" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="F853" t="s">
         <v>2</v>
@@ -13643,7 +14394,7 @@
         <v>5</v>
       </c>
       <c r="E857" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="F857" t="s">
         <v>2</v>
@@ -13660,7 +14411,7 @@
         <v>5</v>
       </c>
       <c r="E858" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="F858" t="s">
         <v>2</v>
@@ -13676,7 +14427,10 @@
         <v>133</v>
       </c>
       <c r="B861" t="s">
-        <v>814</v>
+        <v>813</v>
+      </c>
+      <c r="D861">
+        <v>5</v>
       </c>
     </row>
     <row r="862" spans="1:6" x14ac:dyDescent="0.25">
@@ -13690,7 +14444,7 @@
         <v>5</v>
       </c>
       <c r="E862" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="F862" t="s">
         <v>2</v>
@@ -13720,7 +14474,7 @@
         <v>5</v>
       </c>
       <c r="E865" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="F865" t="s">
         <v>2</v>
@@ -13750,7 +14504,7 @@
         <v>5</v>
       </c>
       <c r="E868" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="F868" t="s">
         <v>2</v>
@@ -13780,7 +14534,7 @@
         <v>5</v>
       </c>
       <c r="E871" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="F871" t="s">
         <v>2</v>
@@ -13796,238 +14550,147 @@
         <v>135</v>
       </c>
     </row>
-    <row r="875" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A875" t="s">
-        <v>133</v>
-      </c>
-      <c r="B875" t="s">
-        <v>810</v>
-      </c>
-      <c r="D875">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="876" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A876" t="s">
-        <v>466</v>
-      </c>
-      <c r="B876" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="877" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A877" t="s">
-        <v>134</v>
-      </c>
-      <c r="B877" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="878" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A878" t="s">
-        <v>11</v>
-      </c>
-      <c r="B878" t="s">
-        <v>812</v>
-      </c>
-      <c r="D878">
-        <v>5</v>
-      </c>
-      <c r="E878" t="s">
-        <v>856</v>
-      </c>
-      <c r="F878" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="879" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A879" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="880" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A880" t="s">
-        <v>466</v>
-      </c>
-      <c r="B880" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="881" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A881" t="s">
-        <v>134</v>
-      </c>
-      <c r="B881" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="882" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A882" t="s">
-        <v>11</v>
-      </c>
-      <c r="B882" t="s">
-        <v>387</v>
-      </c>
-      <c r="D882">
-        <v>5</v>
-      </c>
-      <c r="E882" t="s">
-        <v>857</v>
-      </c>
-      <c r="F882" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="883" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A883" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="884" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A884" t="s">
-        <v>466</v>
-      </c>
-      <c r="B884" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="885" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A885" t="s">
-        <v>134</v>
-      </c>
-      <c r="B885" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="886" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A886" t="s">
-        <v>11</v>
-      </c>
-      <c r="B886" t="s">
-        <v>813</v>
-      </c>
-      <c r="D886">
-        <v>5</v>
-      </c>
-      <c r="E886" t="s">
-        <v>858</v>
-      </c>
-      <c r="F886" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="887" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
-        <v>650</v>
+        <v>133</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1088</v>
       </c>
     </row>
     <row r="888" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
-        <v>135</v>
+        <v>11</v>
+      </c>
+      <c r="B888" t="s">
+        <v>387</v>
+      </c>
+      <c r="D888">
+        <v>5</v>
+      </c>
+      <c r="E888" t="s">
+        <v>849</v>
+      </c>
+      <c r="F888" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="889" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>466</v>
+      </c>
+      <c r="B889" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="890" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="B890" t="s">
-        <v>575</v>
+        <v>814</v>
+      </c>
+      <c r="D890">
+        <v>5</v>
+      </c>
+      <c r="E890" t="s">
+        <v>851</v>
+      </c>
+      <c r="F890" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="891" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
-        <v>466</v>
-      </c>
-      <c r="B891" t="s">
-        <v>708</v>
+        <v>650</v>
       </c>
     </row>
     <row r="892" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
-        <v>67</v>
+        <v>466</v>
       </c>
       <c r="B892" t="s">
-        <v>818</v>
-      </c>
-      <c r="D892">
-        <v>5</v>
-      </c>
-      <c r="E892" t="s">
-        <v>859</v>
-      </c>
-      <c r="F892" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="893" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
-        <v>650</v>
+        <v>68</v>
+      </c>
+      <c r="B893" t="s">
+        <v>815</v>
+      </c>
+      <c r="D893">
+        <v>5</v>
+      </c>
+      <c r="E893" t="s">
+        <v>852</v>
+      </c>
+      <c r="F893" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="894" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
-        <v>466</v>
-      </c>
-      <c r="B894" t="s">
-        <v>68</v>
+        <v>650</v>
       </c>
     </row>
     <row r="895" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B895" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="D895">
         <v>5</v>
       </c>
       <c r="E895" t="s">
-        <v>860</v>
-      </c>
-      <c r="F895" t="s">
-        <v>2</v>
+        <v>853</v>
       </c>
     </row>
     <row r="896" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
-        <v>650</v>
+        <v>134</v>
+      </c>
+      <c r="B896" t="s">
+        <v>1055</v>
       </c>
     </row>
     <row r="897" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B897" t="s">
-        <v>820</v>
+        <v>580</v>
       </c>
       <c r="D897">
         <v>5</v>
       </c>
       <c r="E897" t="s">
-        <v>861</v>
+        <v>854</v>
+      </c>
+      <c r="F897" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="898" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
         <v>134</v>
       </c>
-      <c r="B898" t="s">
-        <v>826</v>
-      </c>
     </row>
     <row r="899" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
         <v>11</v>
       </c>
       <c r="B899" t="s">
-        <v>580</v>
+        <v>817</v>
       </c>
       <c r="D899">
         <v>5</v>
       </c>
       <c r="E899" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
       <c r="F899" t="s">
         <v>2</v>
@@ -14035,57 +14698,66 @@
     </row>
     <row r="900" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
-        <v>134</v>
-      </c>
-      <c r="B900" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="901" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A901" t="s">
-        <v>11</v>
-      </c>
-      <c r="B901" t="s">
-        <v>822</v>
-      </c>
-      <c r="D901">
-        <v>5</v>
-      </c>
-      <c r="E901" t="s">
-        <v>863</v>
-      </c>
-      <c r="F901" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="902" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="B902" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D902">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="903" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
+        <v>11</v>
+      </c>
+      <c r="B903" t="s">
+        <v>812</v>
+      </c>
+      <c r="D903">
+        <v>5</v>
+      </c>
+      <c r="E903" t="s">
+        <v>850</v>
+      </c>
+      <c r="F903" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="904" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A904" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="B904" t="s">
-        <v>576</v>
+        <v>818</v>
       </c>
       <c r="D904">
         <v>5</v>
+      </c>
+      <c r="E904" t="s">
+        <v>868</v>
+      </c>
+      <c r="F904" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="905" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A905" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B905" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="D905">
         <v>5</v>
       </c>
       <c r="E905" t="s">
-        <v>878</v>
+        <v>869</v>
       </c>
       <c r="F905" t="s">
         <v>2</v>
@@ -14093,82 +14765,79 @@
     </row>
     <row r="906" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
       <c r="B906" t="s">
-        <v>824</v>
-      </c>
-      <c r="D906">
-        <v>5</v>
-      </c>
-      <c r="E906" t="s">
-        <v>879</v>
-      </c>
-      <c r="F906" t="s">
-        <v>2</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="907" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A907" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="B907" t="s">
-        <v>825</v>
+        <v>820</v>
+      </c>
+      <c r="D907">
+        <v>5</v>
+      </c>
+      <c r="E907" t="s">
+        <v>870</v>
+      </c>
+      <c r="F907" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="908" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A908" t="s">
-        <v>11</v>
-      </c>
-      <c r="B908" t="s">
-        <v>827</v>
-      </c>
-      <c r="D908">
-        <v>5</v>
-      </c>
-      <c r="E908" t="s">
-        <v>880</v>
-      </c>
-      <c r="F908" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
     </row>
     <row r="909" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="B909" t="s">
-        <v>821</v>
+        <v>817</v>
+      </c>
+      <c r="E909" t="s">
+        <v>855</v>
+      </c>
+      <c r="F909" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="910" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
-        <v>11</v>
-      </c>
-      <c r="B910" t="s">
-        <v>822</v>
-      </c>
-      <c r="E910" t="s">
-        <v>863</v>
-      </c>
-      <c r="F910" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="911" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A911" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="912" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A912" t="s">
+        <v>133</v>
+      </c>
+      <c r="B912" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D912">
+        <v>5</v>
       </c>
     </row>
     <row r="913" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A913" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B913" t="s">
-        <v>828</v>
+        <v>811</v>
       </c>
       <c r="D913">
         <v>5</v>
+      </c>
+      <c r="E913" t="s">
+        <v>848</v>
+      </c>
+      <c r="F913" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="914" spans="1:6" x14ac:dyDescent="0.25">
@@ -14176,13 +14845,13 @@
         <v>68</v>
       </c>
       <c r="B914" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D914">
         <v>5</v>
       </c>
       <c r="E914" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="F914" t="s">
         <v>2</v>
@@ -14193,13 +14862,13 @@
         <v>67</v>
       </c>
       <c r="B915" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="D915">
         <v>5</v>
       </c>
       <c r="E915" t="s">
-        <v>868</v>
+        <v>858</v>
       </c>
       <c r="F915" t="s">
         <v>2</v>
@@ -14210,7 +14879,7 @@
         <v>134</v>
       </c>
       <c r="B916" t="s">
-        <v>867</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="917" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14218,13 +14887,13 @@
         <v>11</v>
       </c>
       <c r="B917" t="s">
-        <v>866</v>
+        <v>1089</v>
       </c>
       <c r="D917">
         <v>5</v>
       </c>
       <c r="E917" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="F917" t="s">
         <v>2</v>
@@ -14234,22 +14903,19 @@
       <c r="A918" t="s">
         <v>134</v>
       </c>
-      <c r="B918" t="s">
-        <v>821</v>
-      </c>
     </row>
     <row r="919" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A919" t="s">
         <v>11</v>
       </c>
       <c r="B919" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
       <c r="D919">
         <v>5</v>
       </c>
       <c r="E919" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="F919" t="s">
         <v>2</v>
@@ -14265,7 +14931,7 @@
         <v>133</v>
       </c>
       <c r="B922" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="D922">
         <v>5</v>
@@ -14276,13 +14942,13 @@
         <v>11</v>
       </c>
       <c r="B923" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="D923">
         <v>5</v>
       </c>
       <c r="E923" t="s">
-        <v>869</v>
+        <v>859</v>
       </c>
       <c r="F923" t="s">
         <v>2</v>
@@ -14290,24 +14956,33 @@
     </row>
     <row r="924" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A924" t="s">
-        <v>466</v>
+        <v>66</v>
       </c>
       <c r="B924" t="s">
-        <v>66</v>
+        <v>824</v>
+      </c>
+      <c r="D924">
+        <v>5</v>
+      </c>
+      <c r="E924" t="s">
+        <v>860</v>
+      </c>
+      <c r="F924" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="925" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A925" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B925" t="s">
-        <v>832</v>
+        <v>825</v>
       </c>
       <c r="D925">
         <v>5</v>
       </c>
       <c r="E925" t="s">
-        <v>870</v>
+        <v>861</v>
       </c>
       <c r="F925" t="s">
         <v>2</v>
@@ -14315,28 +14990,6 @@
     </row>
     <row r="926" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A926" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="927" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A927" t="s">
-        <v>11</v>
-      </c>
-      <c r="B927" t="s">
-        <v>833</v>
-      </c>
-      <c r="D927">
-        <v>5</v>
-      </c>
-      <c r="E927" t="s">
-        <v>871</v>
-      </c>
-      <c r="F927" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="928" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A928" t="s">
         <v>135</v>
       </c>
     </row>
@@ -14345,7 +14998,7 @@
         <v>133</v>
       </c>
       <c r="B930" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
     </row>
     <row r="931" spans="1:6" x14ac:dyDescent="0.25">
@@ -14353,13 +15006,13 @@
         <v>67</v>
       </c>
       <c r="B931" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="D931">
         <v>5</v>
       </c>
       <c r="E931" t="s">
-        <v>872</v>
+        <v>862</v>
       </c>
       <c r="F931" t="s">
         <v>2</v>
@@ -14367,37 +15020,36 @@
     </row>
     <row r="932" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A932" t="s">
-        <v>466</v>
+        <v>67</v>
       </c>
       <c r="B932" t="s">
-        <v>68</v>
+        <v>827</v>
+      </c>
+      <c r="D932">
+        <v>5</v>
+      </c>
+      <c r="E932" t="s">
+        <v>858</v>
+      </c>
+      <c r="F932" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="933" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A933" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="B933" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="D933">
         <v>5</v>
       </c>
       <c r="E933" t="s">
-        <v>868</v>
+        <v>858</v>
       </c>
       <c r="F933" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="934" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A934" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="935" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A935" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="937" spans="1:6" x14ac:dyDescent="0.25">
@@ -14405,7 +15057,7 @@
         <v>133</v>
       </c>
       <c r="B937" t="s">
-        <v>887</v>
+        <v>877</v>
       </c>
     </row>
     <row r="938" spans="1:6" x14ac:dyDescent="0.25">
@@ -14413,13 +15065,13 @@
         <v>66</v>
       </c>
       <c r="B938" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="D938">
         <v>5</v>
       </c>
       <c r="E938" t="s">
-        <v>873</v>
+        <v>863</v>
       </c>
       <c r="F938" t="s">
         <v>2</v>
@@ -14427,11 +15079,6 @@
     </row>
     <row r="939" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A939" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="940" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A940" t="s">
         <v>135</v>
       </c>
     </row>
@@ -14440,7 +15087,7 @@
         <v>133</v>
       </c>
       <c r="B942" t="s">
-        <v>888</v>
+        <v>878</v>
       </c>
     </row>
     <row r="943" spans="1:6" x14ac:dyDescent="0.25">
@@ -14448,7 +15095,7 @@
         <v>466</v>
       </c>
       <c r="B943" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
     </row>
     <row r="944" spans="1:6" x14ac:dyDescent="0.25">
@@ -14456,13 +15103,13 @@
         <v>68</v>
       </c>
       <c r="B944" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="D944">
         <v>5</v>
       </c>
       <c r="E944" t="s">
-        <v>874</v>
+        <v>864</v>
       </c>
       <c r="F944" t="s">
         <v>2</v>
@@ -14478,13 +15125,13 @@
         <v>68</v>
       </c>
       <c r="B946" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="D946">
         <v>5</v>
       </c>
       <c r="E946" t="s">
-        <v>875</v>
+        <v>865</v>
       </c>
       <c r="F946" t="s">
         <v>2</v>
@@ -14505,7 +15152,7 @@
         <v>133</v>
       </c>
       <c r="B950" t="s">
-        <v>881</v>
+        <v>871</v>
       </c>
       <c r="D950">
         <v>5</v>
@@ -14516,13 +15163,13 @@
         <v>67</v>
       </c>
       <c r="B951" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="D951">
         <v>5</v>
       </c>
       <c r="E951" t="s">
-        <v>990</v>
+        <v>980</v>
       </c>
       <c r="F951" t="s">
         <v>2</v>
@@ -14533,13 +15180,13 @@
         <v>66</v>
       </c>
       <c r="B952" t="s">
-        <v>883</v>
+        <v>873</v>
       </c>
       <c r="D952">
         <v>5</v>
       </c>
       <c r="E952" t="s">
-        <v>991</v>
+        <v>981</v>
       </c>
       <c r="F952" t="s">
         <v>2</v>
@@ -14550,13 +15197,13 @@
         <v>67</v>
       </c>
       <c r="B953" t="s">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="D953">
         <v>5</v>
       </c>
       <c r="E953" t="s">
-        <v>992</v>
+        <v>982</v>
       </c>
       <c r="F953" t="s">
         <v>2</v>
@@ -14567,13 +15214,13 @@
         <v>67</v>
       </c>
       <c r="B954" t="s">
-        <v>884</v>
+        <v>874</v>
       </c>
       <c r="D954">
         <v>5</v>
       </c>
       <c r="E954" t="s">
-        <v>875</v>
+        <v>865</v>
       </c>
       <c r="F954" t="s">
         <v>2</v>
@@ -14584,13 +15231,13 @@
         <v>66</v>
       </c>
       <c r="B955" t="s">
-        <v>885</v>
+        <v>875</v>
       </c>
       <c r="D955">
         <v>5</v>
       </c>
       <c r="E955" t="s">
-        <v>993</v>
+        <v>983</v>
       </c>
       <c r="F955" t="s">
         <v>2</v>
@@ -14601,13 +15248,13 @@
         <v>67</v>
       </c>
       <c r="B956" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="D956">
         <v>5</v>
       </c>
       <c r="E956" t="s">
-        <v>994</v>
+        <v>984</v>
       </c>
       <c r="F956" t="s">
         <v>2</v>
@@ -14618,13 +15265,13 @@
         <v>67</v>
       </c>
       <c r="B957" t="s">
-        <v>889</v>
+        <v>879</v>
       </c>
       <c r="D957">
         <v>5</v>
       </c>
       <c r="E957" t="s">
-        <v>995</v>
+        <v>985</v>
       </c>
       <c r="F957" t="s">
         <v>2</v>
@@ -14635,7 +15282,7 @@
         <v>134</v>
       </c>
       <c r="B958" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
     </row>
     <row r="959" spans="1:6" x14ac:dyDescent="0.25">
@@ -14643,13 +15290,13 @@
         <v>11</v>
       </c>
       <c r="B959" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="D959">
         <v>5</v>
       </c>
       <c r="E959" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="F959" t="s">
         <v>2</v>
@@ -14660,7 +15307,7 @@
         <v>134</v>
       </c>
       <c r="B960" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
     </row>
     <row r="961" spans="1:6" x14ac:dyDescent="0.25">
@@ -14674,7 +15321,7 @@
         <v>5</v>
       </c>
       <c r="E961" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="F961" t="s">
         <v>2</v>
@@ -14690,7 +15337,7 @@
         <v>133</v>
       </c>
       <c r="B964" t="s">
-        <v>893</v>
+        <v>883</v>
       </c>
       <c r="D964">
         <v>5</v>
@@ -14701,7 +15348,7 @@
         <v>466</v>
       </c>
       <c r="B965" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
     </row>
     <row r="966" spans="1:6" x14ac:dyDescent="0.25">
@@ -14709,13 +15356,13 @@
         <v>68</v>
       </c>
       <c r="B966" t="s">
-        <v>894</v>
+        <v>884</v>
       </c>
       <c r="D966">
         <v>5</v>
       </c>
       <c r="E966" t="s">
-        <v>996</v>
+        <v>986</v>
       </c>
       <c r="F966" t="s">
         <v>2</v>
@@ -14731,13 +15378,13 @@
         <v>68</v>
       </c>
       <c r="B968" t="s">
-        <v>895</v>
+        <v>885</v>
       </c>
       <c r="D968">
         <v>5</v>
       </c>
       <c r="E968" t="s">
-        <v>997</v>
+        <v>987</v>
       </c>
       <c r="F968" t="s">
         <v>2</v>
@@ -14753,13 +15400,13 @@
         <v>68</v>
       </c>
       <c r="B970" t="s">
-        <v>896</v>
+        <v>886</v>
       </c>
       <c r="D970">
         <v>5</v>
       </c>
       <c r="E970" t="s">
-        <v>998</v>
+        <v>988</v>
       </c>
       <c r="F970" t="s">
         <v>2</v>
@@ -14770,13 +15417,13 @@
         <v>66</v>
       </c>
       <c r="B971" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="D971">
         <v>5</v>
       </c>
       <c r="E971" t="s">
-        <v>999</v>
+        <v>989</v>
       </c>
       <c r="F971" t="s">
         <v>2</v>
@@ -14787,7 +15434,7 @@
         <v>134</v>
       </c>
       <c r="B972" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
     </row>
     <row r="973" spans="1:6" x14ac:dyDescent="0.25">
@@ -14795,13 +15442,13 @@
         <v>11</v>
       </c>
       <c r="B973" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="D973">
         <v>5</v>
       </c>
       <c r="E973" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="F973" t="s">
         <v>2</v>
@@ -14812,7 +15459,7 @@
         <v>134</v>
       </c>
       <c r="B974" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
     </row>
     <row r="975" spans="1:6" x14ac:dyDescent="0.25">
@@ -14826,7 +15473,7 @@
         <v>5</v>
       </c>
       <c r="E975" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="F975" t="s">
         <v>2</v>
@@ -14842,7 +15489,7 @@
         <v>133</v>
       </c>
       <c r="B978" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="D978">
         <v>5</v>
@@ -14853,13 +15500,13 @@
         <v>66</v>
       </c>
       <c r="B979" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="D979">
         <v>5</v>
       </c>
       <c r="E979" t="s">
-        <v>1000</v>
+        <v>990</v>
       </c>
       <c r="F979" t="s">
         <v>2</v>
@@ -14870,13 +15517,13 @@
         <v>67</v>
       </c>
       <c r="B980" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="D980">
         <v>5</v>
       </c>
       <c r="E980" t="s">
-        <v>1001</v>
+        <v>991</v>
       </c>
       <c r="F980" t="s">
         <v>2</v>
@@ -14887,13 +15534,13 @@
         <v>68</v>
       </c>
       <c r="B981" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="D981">
         <v>5</v>
       </c>
       <c r="E981" t="s">
-        <v>1002</v>
+        <v>992</v>
       </c>
       <c r="F981" t="s">
         <v>2</v>
@@ -14904,7 +15551,7 @@
         <v>134</v>
       </c>
       <c r="B982" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
     </row>
     <row r="983" spans="1:6" x14ac:dyDescent="0.25">
@@ -14912,13 +15559,13 @@
         <v>11</v>
       </c>
       <c r="B983" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="D983">
         <v>5</v>
       </c>
       <c r="E983" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="F983" t="s">
         <v>2</v>
@@ -14929,7 +15576,7 @@
         <v>134</v>
       </c>
       <c r="B984" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
     </row>
     <row r="985" spans="1:6" x14ac:dyDescent="0.25">
@@ -14943,7 +15590,7 @@
         <v>5</v>
       </c>
       <c r="E985" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="F985" t="s">
         <v>2</v>
@@ -14959,7 +15606,7 @@
         <v>133</v>
       </c>
       <c r="B988" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="D988">
         <v>5</v>
@@ -14970,10 +15617,10 @@
         <v>66</v>
       </c>
       <c r="B989" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="E989" t="s">
-        <v>1003</v>
+        <v>993</v>
       </c>
       <c r="F989" t="s">
         <v>2</v>
@@ -14989,7 +15636,7 @@
         <v>133</v>
       </c>
       <c r="B992" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="D992">
         <v>5</v>
@@ -15000,7 +15647,7 @@
         <v>466</v>
       </c>
       <c r="B993" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
     </row>
     <row r="994" spans="1:6" x14ac:dyDescent="0.25">
@@ -15008,13 +15655,13 @@
         <v>68</v>
       </c>
       <c r="B994" t="s">
-        <v>906</v>
+        <v>896</v>
       </c>
       <c r="D994">
         <v>5</v>
       </c>
       <c r="E994" t="s">
-        <v>1004</v>
+        <v>994</v>
       </c>
       <c r="F994" t="s">
         <v>2</v>
@@ -15030,13 +15677,13 @@
         <v>68</v>
       </c>
       <c r="B996" t="s">
-        <v>907</v>
+        <v>897</v>
       </c>
       <c r="D996">
         <v>5</v>
       </c>
       <c r="E996" t="s">
-        <v>1005</v>
+        <v>995</v>
       </c>
       <c r="F996" t="s">
         <v>2</v>
@@ -15060,7 +15707,7 @@
         <v>133</v>
       </c>
       <c r="B1000" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="D1000">
         <v>5</v>
@@ -15071,13 +15718,13 @@
         <v>67</v>
       </c>
       <c r="B1001" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="D1001">
         <v>5</v>
       </c>
       <c r="E1001" t="s">
-        <v>1006</v>
+        <v>996</v>
       </c>
       <c r="F1001" t="s">
         <v>2</v>
@@ -15093,7 +15740,7 @@
         <v>133</v>
       </c>
       <c r="B1004" t="s">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="D1004">
         <v>5</v>
@@ -15104,13 +15751,13 @@
         <v>67</v>
       </c>
       <c r="B1005" t="s">
-        <v>984</v>
+        <v>974</v>
       </c>
       <c r="D1005">
         <v>5</v>
       </c>
       <c r="E1005" t="s">
-        <v>1007</v>
+        <v>997</v>
       </c>
       <c r="F1005" t="s">
         <v>2</v>
@@ -15126,7 +15773,7 @@
         <v>133</v>
       </c>
       <c r="B1008" t="s">
-        <v>985</v>
+        <v>975</v>
       </c>
       <c r="D1008">
         <v>5</v>
@@ -15137,33 +15784,33 @@
         <v>466</v>
       </c>
       <c r="B1009" t="s">
-        <v>986</v>
+        <v>976</v>
       </c>
     </row>
     <row r="1010" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="B1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="C1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="D1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="E1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="F1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="G1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="H1010" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
     </row>
     <row r="1011" spans="1:8" x14ac:dyDescent="0.25">
@@ -15231,10 +15878,10 @@
         <v>68</v>
       </c>
       <c r="B1017" t="s">
-        <v>988</v>
+        <v>978</v>
       </c>
       <c r="E1017" t="s">
-        <v>1008</v>
+        <v>998</v>
       </c>
       <c r="F1017" t="s">
         <v>2</v>
@@ -15255,7 +15902,7 @@
         <v>133</v>
       </c>
       <c r="B1021" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="D1021">
         <v>5</v>
@@ -15274,13 +15921,13 @@
         <v>67</v>
       </c>
       <c r="B1023" t="s">
-        <v>909</v>
+        <v>899</v>
       </c>
       <c r="D1023">
         <v>5</v>
       </c>
       <c r="E1023" t="s">
-        <v>1009</v>
+        <v>999</v>
       </c>
       <c r="F1023" t="s">
         <v>2</v>
@@ -15291,7 +15938,7 @@
         <v>134</v>
       </c>
       <c r="B1024" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
     </row>
     <row r="1025" spans="1:6" x14ac:dyDescent="0.25">
@@ -15299,13 +15946,13 @@
         <v>11</v>
       </c>
       <c r="B1025" t="s">
-        <v>911</v>
+        <v>901</v>
       </c>
       <c r="D1025">
         <v>5</v>
       </c>
       <c r="E1025" t="s">
-        <v>1010</v>
+        <v>1000</v>
       </c>
       <c r="F1025" t="s">
         <v>2</v>
@@ -15316,7 +15963,7 @@
         <v>134</v>
       </c>
       <c r="B1026" t="s">
-        <v>927</v>
+        <v>917</v>
       </c>
     </row>
     <row r="1027" spans="1:6" x14ac:dyDescent="0.25">
@@ -15324,13 +15971,13 @@
         <v>11</v>
       </c>
       <c r="B1027" t="s">
-        <v>912</v>
+        <v>902</v>
       </c>
       <c r="D1027">
         <v>5</v>
       </c>
       <c r="E1027" t="s">
-        <v>1011</v>
+        <v>1001</v>
       </c>
       <c r="F1027" t="s">
         <v>2</v>
@@ -15354,13 +16001,13 @@
         <v>66</v>
       </c>
       <c r="B1030" t="s">
-        <v>925</v>
+        <v>915</v>
       </c>
       <c r="D1030">
         <v>5</v>
       </c>
       <c r="E1030" t="s">
-        <v>1012</v>
+        <v>1002</v>
       </c>
       <c r="F1030" t="s">
         <v>2</v>
@@ -15371,13 +16018,13 @@
         <v>66</v>
       </c>
       <c r="B1031" t="s">
-        <v>926</v>
+        <v>916</v>
       </c>
       <c r="D1031">
         <v>5</v>
       </c>
       <c r="E1031" t="s">
-        <v>1013</v>
+        <v>1003</v>
       </c>
       <c r="F1031" t="s">
         <v>2</v>
@@ -15388,7 +16035,7 @@
         <v>134</v>
       </c>
       <c r="B1032" t="s">
-        <v>929</v>
+        <v>919</v>
       </c>
     </row>
     <row r="1033" spans="1:6" x14ac:dyDescent="0.25">
@@ -15396,13 +16043,13 @@
         <v>11</v>
       </c>
       <c r="B1033" t="s">
-        <v>928</v>
+        <v>918</v>
       </c>
       <c r="D1033">
         <v>5</v>
       </c>
       <c r="E1033" t="s">
-        <v>1014</v>
+        <v>1004</v>
       </c>
       <c r="F1033" t="s">
         <v>2</v>
@@ -15413,7 +16060,7 @@
         <v>134</v>
       </c>
       <c r="B1034" t="s">
-        <v>929</v>
+        <v>919</v>
       </c>
     </row>
     <row r="1035" spans="1:6" x14ac:dyDescent="0.25">
@@ -15421,10 +16068,10 @@
         <v>11</v>
       </c>
       <c r="B1035" t="s">
-        <v>930</v>
+        <v>920</v>
       </c>
       <c r="E1035" t="s">
-        <v>1015</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="1036" spans="1:6" x14ac:dyDescent="0.25">
@@ -15437,7 +16084,7 @@
         <v>133</v>
       </c>
       <c r="B1038" t="s">
-        <v>929</v>
+        <v>919</v>
       </c>
       <c r="D1038">
         <v>5</v>
@@ -15448,13 +16095,13 @@
         <v>66</v>
       </c>
       <c r="B1039" t="s">
-        <v>931</v>
+        <v>921</v>
       </c>
       <c r="D1039">
         <v>5</v>
       </c>
       <c r="E1039" t="s">
-        <v>1016</v>
+        <v>1006</v>
       </c>
       <c r="F1039" t="s">
         <v>2</v>
@@ -15465,13 +16112,13 @@
         <v>66</v>
       </c>
       <c r="B1040" t="s">
-        <v>932</v>
+        <v>922</v>
       </c>
       <c r="D1040">
         <v>5</v>
       </c>
       <c r="E1040" t="s">
-        <v>1017</v>
+        <v>1007</v>
       </c>
       <c r="F1040" t="s">
         <v>2</v>
@@ -15482,13 +16129,13 @@
         <v>66</v>
       </c>
       <c r="B1041" t="s">
-        <v>933</v>
+        <v>923</v>
       </c>
       <c r="D1041">
         <v>5</v>
       </c>
       <c r="E1041" t="s">
-        <v>1018</v>
+        <v>1008</v>
       </c>
       <c r="F1041" t="s">
         <v>2</v>
@@ -15499,13 +16146,13 @@
         <v>66</v>
       </c>
       <c r="B1042" t="s">
-        <v>934</v>
+        <v>924</v>
       </c>
       <c r="D1042">
         <v>5</v>
       </c>
       <c r="E1042" t="s">
-        <v>1019</v>
+        <v>1009</v>
       </c>
       <c r="F1042" t="s">
         <v>2</v>
@@ -15516,13 +16163,13 @@
         <v>66</v>
       </c>
       <c r="B1043" t="s">
-        <v>935</v>
+        <v>925</v>
       </c>
       <c r="D1043">
         <v>5</v>
       </c>
       <c r="E1043" t="s">
-        <v>1020</v>
+        <v>1010</v>
       </c>
       <c r="F1043" t="s">
         <v>2</v>
@@ -15538,7 +16185,7 @@
         <v>133</v>
       </c>
       <c r="B1046" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="D1046">
         <v>5</v>
@@ -15549,13 +16196,13 @@
         <v>67</v>
       </c>
       <c r="B1047" t="s">
-        <v>913</v>
+        <v>903</v>
       </c>
       <c r="D1047">
         <v>5</v>
       </c>
       <c r="E1047" t="s">
-        <v>1021</v>
+        <v>1011</v>
       </c>
       <c r="F1047" t="s">
         <v>2</v>
@@ -15566,13 +16213,13 @@
         <v>11</v>
       </c>
       <c r="B1048" t="s">
-        <v>914</v>
+        <v>904</v>
       </c>
       <c r="D1048">
         <v>5</v>
       </c>
       <c r="E1048" t="s">
-        <v>1022</v>
+        <v>1012</v>
       </c>
       <c r="F1048" t="s">
         <v>2</v>
@@ -15583,13 +16230,13 @@
         <v>67</v>
       </c>
       <c r="B1049" t="s">
-        <v>915</v>
+        <v>905</v>
       </c>
       <c r="D1049">
         <v>5</v>
       </c>
       <c r="E1049" t="s">
-        <v>1023</v>
+        <v>1013</v>
       </c>
       <c r="F1049" t="s">
         <v>2</v>
@@ -15600,7 +16247,7 @@
         <v>134</v>
       </c>
       <c r="B1050" t="s">
-        <v>916</v>
+        <v>906</v>
       </c>
     </row>
     <row r="1051" spans="1:6" x14ac:dyDescent="0.25">
@@ -15608,13 +16255,13 @@
         <v>11</v>
       </c>
       <c r="B1051" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="D1051">
         <v>5</v>
       </c>
       <c r="E1051" t="s">
-        <v>1024</v>
+        <v>1014</v>
       </c>
       <c r="F1051" t="s">
         <v>2</v>
@@ -15625,7 +16272,7 @@
         <v>134</v>
       </c>
       <c r="B1052" t="s">
-        <v>927</v>
+        <v>917</v>
       </c>
     </row>
     <row r="1053" spans="1:6" x14ac:dyDescent="0.25">
@@ -15633,13 +16280,13 @@
         <v>11</v>
       </c>
       <c r="B1053" t="s">
-        <v>918</v>
+        <v>908</v>
       </c>
       <c r="D1053">
         <v>5</v>
       </c>
       <c r="E1053" t="s">
-        <v>1025</v>
+        <v>1015</v>
       </c>
       <c r="F1053" t="s">
         <v>2</v>
@@ -15655,7 +16302,7 @@
         <v>133</v>
       </c>
       <c r="B1056" t="s">
-        <v>927</v>
+        <v>917</v>
       </c>
       <c r="D1056">
         <v>5</v>
@@ -15666,13 +16313,13 @@
         <v>67</v>
       </c>
       <c r="B1057" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
       <c r="D1057">
         <v>5</v>
       </c>
       <c r="E1057" t="s">
-        <v>1026</v>
+        <v>1016</v>
       </c>
       <c r="F1057" t="s">
         <v>2</v>
@@ -15688,7 +16335,7 @@
         <v>133</v>
       </c>
       <c r="B1060" t="s">
-        <v>936</v>
+        <v>926</v>
       </c>
       <c r="D1060">
         <v>5</v>
@@ -15699,13 +16346,13 @@
         <v>66</v>
       </c>
       <c r="B1061" t="s">
-        <v>937</v>
+        <v>927</v>
       </c>
       <c r="D1061">
         <v>5</v>
       </c>
       <c r="E1061" t="s">
-        <v>1027</v>
+        <v>1017</v>
       </c>
       <c r="F1061" t="s">
         <v>2</v>
@@ -15721,7 +16368,7 @@
         <v>133</v>
       </c>
       <c r="B1064" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="D1064">
         <v>5</v>
@@ -15740,13 +16387,13 @@
         <v>67</v>
       </c>
       <c r="B1066" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="D1066">
         <v>5</v>
       </c>
       <c r="E1066" t="s">
-        <v>868</v>
+        <v>858</v>
       </c>
       <c r="F1066" t="s">
         <v>2</v>
@@ -15757,13 +16404,13 @@
         <v>11</v>
       </c>
       <c r="B1067" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="D1067">
         <v>5</v>
       </c>
       <c r="E1067" t="s">
-        <v>1028</v>
+        <v>1018</v>
       </c>
       <c r="F1067" t="s">
         <v>2</v>
@@ -15774,13 +16421,13 @@
         <v>67</v>
       </c>
       <c r="B1068" t="s">
-        <v>922</v>
+        <v>912</v>
       </c>
       <c r="D1068">
         <v>5</v>
       </c>
       <c r="E1068" t="s">
-        <v>1029</v>
+        <v>1019</v>
       </c>
       <c r="F1068" t="s">
         <v>2</v>
@@ -15804,13 +16451,13 @@
         <v>11</v>
       </c>
       <c r="B1071" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="D1071">
         <v>5</v>
       </c>
       <c r="E1071" t="s">
-        <v>1028</v>
+        <v>1018</v>
       </c>
       <c r="F1071" t="s">
         <v>2</v>
@@ -15821,13 +16468,13 @@
         <v>66</v>
       </c>
       <c r="B1072" t="s">
-        <v>938</v>
+        <v>928</v>
       </c>
       <c r="D1072">
         <v>5</v>
       </c>
       <c r="E1072" t="s">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="F1072" t="s">
         <v>2</v>
@@ -15843,13 +16490,13 @@
         <v>68</v>
       </c>
       <c r="B1074" t="s">
-        <v>923</v>
+        <v>913</v>
       </c>
       <c r="D1074">
         <v>5</v>
       </c>
       <c r="E1074" t="s">
-        <v>1031</v>
+        <v>1021</v>
       </c>
       <c r="F1074" t="s">
         <v>2</v>
@@ -15860,13 +16507,13 @@
         <v>11</v>
       </c>
       <c r="B1075" t="s">
-        <v>924</v>
+        <v>914</v>
       </c>
       <c r="D1075">
         <v>5</v>
       </c>
       <c r="E1075" t="s">
-        <v>1032</v>
+        <v>1022</v>
       </c>
       <c r="F1075" t="s">
         <v>2</v>
@@ -15882,7 +16529,7 @@
         <v>133</v>
       </c>
       <c r="B1078" t="s">
-        <v>939</v>
+        <v>929</v>
       </c>
       <c r="D1078">
         <v>5</v>
@@ -15901,13 +16548,13 @@
         <v>67</v>
       </c>
       <c r="B1080" t="s">
-        <v>940</v>
+        <v>930</v>
       </c>
       <c r="D1080">
         <v>5</v>
       </c>
       <c r="E1080" t="s">
-        <v>1033</v>
+        <v>1023</v>
       </c>
       <c r="F1080" t="s">
         <v>2</v>
@@ -15937,7 +16584,7 @@
         <v>5</v>
       </c>
       <c r="E1083" t="s">
-        <v>1034</v>
+        <v>1024</v>
       </c>
       <c r="F1083" t="s">
         <v>2</v>
@@ -15953,7 +16600,7 @@
         <v>134</v>
       </c>
       <c r="B1085" t="s">
-        <v>941</v>
+        <v>931</v>
       </c>
     </row>
     <row r="1086" spans="1:6" x14ac:dyDescent="0.25">
@@ -15961,13 +16608,13 @@
         <v>11</v>
       </c>
       <c r="B1086" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="D1086">
         <v>5</v>
       </c>
       <c r="E1086" t="s">
-        <v>1035</v>
+        <v>1025</v>
       </c>
       <c r="F1086" t="s">
         <v>2</v>
@@ -15978,7 +16625,7 @@
         <v>134</v>
       </c>
       <c r="B1087" t="s">
-        <v>942</v>
+        <v>932</v>
       </c>
     </row>
     <row r="1088" spans="1:6" x14ac:dyDescent="0.25">
@@ -15986,13 +16633,13 @@
         <v>11</v>
       </c>
       <c r="B1088" t="s">
-        <v>944</v>
+        <v>934</v>
       </c>
       <c r="D1088">
         <v>5</v>
       </c>
       <c r="E1088" t="s">
-        <v>1036</v>
+        <v>1026</v>
       </c>
       <c r="F1088" t="s">
         <v>2</v>
@@ -16008,7 +16655,7 @@
         <v>133</v>
       </c>
       <c r="B1091" t="s">
-        <v>941</v>
+        <v>931</v>
       </c>
       <c r="D1091">
         <v>5</v>
@@ -16025,7 +16672,7 @@
         <v>5</v>
       </c>
       <c r="E1092" t="s">
-        <v>1037</v>
+        <v>1027</v>
       </c>
       <c r="F1092" t="s">
         <v>2</v>
@@ -16041,7 +16688,7 @@
         <v>133</v>
       </c>
       <c r="B1095" t="s">
-        <v>942</v>
+        <v>932</v>
       </c>
       <c r="D1095">
         <v>5</v>
@@ -16052,13 +16699,13 @@
         <v>11</v>
       </c>
       <c r="B1096" t="s">
-        <v>945</v>
+        <v>935</v>
       </c>
       <c r="D1096">
         <v>5</v>
       </c>
       <c r="E1096" t="s">
-        <v>1036</v>
+        <v>1026</v>
       </c>
       <c r="F1096" t="s">
         <v>2</v>
@@ -16074,7 +16721,7 @@
         <v>133</v>
       </c>
       <c r="B1099" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="D1099">
         <v>5</v>
@@ -16085,13 +16732,13 @@
         <v>71</v>
       </c>
       <c r="B1100" t="s">
-        <v>949</v>
+        <v>939</v>
       </c>
       <c r="D1100">
         <v>5</v>
       </c>
       <c r="E1100" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="F1100" t="s">
         <v>2</v>
@@ -16107,7 +16754,7 @@
         <v>133</v>
       </c>
       <c r="B1103" t="s">
-        <v>947</v>
+        <v>937</v>
       </c>
       <c r="D1103">
         <v>5</v>
@@ -16118,13 +16765,13 @@
         <v>71</v>
       </c>
       <c r="B1104" t="s">
-        <v>957</v>
+        <v>947</v>
       </c>
       <c r="D1104">
         <v>5</v>
       </c>
       <c r="E1104" t="s">
-        <v>1039</v>
+        <v>1029</v>
       </c>
       <c r="F1104" t="s">
         <v>2</v>
@@ -16140,7 +16787,7 @@
         <v>133</v>
       </c>
       <c r="B1107" t="s">
-        <v>948</v>
+        <v>938</v>
       </c>
       <c r="D1107">
         <v>5</v>
@@ -16151,13 +16798,13 @@
         <v>71</v>
       </c>
       <c r="B1108" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="D1108">
         <v>5</v>
       </c>
       <c r="E1108" t="s">
-        <v>1041</v>
+        <v>1031</v>
       </c>
       <c r="F1108" t="s">
         <v>2</v>
@@ -16170,10 +16817,10 @@
     </row>
     <row r="1111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1111" t="s">
-        <v>950</v>
+        <v>940</v>
       </c>
       <c r="B1111" t="s">
-        <v>951</v>
+        <v>941</v>
       </c>
       <c r="D1111">
         <v>5</v>
@@ -16181,13 +16828,13 @@
     </row>
     <row r="1112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1112" t="s">
-        <v>953</v>
+        <v>943</v>
       </c>
       <c r="B1112" t="s">
-        <v>952</v>
+        <v>942</v>
       </c>
       <c r="E1112" t="s">
-        <v>1042</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="1113" spans="1:6" x14ac:dyDescent="0.25">
@@ -16203,13 +16850,13 @@
         <v>67</v>
       </c>
       <c r="B1114" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="D1114">
         <v>5</v>
       </c>
       <c r="E1114" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="F1114" t="s">
         <v>2</v>
@@ -16233,13 +16880,13 @@
         <v>66</v>
       </c>
       <c r="B1117" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="D1117">
         <v>5</v>
       </c>
       <c r="E1117" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="F1117" t="s">
         <v>2</v>
@@ -16263,13 +16910,13 @@
         <v>68</v>
       </c>
       <c r="B1120" t="s">
-        <v>955</v>
+        <v>945</v>
       </c>
       <c r="D1120">
         <v>5</v>
       </c>
       <c r="E1120" t="s">
-        <v>1045</v>
+        <v>1035</v>
       </c>
       <c r="F1120" t="s">
         <v>2</v>
@@ -16285,13 +16932,13 @@
         <v>11</v>
       </c>
       <c r="B1122" t="s">
-        <v>956</v>
+        <v>946</v>
       </c>
       <c r="D1122">
         <v>5</v>
       </c>
       <c r="E1122" t="s">
-        <v>1046</v>
+        <v>1036</v>
       </c>
       <c r="F1122" t="s">
         <v>2</v>
@@ -16307,7 +16954,7 @@
         <v>133</v>
       </c>
       <c r="B1125" t="s">
-        <v>963</v>
+        <v>953</v>
       </c>
       <c r="D1125">
         <v>5</v>
@@ -16318,7 +16965,7 @@
         <v>134</v>
       </c>
       <c r="B1126" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
     </row>
     <row r="1127" spans="1:6" x14ac:dyDescent="0.25">
@@ -16332,7 +16979,7 @@
         <v>5</v>
       </c>
       <c r="E1127" t="s">
-        <v>965</v>
+        <v>955</v>
       </c>
       <c r="F1127" t="s">
         <v>2</v>
@@ -16343,7 +16990,7 @@
         <v>134</v>
       </c>
       <c r="B1128" t="s">
-        <v>967</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1129" spans="1:6" x14ac:dyDescent="0.25">
@@ -16357,7 +17004,7 @@
         <v>5</v>
       </c>
       <c r="E1129" t="s">
-        <v>964</v>
+        <v>954</v>
       </c>
       <c r="F1129" t="s">
         <v>2</v>
@@ -16373,7 +17020,7 @@
         <v>133</v>
       </c>
       <c r="B1132" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="D1132">
         <v>5</v>
@@ -16392,13 +17039,13 @@
         <v>68</v>
       </c>
       <c r="B1134" t="s">
-        <v>968</v>
+        <v>958</v>
       </c>
       <c r="D1134">
         <v>5</v>
       </c>
       <c r="E1134" t="s">
-        <v>1047</v>
+        <v>1037</v>
       </c>
       <c r="F1134" t="s">
         <v>2</v>
@@ -16422,13 +17069,13 @@
         <v>67</v>
       </c>
       <c r="B1137" t="s">
-        <v>969</v>
+        <v>959</v>
       </c>
       <c r="D1137">
         <v>5</v>
       </c>
       <c r="E1137" t="s">
-        <v>1048</v>
+        <v>1038</v>
       </c>
       <c r="F1137" t="s">
         <v>2</v>
@@ -16452,13 +17099,13 @@
         <v>66</v>
       </c>
       <c r="B1140" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
       <c r="D1140">
         <v>5</v>
       </c>
       <c r="E1140" t="s">
-        <v>1049</v>
+        <v>1039</v>
       </c>
       <c r="F1140" t="s">
         <v>2</v>
@@ -16474,7 +17121,7 @@
         <v>71</v>
       </c>
       <c r="B1142" t="s">
-        <v>970</v>
+        <v>960</v>
       </c>
     </row>
     <row r="1143" spans="1:6" x14ac:dyDescent="0.25">
@@ -16507,7 +17154,7 @@
         <v>134</v>
       </c>
       <c r="B1145" t="s">
-        <v>972</v>
+        <v>962</v>
       </c>
     </row>
     <row r="1146" spans="1:6" x14ac:dyDescent="0.25">
@@ -16537,7 +17184,7 @@
         <v>133</v>
       </c>
       <c r="B1149" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="D1149">
         <v>5</v>
@@ -16554,7 +17201,7 @@
         <v>5</v>
       </c>
       <c r="E1150" t="s">
-        <v>1050</v>
+        <v>1040</v>
       </c>
       <c r="F1150" t="s">
         <v>2</v>
@@ -16570,7 +17217,7 @@
         <v>133</v>
       </c>
       <c r="B1153" t="s">
-        <v>967</v>
+        <v>957</v>
       </c>
       <c r="D1153">
         <v>5</v>
@@ -16581,10 +17228,10 @@
         <v>71</v>
       </c>
       <c r="B1154" t="s">
-        <v>973</v>
+        <v>963</v>
       </c>
       <c r="E1154" t="s">
-        <v>1051</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="1155" spans="1:6" x14ac:dyDescent="0.25">
@@ -16600,13 +17247,13 @@
         <v>67</v>
       </c>
       <c r="B1156" t="s">
-        <v>974</v>
+        <v>964</v>
       </c>
       <c r="D1156">
         <v>5</v>
       </c>
       <c r="E1156" t="s">
-        <v>1052</v>
+        <v>1042</v>
       </c>
       <c r="F1156" t="s">
         <v>2</v>
@@ -16630,13 +17277,13 @@
         <v>68</v>
       </c>
       <c r="B1159" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="D1159">
         <v>5</v>
       </c>
       <c r="E1159" t="s">
-        <v>1053</v>
+        <v>1043</v>
       </c>
       <c r="F1159" t="s">
         <v>2</v>
@@ -16660,13 +17307,13 @@
         <v>66</v>
       </c>
       <c r="B1162" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="D1162">
         <v>5</v>
       </c>
       <c r="E1162" t="s">
-        <v>1054</v>
+        <v>1044</v>
       </c>
       <c r="F1162" t="s">
         <v>2</v>
@@ -16677,13 +17324,13 @@
         <v>66</v>
       </c>
       <c r="B1163" t="s">
-        <v>977</v>
+        <v>967</v>
       </c>
       <c r="D1163">
         <v>5</v>
       </c>
       <c r="E1163" t="s">
-        <v>1055</v>
+        <v>1045</v>
       </c>
       <c r="F1163" t="s">
         <v>2</v>
@@ -16694,13 +17341,13 @@
         <v>71</v>
       </c>
       <c r="B1164" t="s">
-        <v>978</v>
+        <v>968</v>
       </c>
       <c r="D1164">
         <v>5</v>
       </c>
       <c r="E1164" t="s">
-        <v>1038</v>
+        <v>1028</v>
       </c>
       <c r="F1164" t="s">
         <v>2</v>
@@ -16711,13 +17358,13 @@
         <v>11</v>
       </c>
       <c r="B1165" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="D1165">
         <v>5</v>
       </c>
       <c r="E1165" t="s">
-        <v>1056</v>
+        <v>1046</v>
       </c>
       <c r="F1165" t="s">
         <v>2</v>
@@ -16728,13 +17375,13 @@
         <v>11</v>
       </c>
       <c r="B1166" t="s">
-        <v>980</v>
+        <v>970</v>
       </c>
       <c r="D1166">
         <v>5</v>
       </c>
       <c r="E1166" t="s">
-        <v>1057</v>
+        <v>1047</v>
       </c>
       <c r="F1166" t="s">
         <v>2</v>
@@ -16745,13 +17392,13 @@
         <v>71</v>
       </c>
       <c r="B1167" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
       <c r="D1167">
         <v>5</v>
       </c>
       <c r="E1167" t="s">
-        <v>1058</v>
+        <v>1048</v>
       </c>
       <c r="F1167" t="s">
         <v>2</v>
@@ -16775,13 +17422,13 @@
         <v>67</v>
       </c>
       <c r="B1170" t="s">
-        <v>982</v>
+        <v>972</v>
       </c>
       <c r="D1170">
         <v>5</v>
       </c>
       <c r="E1170" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="F1170" t="s">
         <v>2</v>
@@ -16792,13 +17439,13 @@
         <v>71</v>
       </c>
       <c r="B1171" t="s">
-        <v>978</v>
+        <v>968</v>
       </c>
       <c r="D1171">
         <v>5</v>
       </c>
       <c r="E1171" t="s">
-        <v>1038</v>
+        <v>1028</v>
       </c>
       <c r="F1171" t="s">
         <v>2</v>
@@ -16809,13 +17456,13 @@
         <v>11</v>
       </c>
       <c r="B1172" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="D1172">
         <v>5</v>
       </c>
       <c r="E1172" t="s">
-        <v>1056</v>
+        <v>1046</v>
       </c>
       <c r="F1172" t="s">
         <v>2</v>
@@ -16826,13 +17473,13 @@
         <v>11</v>
       </c>
       <c r="B1173" t="s">
-        <v>980</v>
+        <v>970</v>
       </c>
       <c r="D1173">
         <v>5</v>
       </c>
       <c r="E1173" t="s">
-        <v>1057</v>
+        <v>1047</v>
       </c>
       <c r="F1173" t="s">
         <v>2</v>
@@ -16843,13 +17490,13 @@
         <v>71</v>
       </c>
       <c r="B1174" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
       <c r="D1174">
         <v>5</v>
       </c>
       <c r="E1174" t="s">
-        <v>1058</v>
+        <v>1048</v>
       </c>
       <c r="F1174" t="s">
         <v>2</v>
@@ -16865,7 +17512,7 @@
         <v>99</v>
       </c>
       <c r="B1177" t="s">
-        <v>989</v>
+        <v>979</v>
       </c>
     </row>
     <row r="1190" spans="1:7" x14ac:dyDescent="0.25">
@@ -17043,6 +17690,9 @@
       <c r="B1211" t="s">
         <v>691</v>
       </c>
+      <c r="D1211">
+        <v>7</v>
+      </c>
     </row>
     <row r="1212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1212" t="s">
@@ -17231,6 +17881,9 @@
       <c r="B1228" t="s">
         <v>695</v>
       </c>
+      <c r="D1228">
+        <v>7</v>
+      </c>
     </row>
     <row r="1229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1229" t="s">
@@ -17372,50 +18025,210 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+  <conditionalFormatting sqref="A1:H881 A883:H902 G903:H903 A904:H1048576">
+    <cfRule type="expression" dxfId="77" priority="31">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="76" priority="32">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="75" priority="33">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="74" priority="34">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="73" priority="35">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="72" priority="36">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="71" priority="37">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="70" priority="38">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="69" priority="39">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="68" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="67" priority="40" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="66" priority="41" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="12" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="65" priority="42" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="64" priority="43" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G882:H882">
+    <cfRule type="expression" dxfId="49" priority="77">
+      <formula>LEFT($A889, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="78">
+      <formula>$A889="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="79">
+      <formula>$A889="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="80">
+      <formula>$A889="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="81">
+      <formula>$A889="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="82">
+      <formula>$A889="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="83">
+      <formula>$A889="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="84">
+      <formula>$A889="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="85">
+      <formula>$A889="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="86">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G889:H889">
+    <cfRule type="expression" dxfId="39" priority="87">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="88">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="89">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="90">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="91">
+      <formula>#REF!="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="92">
+      <formula>#REF!="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="93">
+      <formula>#REF!="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="94">
+      <formula>#REF!="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="95">
+      <formula>#REF!="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="96">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A882:F882">
+    <cfRule type="expression" dxfId="29" priority="21">
+      <formula>LEFT($A882, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="22">
+      <formula>$A882="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="23">
+      <formula>$A882="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="24">
+      <formula>$A882="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="25">
+      <formula>$A882="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="26">
+      <formula>$A882="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="27">
+      <formula>$A882="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="28">
+      <formula>$A882="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="29">
+      <formula>$A882="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="30">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G887:H887">
+    <cfRule type="expression" dxfId="19" priority="11">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="12">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="14">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>#REF!="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>#REF!="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>#REF!="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>#REF!="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="19">
+      <formula>#REF!="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="20">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A903:F903">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>LEFT($A903, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="2">
+      <formula>$A903="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>$A903="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>$A903="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$A903="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$A903="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>$A903="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>$A903="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>$A903="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17498,10 +18311,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="B11" t="s">
-        <v>1070</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -17526,48 +18339,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="37" priority="1">
+    <cfRule type="expression" dxfId="63" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="2">
+    <cfRule type="expression" dxfId="62" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="3">
+    <cfRule type="expression" dxfId="61" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="60" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="5">
+    <cfRule type="expression" dxfId="59" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="6">
+    <cfRule type="expression" dxfId="58" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="7">
+    <cfRule type="expression" dxfId="57" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="8">
+    <cfRule type="expression" dxfId="56" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="9">
+    <cfRule type="expression" dxfId="55" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26">
+    <cfRule type="expression" dxfId="54" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="53" priority="13" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="52" priority="22" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="51" priority="24" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="50" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added some common conversations to each DayBehaviour
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AA3612-E00A-43A7-ACCB-2471A7752C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DC8D4A-35CE-4930-9705-2673741CA369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -4291,8 +4291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B392" sqref="B392"/>
+    <sheetView tabSelected="1" topLeftCell="A806" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B786" sqref="B786"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16963,6 +16963,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -17201,24 +17218,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17235,29 +17260,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added missing overcrowding convos
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DC8D4A-35CE-4930-9705-2673741CA369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC39FB2A-92F6-455E-9662-62C6E2FAB9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="1092">
   <si>
     <t>Context</t>
   </si>
@@ -4291,8 +4291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A806" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B786" sqref="B786"/>
+    <sheetView tabSelected="1" topLeftCell="A985" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C998" sqref="C998"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13668,18 +13668,6 @@
     <row r="931" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A931" t="s">
         <v>135</v>
-      </c>
-      <c r="B931" t="s">
-        <v>821</v>
-      </c>
-      <c r="D931">
-        <v>5</v>
-      </c>
-      <c r="E931" t="s">
-        <v>852</v>
-      </c>
-      <c r="F931" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="933" spans="1:6" x14ac:dyDescent="0.25">
@@ -16963,23 +16951,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -17218,32 +17189,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17260,4 +17223,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Day 6 morning complete
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC39FB2A-92F6-455E-9662-62C6E2FAB9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057F9F7B-B35A-41D9-97C5-84129EC932A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="1180">
   <si>
     <t>Context</t>
   </si>
@@ -3313,6 +3313,270 @@
   </si>
   <si>
     <t>p_5_is_the_car_violet</t>
+  </si>
+  <si>
+    <t>We should be alright for a few days at least.</t>
+  </si>
+  <si>
+    <t>p6_supplies</t>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>tv6</t>
+  </si>
+  <si>
+    <t>p6_outside</t>
+  </si>
+  <si>
+    <t>The war in Brasnia continues to expand outwards. Citizens of the north and east are expected to hear firefights and artillery. Ceasefire negotiations continue with the US still apprehensive.</t>
+  </si>
+  <si>
+    <t>It looks clearer and clearer by the day... still hostile though.</t>
+  </si>
+  <si>
+    <t>*STATIC*</t>
+  </si>
+  <si>
+    <t>Bob wakes up</t>
+  </si>
+  <si>
+    <t>Big guys got the TV down by the looks of it.</t>
+  </si>
+  <si>
+    <t>We could use some more information on what's happening.</t>
+  </si>
+  <si>
+    <t>It's just fighting and more fighting.</t>
+  </si>
+  <si>
+    <t>b_6_tv_taken_down</t>
+  </si>
+  <si>
+    <t>p_6_tv_could_use_info</t>
+  </si>
+  <si>
+    <t>b_6_tv_fighting</t>
+  </si>
+  <si>
+    <t>j_6_good_morning</t>
+  </si>
+  <si>
+    <t>*sigh*</t>
+  </si>
+  <si>
+    <t>Hi.</t>
+  </si>
+  <si>
+    <t>p_6_j_hi</t>
+  </si>
+  <si>
+    <t>*your beds arent half bad actually*</t>
+  </si>
+  <si>
+    <t>v_6_wake_up</t>
+  </si>
+  <si>
+    <t>Dad wakes up</t>
+  </si>
+  <si>
+    <t>Morning guys... Thanks for letting me stay the night.</t>
+  </si>
+  <si>
+    <t>Don't want to be that guy, but you did say you were just staying the night.</t>
+  </si>
+  <si>
+    <t>I'm a man of my word. It was nice getting to briefly meet you folks, but it's time for me to hit the road... My son's out there somewhere.</t>
+  </si>
+  <si>
+    <t>Is there anything we can give you to help you out?</t>
+  </si>
+  <si>
+    <t>I'm not sure... I've got food, water, clothes on my back and a good pair of mitts.</t>
+  </si>
+  <si>
+    <t>!HasShotgun</t>
+  </si>
+  <si>
+    <t>Nothing for Dad</t>
+  </si>
+  <si>
+    <t>Sorry, but I don't think there's anything else we can do for you.</t>
+  </si>
+  <si>
+    <t>Offer Shotgun</t>
+  </si>
+  <si>
+    <t>Send him on his way</t>
+  </si>
+  <si>
+    <t>Give Dad shotgun</t>
+  </si>
+  <si>
+    <t>Offer Dad shotgun</t>
+  </si>
+  <si>
+    <t>That's alright, just spending the night is nice enough.</t>
+  </si>
+  <si>
+    <t>Dad leaves</t>
+  </si>
+  <si>
+    <t>It would certainly help me out.</t>
+  </si>
+  <si>
+    <t>Bob &amp;&amp; !Jessica</t>
+  </si>
+  <si>
+    <t>(to you) Don't give him our gun. He's only been here for a night and he could still be dangerous.</t>
+  </si>
+  <si>
+    <t>Bob &amp;&amp; Jessica</t>
+  </si>
+  <si>
+    <t>(to you) Be careful with him...</t>
+  </si>
+  <si>
+    <t>(to you) Give it to him, he can use it a lot more than we can.</t>
+  </si>
+  <si>
+    <t>*ask him some more questions before you give him the gun*</t>
+  </si>
+  <si>
+    <t>Dad questions</t>
+  </si>
+  <si>
+    <t>"Will you bring the gun back to us?"</t>
+  </si>
+  <si>
+    <t>"Do you really think this would help you out?"</t>
+  </si>
+  <si>
+    <t>Give Shotgun</t>
+  </si>
+  <si>
+    <t>Keep Shotgun</t>
+  </si>
+  <si>
+    <t>Keep shotgun</t>
+  </si>
+  <si>
+    <t>Will shotgun help Dad</t>
+  </si>
+  <si>
+    <t>Will Dad bring shotgun back</t>
+  </si>
+  <si>
+    <t>I'm not sure if you would be seeing it again. I don't plan on coming back, but who knows what way the wind blows.</t>
+  </si>
+  <si>
+    <t>Yes, my son might be somewhere dangerous.</t>
+  </si>
+  <si>
+    <t>b_6_sigh</t>
+  </si>
+  <si>
+    <t>Thank you... I will remember this.</t>
+  </si>
+  <si>
+    <t>I think we should keep the shotgun.</t>
+  </si>
+  <si>
+    <t>I understand. You have to keep yourself safe too.</t>
+  </si>
+  <si>
+    <t>Regardless, thanks for the hospitality. Stay safe!</t>
+  </si>
+  <si>
+    <t>Bye! Hope you can find your son!</t>
+  </si>
+  <si>
+    <t>Good luck.</t>
+  </si>
+  <si>
+    <t>(to you) *i don't think he'll find his son*</t>
+  </si>
+  <si>
+    <t>dad_6_wake_up</t>
+  </si>
+  <si>
+    <t>b_6_d_you_gotta_leave</t>
+  </si>
+  <si>
+    <t>dad_6_i_will_leave</t>
+  </si>
+  <si>
+    <t>j_6_d_anything_to_give</t>
+  </si>
+  <si>
+    <t>dad_6_dont_need_anything</t>
+  </si>
+  <si>
+    <t>p_6_d_offer_shotgun</t>
+  </si>
+  <si>
+    <t>p_6_d_send_dad_along</t>
+  </si>
+  <si>
+    <t>p_6_d_nothing_else</t>
+  </si>
+  <si>
+    <t>dad_6_nothing_is_alright</t>
+  </si>
+  <si>
+    <t>dad_6_shotgun_would_help</t>
+  </si>
+  <si>
+    <t>b_6_d_be_cautious</t>
+  </si>
+  <si>
+    <t>b_6_d_dont_give_gun</t>
+  </si>
+  <si>
+    <t>j_6_d_give_gun</t>
+  </si>
+  <si>
+    <t>v_6_d_ask_questions_before</t>
+  </si>
+  <si>
+    <t>p_6_d_will_you_bring_back</t>
+  </si>
+  <si>
+    <t>p_6_d_will_gun_help</t>
+  </si>
+  <si>
+    <t>p_6_d_give_shotgun</t>
+  </si>
+  <si>
+    <t>p_6_d_keep_shotgun</t>
+  </si>
+  <si>
+    <t>dad_6_p_wont_bring_back</t>
+  </si>
+  <si>
+    <t>dad_6_p_son_maybe_danger</t>
+  </si>
+  <si>
+    <t>dad_6_thanks_for_gun</t>
+  </si>
+  <si>
+    <t>p_6_d_we_should_keep_gun</t>
+  </si>
+  <si>
+    <t>dad_6_understand</t>
+  </si>
+  <si>
+    <t>dad_6_goodbye</t>
+  </si>
+  <si>
+    <t>j_6_d_goodbye</t>
+  </si>
+  <si>
+    <t>b_6_d_goodbye</t>
+  </si>
+  <si>
+    <t>v_6_d_goodbye</t>
   </si>
 </sst>
 </file>
@@ -4289,10 +4553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H1237"/>
+  <dimension ref="A1:H1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A985" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C998" sqref="C998"/>
+    <sheetView tabSelected="1" topLeftCell="A1347" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1371" sqref="E1371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16229,525 +16493,1794 @@
         <v>135</v>
       </c>
     </row>
-    <row r="1185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1185" t="s">
+    <row r="1239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1239" t="s">
         <v>99</v>
       </c>
-      <c r="B1185" t="s">
+      <c r="B1239" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="1190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1190" t="s">
+    <row r="1240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1240" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>661</v>
+      </c>
+      <c r="D1240">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1241" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D1241">
+        <v>6</v>
+      </c>
+      <c r="E1241" t="s">
+        <v>1095</v>
+      </c>
+      <c r="F1241" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1241" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1242" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1245" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>663</v>
+      </c>
+      <c r="D1245">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1246" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D1246">
+        <v>6</v>
+      </c>
+      <c r="E1246" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F1246" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1246" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1247" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1249" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>664</v>
+      </c>
+      <c r="D1249">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1250" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1250">
+        <v>6</v>
+      </c>
+      <c r="E1250" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F1250" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1250" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1251" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1253" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>665</v>
+      </c>
+      <c r="D1253">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1254" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D1254">
+        <v>6</v>
+      </c>
+      <c r="E1254" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F1254" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1254" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1255" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1260" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D1260">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1261" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D1261">
+        <v>6</v>
+      </c>
+      <c r="E1261" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F1261" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1261" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1262" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D1262">
+        <v>6</v>
+      </c>
+      <c r="E1262" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F1262" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1262" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1263" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D1263">
+        <v>6</v>
+      </c>
+      <c r="E1263" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F1263" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1263" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1264" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1266" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1266">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1267" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1267">
+        <v>6</v>
+      </c>
+      <c r="E1267" t="s">
+        <v>1107</v>
+      </c>
+      <c r="F1267" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1267" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1268" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1269" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D1269">
+        <v>6</v>
+      </c>
+      <c r="E1269" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F1269" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1269" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1270" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1271" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D1271">
+        <v>6</v>
+      </c>
+      <c r="E1271" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F1271" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1271" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1272" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1273" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1275" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1276" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D1276">
+        <v>6</v>
+      </c>
+      <c r="E1276" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F1276" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1276" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1277" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1279" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D1279">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1280" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D1280">
+        <v>6</v>
+      </c>
+      <c r="E1280" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F1280" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1280" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1281" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1282" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D1282">
+        <v>6</v>
+      </c>
+      <c r="E1282" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F1282" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1282" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1283" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1284" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D1284">
+        <v>6</v>
+      </c>
+      <c r="E1284" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F1284" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1284" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1285" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1286" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D1286">
+        <v>6</v>
+      </c>
+      <c r="E1286" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F1286" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1286" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1287" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D1287">
+        <v>6</v>
+      </c>
+      <c r="E1287" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F1287" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1287" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1288" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1289" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1290" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1290" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1291" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1292" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1293" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D1293">
+        <v>6</v>
+      </c>
+      <c r="E1293" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F1293" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1293" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1294" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1295" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D1295">
+        <v>6</v>
+      </c>
+      <c r="E1295" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F1295" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1295" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1296" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1299" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1299">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1300" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D1300">
+        <v>6</v>
+      </c>
+      <c r="E1300" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F1300" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1300" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1301" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D1301">
+        <v>6</v>
+      </c>
+      <c r="E1301" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F1301" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1301" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1302" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1302" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1303" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1305" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1305" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D1305">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1306" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1306" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D1306">
+        <v>6</v>
+      </c>
+      <c r="E1306" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F1306" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1306" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1307" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1307" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1308" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1308" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1308">
+        <v>6</v>
+      </c>
+      <c r="E1308" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F1308" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1308" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1309" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1309" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1310" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1310" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D1310">
+        <v>6</v>
+      </c>
+      <c r="E1310" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F1310" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1310" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1311" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1312" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1313" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1313" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D1313">
+        <v>6</v>
+      </c>
+      <c r="E1313" t="s">
+        <v>1165</v>
+      </c>
+      <c r="F1313" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1313" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1314" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1315" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1315" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1316" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1316" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D1316">
+        <v>6</v>
+      </c>
+      <c r="E1316" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F1316" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1316" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1317" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1318" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1318" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1319" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1322" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1322" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D1322">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1323" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1323" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1324" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1324" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D1324">
+        <v>6</v>
+      </c>
+      <c r="E1324" t="s">
+        <v>1167</v>
+      </c>
+      <c r="F1324" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1324" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1325" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1325" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1326" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1326" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D1326">
+        <v>6</v>
+      </c>
+      <c r="E1326" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F1326" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1326" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1327" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1327" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1328" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1328" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D1328">
+        <v>6</v>
+      </c>
+      <c r="E1328" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F1328" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1328" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1329" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1329" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1330" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1330" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D1330">
+        <v>6</v>
+      </c>
+      <c r="E1330" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F1330" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1330" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1331" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1333" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1333" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D1333">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1334" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1334" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D1334">
+        <v>6</v>
+      </c>
+      <c r="E1334" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F1334" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1334" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1335" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1335" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1336" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1338" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1338" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1338">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1339" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1339" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D1339">
+        <v>6</v>
+      </c>
+      <c r="E1339" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F1339" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1339" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1340" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1340" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1341" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1343" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1343" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D1343">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1344" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1344" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1345" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1345" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D1345">
+        <v>6</v>
+      </c>
+      <c r="E1345" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F1345" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1345" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1346" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1347" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1347" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D1347">
+        <v>6</v>
+      </c>
+      <c r="E1347" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F1347" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1347" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1348" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1348" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1349" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1351" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1351" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D1351">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1352" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1352" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D1352">
+        <v>6</v>
+      </c>
+      <c r="E1352" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F1352" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1352" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1353" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1353" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D1353">
+        <v>6</v>
+      </c>
+      <c r="E1353" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F1353" t="s">
+        <v>647</v>
+      </c>
+      <c r="G1353" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1354" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1354" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1355" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1361" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1361" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1361">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1362" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1362" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D1362">
+        <v>6</v>
+      </c>
+      <c r="E1362" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1363" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1363" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1364" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1364" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D1364">
+        <v>6</v>
+      </c>
+      <c r="E1364" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1365" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1366" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1366" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1367" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1367" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D1367">
+        <v>6</v>
+      </c>
+      <c r="E1367" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1368" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1369" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1369" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1370" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1370" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D1370">
+        <v>6</v>
+      </c>
+      <c r="E1370" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1371" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1372" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1562" t="s">
         <v>99</v>
       </c>
-      <c r="B1190" t="s">
+      <c r="B1562" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="1191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1191" t="s">
+    <row r="1563" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1563" t="s">
         <v>99</v>
       </c>
-      <c r="B1191" t="s">
+      <c r="B1563" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="1192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1192" t="s">
+    <row r="1564" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1564" t="s">
         <v>133</v>
       </c>
-      <c r="B1192" t="s">
+      <c r="B1564" t="s">
         <v>661</v>
       </c>
-      <c r="D1192">
+      <c r="D1564">
         <v>7</v>
       </c>
     </row>
-    <row r="1193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1193" t="s">
+    <row r="1565" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1565" t="s">
         <v>154</v>
       </c>
-      <c r="B1193" t="s">
+      <c r="B1565" t="s">
         <v>662</v>
       </c>
-      <c r="D1193">
+      <c r="D1565">
         <v>7</v>
       </c>
-      <c r="E1193" t="s">
+      <c r="E1565" t="s">
         <v>670</v>
       </c>
-      <c r="F1193" t="s">
+      <c r="F1565" t="s">
         <v>647</v>
       </c>
-      <c r="G1193" t="s">
+      <c r="G1565" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1194" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1194" t="s">
+    <row r="1566" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1566" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1197" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1197" t="s">
+    <row r="1569" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1569" t="s">
         <v>133</v>
       </c>
-      <c r="B1197" t="s">
+      <c r="B1569" t="s">
         <v>663</v>
       </c>
-      <c r="D1197">
+      <c r="D1569">
         <v>7</v>
       </c>
     </row>
-    <row r="1198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1198" t="s">
+    <row r="1570" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1570" t="s">
         <v>145</v>
       </c>
-      <c r="B1198" t="s">
+      <c r="B1570" t="s">
         <v>667</v>
       </c>
-      <c r="D1198">
+      <c r="D1570">
         <v>7</v>
       </c>
-      <c r="E1198" t="s">
+      <c r="E1570" t="s">
         <v>669</v>
       </c>
-      <c r="F1198" t="s">
+      <c r="F1570" t="s">
         <v>647</v>
       </c>
-      <c r="G1198" t="s">
+      <c r="G1570" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1199" t="s">
+    <row r="1571" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1571" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1201" t="s">
+    <row r="1573" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1573" t="s">
         <v>133</v>
       </c>
-      <c r="B1201" t="s">
+      <c r="B1573" t="s">
         <v>664</v>
       </c>
-      <c r="D1201">
+      <c r="D1573">
         <v>7</v>
       </c>
     </row>
-    <row r="1202" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1202" t="s">
+    <row r="1574" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1574" t="s">
         <v>11</v>
       </c>
-      <c r="B1202" t="s">
+      <c r="B1574" t="s">
         <v>668</v>
       </c>
-      <c r="D1202">
+      <c r="D1574">
         <v>7</v>
       </c>
-      <c r="E1202" t="s">
+      <c r="E1574" t="s">
         <v>671</v>
       </c>
-      <c r="F1202" t="s">
+      <c r="F1574" t="s">
         <v>647</v>
       </c>
-      <c r="G1202" t="s">
+      <c r="G1574" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1203" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1203" t="s">
+    <row r="1575" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1575" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1205" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1205" t="s">
+    <row r="1577" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1577" t="s">
         <v>133</v>
       </c>
-      <c r="B1205" t="s">
+      <c r="B1577" t="s">
         <v>665</v>
       </c>
-      <c r="D1205">
+      <c r="D1577">
         <v>7</v>
       </c>
     </row>
-    <row r="1206" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1206" t="s">
+    <row r="1578" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1578" t="s">
         <v>11</v>
       </c>
-      <c r="B1206" t="s">
+      <c r="B1578" t="s">
         <v>666</v>
       </c>
-      <c r="D1206">
+      <c r="D1578">
         <v>7</v>
       </c>
-      <c r="E1206" t="s">
+      <c r="E1578" t="s">
         <v>672</v>
       </c>
-      <c r="F1206" t="s">
+      <c r="F1578" t="s">
         <v>647</v>
       </c>
-      <c r="G1206" t="s">
+      <c r="G1578" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1207" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1207" t="s">
+    <row r="1579" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1579" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1210" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1210" t="s">
+    <row r="1582" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1582" t="s">
         <v>99</v>
       </c>
-      <c r="B1210" t="s">
+      <c r="B1582" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="1211" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1211" t="s">
+    <row r="1583" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1583" t="s">
         <v>133</v>
       </c>
-      <c r="B1211" t="s">
+      <c r="B1583" t="s">
         <v>685</v>
       </c>
-      <c r="D1211">
+      <c r="D1583">
         <v>7</v>
       </c>
     </row>
-    <row r="1212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1212" t="s">
+    <row r="1584" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1584" t="s">
         <v>11</v>
       </c>
-      <c r="B1212" t="s">
+      <c r="B1584" t="s">
         <v>673</v>
       </c>
-      <c r="D1212">
+      <c r="D1584">
         <v>7</v>
       </c>
-      <c r="E1212" t="s">
+      <c r="E1584" t="s">
         <v>674</v>
       </c>
-      <c r="F1212" t="s">
+      <c r="F1584" t="s">
         <v>647</v>
       </c>
-      <c r="G1212" t="s">
+      <c r="G1584" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1213" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1213" t="s">
+    <row r="1585" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1585" t="s">
         <v>460</v>
       </c>
-      <c r="B1213" t="s">
+      <c r="B1585" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="1214" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1214" t="s">
+    <row r="1586" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1586" t="s">
         <v>67</v>
       </c>
-      <c r="B1214" t="s">
+      <c r="B1586" t="s">
         <v>675</v>
       </c>
-      <c r="D1214">
+      <c r="D1586">
         <v>7</v>
       </c>
-      <c r="E1214" t="s">
+      <c r="E1586" t="s">
         <v>676</v>
       </c>
-      <c r="F1214" t="s">
+      <c r="F1586" t="s">
         <v>647</v>
       </c>
-      <c r="G1214" t="s">
+      <c r="G1586" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1215" t="s">
+    <row r="1587" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1587" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1216" t="s">
+    <row r="1588" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1588" t="s">
         <v>460</v>
       </c>
-      <c r="B1216" t="s">
+      <c r="B1588" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="1217" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1217" t="s">
+    <row r="1589" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1589" t="s">
         <v>66</v>
       </c>
-      <c r="B1217" t="s">
+      <c r="B1589" t="s">
         <v>677</v>
       </c>
-      <c r="C1217" t="s">
+      <c r="C1589" t="s">
         <v>678</v>
       </c>
-      <c r="D1217">
+      <c r="D1589">
         <v>7</v>
       </c>
-      <c r="E1217" t="s">
+      <c r="E1589" t="s">
         <v>687</v>
       </c>
-      <c r="F1217" t="s">
+      <c r="F1589" t="s">
         <v>647</v>
       </c>
-      <c r="G1217" t="s">
+      <c r="G1589" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1218" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1218" t="s">
+    <row r="1590" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1590" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="1219" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1219" t="s">
+    <row r="1591" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1591" t="s">
         <v>66</v>
       </c>
-      <c r="B1219" t="s">
+      <c r="B1591" t="s">
         <v>679</v>
       </c>
-      <c r="D1219">
+      <c r="D1591">
         <v>7</v>
       </c>
-      <c r="E1219" t="s">
+      <c r="E1591" t="s">
         <v>688</v>
       </c>
-      <c r="F1219" t="s">
+      <c r="F1591" t="s">
         <v>647</v>
       </c>
-      <c r="G1219" t="s">
+      <c r="G1591" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1220" t="s">
+    <row r="1592" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1592" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1221" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1221" t="s">
+    <row r="1593" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1593" t="s">
         <v>460</v>
       </c>
-      <c r="B1221" t="s">
+      <c r="B1593" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="1222" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1222" t="s">
+    <row r="1594" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1594" t="s">
         <v>68</v>
       </c>
-      <c r="B1222" t="s">
+      <c r="B1594" t="s">
         <v>681</v>
       </c>
-      <c r="D1222">
+      <c r="D1594">
         <v>7</v>
       </c>
-      <c r="E1222" t="s">
+      <c r="E1594" t="s">
         <v>682</v>
       </c>
-      <c r="F1222" t="s">
+      <c r="F1594" t="s">
         <v>647</v>
       </c>
-      <c r="G1222" t="s">
+      <c r="G1594" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1223" t="s">
+    <row r="1595" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1595" t="s">
         <v>643</v>
       </c>
-      <c r="B1223" t="s">
+      <c r="B1595" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="1224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1224" t="s">
+    <row r="1596" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1596" t="s">
         <v>68</v>
       </c>
-      <c r="B1224" t="s">
+      <c r="B1596" t="s">
         <v>683</v>
       </c>
-      <c r="D1224">
+      <c r="D1596">
         <v>7</v>
       </c>
-      <c r="E1224" t="s">
+      <c r="E1596" t="s">
         <v>684</v>
       </c>
-      <c r="F1224" t="s">
+      <c r="F1596" t="s">
         <v>647</v>
       </c>
-      <c r="G1224" t="s">
+      <c r="G1596" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1225" t="s">
+    <row r="1597" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1597" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1226" t="s">
+    <row r="1598" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1598" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1228" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1228" t="s">
+    <row r="1600" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1600" t="s">
         <v>133</v>
       </c>
-      <c r="B1228" t="s">
+      <c r="B1600" t="s">
         <v>689</v>
       </c>
-      <c r="D1228">
+      <c r="D1600">
         <v>7</v>
       </c>
     </row>
-    <row r="1229" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1229" t="s">
+    <row r="1601" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1601" t="s">
         <v>70</v>
       </c>
-      <c r="B1229" t="s">
+      <c r="B1601" t="s">
         <v>690</v>
       </c>
-      <c r="D1229">
+      <c r="D1601">
         <v>7</v>
       </c>
-      <c r="E1229" t="s">
+      <c r="E1601" t="s">
         <v>696</v>
       </c>
-      <c r="F1229" t="s">
+      <c r="F1601" t="s">
         <v>647</v>
       </c>
-      <c r="G1229" t="s">
+      <c r="G1601" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1230" t="s">
+    <row r="1602" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1602" t="s">
         <v>69</v>
       </c>
-      <c r="B1230" t="s">
+      <c r="B1602" t="s">
         <v>693</v>
       </c>
-      <c r="D1230">
+      <c r="D1602">
         <v>7</v>
       </c>
-      <c r="E1230" t="s">
+      <c r="E1602" t="s">
         <v>697</v>
       </c>
-      <c r="F1230" t="s">
+      <c r="F1602" t="s">
         <v>647</v>
       </c>
-      <c r="G1230" t="s">
+      <c r="G1602" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1231" t="s">
+    <row r="1603" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1603" t="s">
         <v>70</v>
       </c>
-      <c r="B1231" t="s">
+      <c r="B1603" t="s">
         <v>694</v>
       </c>
-      <c r="D1231">
+      <c r="D1603">
         <v>7</v>
       </c>
-      <c r="E1231" t="s">
+      <c r="E1603" t="s">
         <v>698</v>
       </c>
-      <c r="F1231" t="s">
+      <c r="F1603" t="s">
         <v>647</v>
       </c>
-      <c r="G1231" t="s">
+      <c r="G1603" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1232" t="s">
+    <row r="1604" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1604" t="s">
         <v>69</v>
       </c>
-      <c r="B1232" t="s">
+      <c r="B1604" t="s">
         <v>695</v>
       </c>
-      <c r="D1232">
+      <c r="D1604">
         <v>7</v>
       </c>
-      <c r="E1232" t="s">
+      <c r="E1604" t="s">
         <v>699</v>
       </c>
-      <c r="F1232" t="s">
+      <c r="F1604" t="s">
         <v>647</v>
       </c>
-      <c r="G1232" t="s">
+      <c r="G1604" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1233" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1233" t="s">
+    <row r="1605" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1605" t="s">
         <v>460</v>
       </c>
-      <c r="B1233" t="s">
+      <c r="B1605" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="1234" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1234" t="s">
+    <row r="1606" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1606" t="s">
         <v>67</v>
       </c>
-      <c r="B1234" t="s">
+      <c r="B1606" t="s">
         <v>692</v>
       </c>
-      <c r="D1234">
+      <c r="D1606">
         <v>7</v>
       </c>
-      <c r="E1234" t="s">
+      <c r="E1606" t="s">
         <v>700</v>
       </c>
-      <c r="F1234" t="s">
+      <c r="F1606" t="s">
         <v>647</v>
       </c>
-      <c r="G1234" t="s">
+      <c r="G1606" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1235" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1235" t="s">
+    <row r="1607" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1607" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1236" t="s">
+    <row r="1608" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1608" t="s">
         <v>11</v>
       </c>
-      <c r="B1236" t="s">
+      <c r="B1608" t="s">
         <v>691</v>
       </c>
-      <c r="D1236">
+      <c r="D1608">
         <v>7</v>
       </c>
-      <c r="E1236" t="s">
+      <c r="E1608" t="s">
         <v>701</v>
       </c>
-      <c r="F1236" t="s">
+      <c r="F1608" t="s">
         <v>647</v>
       </c>
-      <c r="G1236" t="s">
+      <c r="G1608" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="1237" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1237" t="s">
+    <row r="1609" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1609" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1048576">
+  <conditionalFormatting sqref="A1:H1260 A1264:H1266 A1261:A1263 C1261:H1263 A1267 C1267:H1267 A1268:H1279 A1281:H1281 A1280 A1283:H1283 A1282 A1285:H1285 A1284 A1286:A1287 A1306 A1325:H1325 A1324:A1326 A1339 A1347 A1348:H1351 A1352:A1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1365:H1366 A1364 C1364:H1364 A1367 C1280:H1280 C1282:H1282 C1284:H1284 C1286:H1287 A1288:H1305 C1306:H1306 C1324:H1324 C1326:H1326 A1327:H1338 C1339:H1339 A1340:H1346 C1347:H1347 C1352:H1353 A1307:H1323 C1367:H1367 A1368:H1048576">
     <cfRule type="expression" dxfId="27" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
@@ -16951,6 +18484,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -17189,24 +18739,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17223,29 +18781,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New var - OnePartyMember
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057F9F7B-B35A-41D9-97C5-84129EC932A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5116462E-BC4E-49AD-8246-9703B6640366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3188" uniqueCount="1186">
   <si>
     <t>Context</t>
   </si>
@@ -3577,6 +3577,24 @@
   </si>
   <si>
     <t>v_6_d_goodbye</t>
+  </si>
+  <si>
+    <t>Enter scavenging</t>
+  </si>
+  <si>
+    <t>The weather's clearing up a bit, and we could use some more food. Who wants to go out?</t>
+  </si>
+  <si>
+    <t>Before scavenge choice Jessica</t>
+  </si>
+  <si>
+    <t>!Bob &amp;&amp; !Violet</t>
+  </si>
+  <si>
+    <t>The weather's clearing up a bit, and we could use some more food. Do you want to go out?</t>
+  </si>
+  <si>
+    <t>OnePartyMember</t>
   </si>
 </sst>
 </file>
@@ -3634,46 +3652,526 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="48">
     <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -4235,6 +4733,46 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4555,8 +5093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1347" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1371" sqref="E1371"/>
+    <sheetView tabSelected="1" topLeftCell="A1374" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1385" sqref="C1385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,49 +7535,40 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>135</v>
+        <v>1049</v>
+      </c>
+      <c r="B222" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>133</v>
-      </c>
-      <c r="B223" t="s">
-        <v>318</v>
-      </c>
-      <c r="D223">
-        <v>1</v>
+        <v>135</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="B224" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="D224">
         <v>1</v>
       </c>
-      <c r="E224" t="s">
-        <v>311</v>
-      </c>
-      <c r="F224" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B225" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D225">
         <v>1</v>
       </c>
       <c r="E225" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F225" t="s">
         <v>2</v>
@@ -7050,13 +7579,13 @@
         <v>66</v>
       </c>
       <c r="B226" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D226">
         <v>1</v>
       </c>
       <c r="E226" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F226" t="s">
         <v>2</v>
@@ -7064,16 +7593,16 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B227" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D227">
         <v>1</v>
       </c>
       <c r="E227" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F227" t="s">
         <v>2</v>
@@ -7081,16 +7610,16 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B228" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D228">
         <v>1</v>
       </c>
       <c r="E228" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F228" t="s">
         <v>2</v>
@@ -7098,16 +7627,16 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B229" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D229">
         <v>1</v>
       </c>
       <c r="E229" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F229" t="s">
         <v>2</v>
@@ -7115,16 +7644,16 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B230" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D230">
         <v>1</v>
       </c>
       <c r="E230" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F230" t="s">
         <v>2</v>
@@ -7132,35 +7661,43 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>135</v>
+        <v>66</v>
+      </c>
+      <c r="B231" t="s">
+        <v>310</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+      <c r="E231" t="s">
+        <v>317</v>
+      </c>
+      <c r="F231" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B232" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>133</v>
-      </c>
-      <c r="B233" t="s">
-        <v>319</v>
-      </c>
-      <c r="D233">
-        <v>1</v>
+        <v>135</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="B234" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D234">
         <v>1</v>
-      </c>
-      <c r="E234" t="s">
-        <v>325</v>
-      </c>
-      <c r="F234" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
@@ -7168,13 +7705,13 @@
         <v>11</v>
       </c>
       <c r="B235" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D235">
         <v>1</v>
       </c>
       <c r="E235" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F235" t="s">
         <v>2</v>
@@ -7182,16 +7719,16 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B236" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D236">
         <v>1</v>
       </c>
       <c r="E236" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F236" t="s">
         <v>2</v>
@@ -7199,16 +7736,16 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B237" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D237">
         <v>1</v>
       </c>
       <c r="E237" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F237" t="s">
         <v>2</v>
@@ -7216,16 +7753,16 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B238" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D238">
         <v>1</v>
       </c>
       <c r="E238" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F238" t="s">
         <v>2</v>
@@ -7233,16 +7770,16 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B239" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D239">
         <v>1</v>
       </c>
       <c r="E239" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F239" t="s">
         <v>2</v>
@@ -7250,9 +7787,26 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
+        <v>11</v>
+      </c>
+      <c r="B240" t="s">
+        <v>323</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+      <c r="E240" t="s">
+        <v>330</v>
+      </c>
+      <c r="F240" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
         <v>135</v>
       </c>
-      <c r="D240">
+      <c r="D241">
         <v>2</v>
       </c>
     </row>
@@ -17770,6 +18324,72 @@
         <v>135</v>
       </c>
     </row>
+    <row r="1384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1384" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1384" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D1384">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1385" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1385" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1386" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1387" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1388" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1388" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1389" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1390" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1392" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1393" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>1183</v>
+      </c>
+    </row>
     <row r="1562" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1562" t="s">
         <v>99</v>
@@ -18280,50 +18900,114 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1260 A1264:H1266 A1261:A1263 C1261:H1263 A1267 C1267:H1267 A1268:H1279 A1281:H1281 A1280 A1283:H1283 A1282 A1285:H1285 A1284 A1286:A1287 A1306 A1325:H1325 A1324:A1326 A1339 A1347 A1348:H1351 A1352:A1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1365:H1366 A1364 C1364:H1364 A1367 C1280:H1280 C1282:H1282 C1284:H1284 C1286:H1287 A1288:H1305 C1306:H1306 C1324:H1324 C1326:H1326 A1327:H1338 C1339:H1339 A1340:H1346 C1347:H1347 C1352:H1353 A1307:H1323 C1367:H1367 A1368:H1048576">
-    <cfRule type="expression" dxfId="27" priority="1">
+  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1368:H1384 A1386 A1387:H1387 A1389:H1048576 C1388:H1388 A1388">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="47" priority="10" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="46" priority="11" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="45" priority="12" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1385:H1385">
+    <cfRule type="expression" dxfId="29" priority="37">
+      <formula>LEFT($A1386, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="38">
+      <formula>$A1386="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="39">
+      <formula>$A1386="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="40">
+      <formula>$A1386="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="41">
+      <formula>$A1386="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="42">
+      <formula>$A1386="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="43">
+      <formula>$A1386="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="44">
+      <formula>$A1386="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="45">
+      <formula>$A1386="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="46">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1386:H1386">
+    <cfRule type="expression" dxfId="19" priority="57">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="58">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="59">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="60">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="61">
+      <formula>#REF!="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="62">
+      <formula>#REF!="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="63">
+      <formula>#REF!="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="64">
+      <formula>#REF!="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="65">
+      <formula>#REF!="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="66">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18434,48 +19118,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="43" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="42" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="41" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="40" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="39" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="38" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="37" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="36" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="35" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="26">
+    <cfRule type="expression" dxfId="34" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18484,23 +19168,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -18739,32 +19406,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18781,4 +19440,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Progress on Jessica scavenging
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5116462E-BC4E-49AD-8246-9703B6640366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7E6AFC-05A5-49D6-BE17-2405E565ADC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3188" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3282" uniqueCount="1214">
   <si>
     <t>Context</t>
   </si>
@@ -3588,13 +3588,97 @@
     <t>Before scavenge choice Jessica</t>
   </si>
   <si>
-    <t>!Bob &amp;&amp; !Violet</t>
-  </si>
-  <si>
     <t>The weather's clearing up a bit, and we could use some more food. Do you want to go out?</t>
   </si>
   <si>
     <t>OnePartyMember</t>
+  </si>
+  <si>
+    <t>I don't think so, even if it's a bit nicer out there I don't think it's a good idea for me to go. I think we also have enough food already, it's just two of us.</t>
+  </si>
+  <si>
+    <t>I don't think anyone should go. The weather looks better outside and we have lots of food left.</t>
+  </si>
+  <si>
+    <t>Added to scavenge party Jessica</t>
+  </si>
+  <si>
+    <t>Are you sure? It's scary out there!</t>
+  </si>
+  <si>
+    <t>TODO: Add some Ifs here to spice it up</t>
+  </si>
+  <si>
+    <t>Do I really have to?</t>
+  </si>
+  <si>
+    <t>Yes, what if the storm comes back and we are stuck inside?</t>
+  </si>
+  <si>
+    <t>Alright... Can I at least take that firearm? Maybe I could trade it with someone...</t>
+  </si>
+  <si>
+    <t>Sure, it could help you stay safe</t>
+  </si>
+  <si>
+    <t>I'd rather keep it here to defend the cabin</t>
+  </si>
+  <si>
+    <t>Send Jessica with shotgun</t>
+  </si>
+  <si>
+    <t>Thank you, I hope I won't need it for anything.</t>
+  </si>
+  <si>
+    <t>Tell Jessica her idea is stupid</t>
+  </si>
+  <si>
+    <t>That sounds stupid</t>
+  </si>
+  <si>
+    <t>I'm just scared, okay...</t>
+  </si>
+  <si>
+    <t>Send Jessica without shotgun</t>
+  </si>
+  <si>
+    <t>Okay, I understand.</t>
+  </si>
+  <si>
+    <t>Jessica died while scavenging</t>
+  </si>
+  <si>
+    <t>It's been too long, I don't think she made it.</t>
+  </si>
+  <si>
+    <t>*i think she's probably dead out there. unfortunate but unsurprising*</t>
+  </si>
+  <si>
+    <t>It's been a bit too long... I don't think she's coming back.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I don't think it's a good idea for me to go. I think we also have enough food already.</t>
+  </si>
+  <si>
+    <t>I'll go.</t>
+  </si>
+  <si>
+    <t>Moron trying to argue against scavenging</t>
+  </si>
+  <si>
+    <t>The player just asked who wants to go out</t>
+  </si>
+  <si>
+    <t>*it could get worse, ill go*</t>
+  </si>
+  <si>
+    <t>Violet &amp;&amp; !HasCar</t>
+  </si>
+  <si>
+    <t>*i want to go to the gas station, there could be a car for us there*</t>
+  </si>
+  <si>
+    <t>Violet &amp;&amp; !HasCar &amp;&amp; Jessica</t>
   </si>
 </sst>
 </file>
@@ -5093,8 +5177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1374" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1385" sqref="C1385"/>
+    <sheetView tabSelected="1" topLeftCell="A1385" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1404" sqref="B1404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18340,7 +18424,7 @@
         <v>460</v>
       </c>
       <c r="B1385" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1386" spans="1:4" x14ac:dyDescent="0.25">
@@ -18348,7 +18432,7 @@
         <v>11</v>
       </c>
       <c r="B1386" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1387" spans="1:4" x14ac:dyDescent="0.25">
@@ -18366,28 +18450,421 @@
     </row>
     <row r="1389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1389" t="s">
-        <v>644</v>
+        <v>1049</v>
+      </c>
+      <c r="B1389" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="1390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1390" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1391" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1392" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1392" t="s">
+    <row r="1393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1393" t="s">
         <v>133</v>
       </c>
-      <c r="B1392" t="s">
+      <c r="B1393" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D1393">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1394" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1394" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1395" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1396" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1397" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1398" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1399" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1400" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1400" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1401" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1402" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1411" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1423" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1423" t="s">
         <v>1182</v>
       </c>
     </row>
-    <row r="1393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1393" t="s">
+    <row r="1424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1424" t="s">
         <v>460</v>
       </c>
-      <c r="B1393" t="s">
-        <v>1183</v>
+      <c r="B1424" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1425" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1425" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1426" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1427" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1427" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1428" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1429" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1431" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1431" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1432" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1432" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1433" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1433" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1434" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1438" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1438" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1439" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1439" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1440" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1440" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1441" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1441" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1442" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1442" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1443" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1443" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1444" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1444" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1445" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1445" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1446" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1446" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1447" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1447" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1448" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1450" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1450" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1451" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1451" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1452" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1452" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1453" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1455" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1455" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1456" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1456" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1457" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1457" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1458" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1460" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1460" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1461" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1461" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1462" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1462" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1463" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1466" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1466" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1467" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1467" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1468" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1468" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1469" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1469" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1470" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1470" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1471" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1472" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1472" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1473" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1474" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="1562" spans="1:7" x14ac:dyDescent="0.25">
@@ -18900,7 +19377,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1368:H1384 A1386 A1387:H1387 A1389:H1048576 C1388:H1388 A1388">
+  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1368:H1384 A1386 A1387:H1387 C1388:H1388 A1388 A1401 C1401:H1401 A1409:A1410 C1409:H1410 A1414 C1414:H1414 C1416:H1416 A1416 A1417:H1419 A1420 C1420:H1420 A1440:B1440 A1415:H1415 A1426:H1426 A1425 A1428:H1431 A1426:B1427 C1424:H1427 A1431:B1432 C1429:H1432 A1433:H1439 A1439:A1441 C1437:H1441 A1442:H1048576 A1421:H1424 A1402:H1408 A1389:H1398 A1400:H1400 A1399 C1399:H1399 A1411:H1413">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Jessica scavenge lines complete
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7E6AFC-05A5-49D6-BE17-2405E565ADC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA3F758-BCB2-435F-AC97-F669E662FC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3282" uniqueCount="1214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="1219">
   <si>
     <t>Context</t>
   </si>
@@ -3679,6 +3679,21 @@
   </si>
   <si>
     <t>Violet &amp;&amp; !HasCar &amp;&amp; Jessica</t>
+  </si>
+  <si>
+    <t>I guess we wouldn't be taking other people's food, but what if that is someone's car?</t>
+  </si>
+  <si>
+    <t>*this is war it's not fair for everyone*</t>
+  </si>
+  <si>
+    <t>That's exactly why we should go. The weather being clear means that we can check farther out for more food. What if the weather goes bad and we are snowed in?</t>
+  </si>
+  <si>
+    <t>We need it. I'll go out.</t>
+  </si>
+  <si>
+    <t>I don't know why you are always so negative. Can't we just eat a bit less and leave some food for people who need it?</t>
   </si>
 </sst>
 </file>
@@ -5177,8 +5192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1385" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1404" sqref="B1404"/>
+    <sheetView tabSelected="1" topLeftCell="A1388" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1402" sqref="E1402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18511,49 +18526,110 @@
         <v>460</v>
       </c>
       <c r="B1398" t="s">
-        <v>680</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1399" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1399" t="s">
-        <v>1210</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1400" t="s">
-        <v>643</v>
+        <v>67</v>
       </c>
       <c r="B1400" t="s">
-        <v>1211</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1401" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1401" t="s">
-        <v>1212</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1402" t="s">
-        <v>644</v>
+        <v>67</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>1217</v>
       </c>
     </row>
     <row r="1403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1403" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1404" t="s">
         <v>460</v>
       </c>
-      <c r="B1403" t="s">
+      <c r="B1404" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1405" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1406" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1407" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1408" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1409" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1409" t="s">
         <v>1213</v>
       </c>
     </row>
+    <row r="1410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1410" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1410" t="s">
+        <v>1214</v>
+      </c>
+    </row>
     <row r="1411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1411" t="s">
+        <v>68</v>
+      </c>
       <c r="B1411" t="s">
-        <v>1186</v>
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1412" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="1423" spans="1:2" x14ac:dyDescent="0.25">
@@ -19377,7 +19453,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1368:H1384 A1386 A1387:H1387 C1388:H1388 A1388 A1401 C1401:H1401 A1409:A1410 C1409:H1410 A1414 C1414:H1414 C1416:H1416 A1416 A1417:H1419 A1420 C1420:H1420 A1440:B1440 A1415:H1415 A1426:H1426 A1425 A1428:H1431 A1426:B1427 C1424:H1427 A1431:B1432 C1429:H1432 A1433:H1439 A1439:A1441 C1437:H1441 A1442:H1048576 A1421:H1424 A1402:H1408 A1389:H1398 A1400:H1400 A1399 C1399:H1399 A1411:H1413">
+  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1368:H1384 A1386 A1387:H1387 C1388:H1388 A1388 C1409:H1410 A1414 C1414:H1414 C1416:H1416 A1416 A1417:H1419 A1420 C1420:H1420 A1440:B1440 A1415:H1415 A1426:H1426 A1425 A1428:H1431 A1426:B1427 C1424:H1427 A1431:B1432 C1429:H1432 A1433:H1439 A1439:A1441 C1437:H1441 A1442:H1048576 A1421:H1424 C1404:H1405 A1403:H1403 A1389:H1399 A1406:H1408 A1408:B1410 A1404:B1406 A1411:H1413 A1409:A1412 A1400:A1402 C1400:H1402">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Day 6 day complete
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA3F758-BCB2-435F-AC97-F669E662FC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B757A3-E5E6-4EEC-808B-7A189D4E7205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3444" uniqueCount="1296">
   <si>
     <t>Context</t>
   </si>
@@ -3694,6 +3694,237 @@
   </si>
   <si>
     <t>I don't know why you are always so negative. Can't we just eat a bit less and leave some food for people who need it?</t>
+  </si>
+  <si>
+    <t>Single person comments on scavenging</t>
+  </si>
+  <si>
+    <t>Might as well.</t>
+  </si>
+  <si>
+    <t>*sure i can go*</t>
+  </si>
+  <si>
+    <t>*i want to go check out the gas station*</t>
+  </si>
+  <si>
+    <t>Removed from scavenge party Jessica</t>
+  </si>
+  <si>
+    <t>Thank you for understanding!</t>
+  </si>
+  <si>
+    <t>Added to scavenge party Bob</t>
+  </si>
+  <si>
+    <t>I'll try to go a bit farther and find somewhere new.</t>
+  </si>
+  <si>
+    <t>Send Bob</t>
+  </si>
+  <si>
+    <t>Mind giving me the gun?</t>
+  </si>
+  <si>
+    <t>Send Bob with shotgun</t>
+  </si>
+  <si>
+    <t>Thanks. I'll see what I can find for us.</t>
+  </si>
+  <si>
+    <t>Send Bob without shotgun</t>
+  </si>
+  <si>
+    <t>Alright, I'm sure it'll be fine anyways. I'll avoid the forests.</t>
+  </si>
+  <si>
+    <t>Bob returned with gun</t>
+  </si>
+  <si>
+    <t>It's certainly clearing up out there. A bit foggy and barely snowing. I found a shed in the forest though... It had bodies in it. Looked fresh too. Executed. War's getting closer.</t>
+  </si>
+  <si>
+    <t>Bob returned without gun</t>
+  </si>
+  <si>
+    <t>I found an abandoned farm up the road. Not a lot inside, but I swear I could see people marching in the distance.</t>
+  </si>
+  <si>
+    <t>Added to scavenge party Violet</t>
+  </si>
+  <si>
+    <t>Send Violet</t>
+  </si>
+  <si>
+    <t>Send Violet with shotgun</t>
+  </si>
+  <si>
+    <t>Send Violet without shotgun</t>
+  </si>
+  <si>
+    <t>Violet returned with gun</t>
+  </si>
+  <si>
+    <t>Violet returned without gun</t>
+  </si>
+  <si>
+    <t>*cool*</t>
+  </si>
+  <si>
+    <t>*can i take the gun*</t>
+  </si>
+  <si>
+    <t>*ok sounds good*</t>
+  </si>
+  <si>
+    <t>*thanks*</t>
+  </si>
+  <si>
+    <t>*weather is improving outside*</t>
+  </si>
+  <si>
+    <t>*weather is clearing and i saw some people walking around*</t>
+  </si>
+  <si>
+    <t>Got Car</t>
+  </si>
+  <si>
+    <t>*i fixed up a car as well! itll be really useful for us*</t>
+  </si>
+  <si>
+    <t>Nice, a car will be really useful for us. Let's hope it has enough gas.</t>
+  </si>
+  <si>
+    <t>p_6_multi_want_to_go_out</t>
+  </si>
+  <si>
+    <t>b_6_might_as_well</t>
+  </si>
+  <si>
+    <t>v_6_sure_i_can_go</t>
+  </si>
+  <si>
+    <t>v_6_wants_to_check_gas_station</t>
+  </si>
+  <si>
+    <t>b_6_ill_go</t>
+  </si>
+  <si>
+    <t>j_6_b_nobody_should_go</t>
+  </si>
+  <si>
+    <t>b_6_j_thats_why_we_should</t>
+  </si>
+  <si>
+    <t>j_6_b_you_are_negative</t>
+  </si>
+  <si>
+    <t>b_6_j_we_need_it_dummy</t>
+  </si>
+  <si>
+    <t>v_6_it_could_get_worse</t>
+  </si>
+  <si>
+    <t>v_6_j_want_car</t>
+  </si>
+  <si>
+    <t>j_6_v_what_if_stealing_car</t>
+  </si>
+  <si>
+    <t>v_6_j_war_isnt_fair</t>
+  </si>
+  <si>
+    <t>j_6_solo_doesnt_want_to_go</t>
+  </si>
+  <si>
+    <t>j_6_multi_doesnt_want_to_go</t>
+  </si>
+  <si>
+    <t>p_6_solo_want_to_go_out</t>
+  </si>
+  <si>
+    <t>j_6_hesitant</t>
+  </si>
+  <si>
+    <t>j_6_relief</t>
+  </si>
+  <si>
+    <t>j_6_bargaining</t>
+  </si>
+  <si>
+    <t>p_6_j_you_must_go</t>
+  </si>
+  <si>
+    <t>j_6_p_can_i_have_gun</t>
+  </si>
+  <si>
+    <t>p_6_that_sounds_stupid</t>
+  </si>
+  <si>
+    <t>p_6_j_i_want_gun</t>
+  </si>
+  <si>
+    <t>p_6_j_sure_take_the_gun</t>
+  </si>
+  <si>
+    <t>j_6_defensive_scared</t>
+  </si>
+  <si>
+    <t>j_6_understanding</t>
+  </si>
+  <si>
+    <t>j_6_thanks_for_gun</t>
+  </si>
+  <si>
+    <t>b_6_jessica_died</t>
+  </si>
+  <si>
+    <t>p_6_jessica_died</t>
+  </si>
+  <si>
+    <t>v_6_jessica_died</t>
+  </si>
+  <si>
+    <t>b_6_trying_further</t>
+  </si>
+  <si>
+    <t>b_6_ask_for_gun</t>
+  </si>
+  <si>
+    <t>b_6_sent_with_gun</t>
+  </si>
+  <si>
+    <t>b_6_sent_without_gun</t>
+  </si>
+  <si>
+    <t>b_6_return_with_gun</t>
+  </si>
+  <si>
+    <t>b_6_return_without_gun</t>
+  </si>
+  <si>
+    <t>v_6_cool</t>
+  </si>
+  <si>
+    <t>v_6_ask_for_gun</t>
+  </si>
+  <si>
+    <t>v_6_sent_with_gun</t>
+  </si>
+  <si>
+    <t>v_6_sent_without_gun</t>
+  </si>
+  <si>
+    <t>v_6_return_with_gun</t>
+  </si>
+  <si>
+    <t>v_6_return_without_gun</t>
+  </si>
+  <si>
+    <t>v_6_got_car</t>
+  </si>
+  <si>
+    <t>b_6_got_car</t>
   </si>
 </sst>
 </file>
@@ -3751,7 +3982,2087 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="128">
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <gradientFill degree="90">
@@ -5192,8 +7503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1388" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1402" sqref="E1402"/>
+    <sheetView tabSelected="1" topLeftCell="A1524" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1543" sqref="E1543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18423,523 +20734,1284 @@
         <v>135</v>
       </c>
     </row>
-    <row r="1384" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1376" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1376" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1376" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D1376">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1377" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1377" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1378" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1378" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D1378">
+        <v>6</v>
+      </c>
+      <c r="E1378" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1379" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1379" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1380" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1381" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1381" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D1381">
+        <v>6</v>
+      </c>
+      <c r="E1381" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1382" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1382" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1383" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1384" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1386" t="s">
         <v>133</v>
       </c>
-      <c r="B1384" t="s">
-        <v>1180</v>
-      </c>
-      <c r="D1384">
+      <c r="B1386" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D1386">
         <v>6</v>
       </c>
     </row>
-    <row r="1385" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1385" t="s">
+    <row r="1387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1387" t="s">
         <v>460</v>
       </c>
-      <c r="B1385" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="1386" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1386" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1386" t="s">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="1387" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1387" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="1388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1387" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1388" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B1388" t="s">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="1389" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1220</v>
+      </c>
+      <c r="D1388">
+        <v>6</v>
+      </c>
+      <c r="E1388" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1389" t="s">
-        <v>1049</v>
+        <v>643</v>
       </c>
       <c r="B1389" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1390" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1390" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D1390">
+        <v>6</v>
+      </c>
+      <c r="E1390" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1391" t="s">
+        <v>643</v>
+      </c>
+      <c r="B1391" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1392" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D1392">
+        <v>6</v>
+      </c>
+      <c r="E1392" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1393" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1394" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1396" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1396" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="1390" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1390" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="1391" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1391" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="1393" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1393" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1393" t="s">
-        <v>1208</v>
-      </c>
-      <c r="D1393">
+      <c r="D1396">
         <v>6</v>
       </c>
     </row>
-    <row r="1394" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1394" t="s">
+    <row r="1397" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1397" t="s">
         <v>99</v>
       </c>
-      <c r="B1394" t="s">
+      <c r="B1397" t="s">
         <v>1209</v>
       </c>
     </row>
-    <row r="1395" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1395" t="s">
-        <v>460</v>
-      </c>
-      <c r="B1395" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="1396" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1396" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1396" t="s">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="1397" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1397" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="1398" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1398" t="s">
         <v>460</v>
       </c>
       <c r="B1398" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1399" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D1399">
+        <v>6</v>
+      </c>
+      <c r="E1399" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1400" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1401" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1401" t="s">
         <v>1131</v>
       </c>
     </row>
-    <row r="1399" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1399" t="s">
+    <row r="1402" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1402" t="s">
         <v>66</v>
       </c>
-      <c r="B1399" t="s">
+      <c r="B1402" t="s">
         <v>1186</v>
       </c>
-    </row>
-    <row r="1400" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1400" t="s">
+      <c r="D1402">
+        <v>6</v>
+      </c>
+      <c r="E1402" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
         <v>67</v>
       </c>
-      <c r="B1400" t="s">
+      <c r="B1403" t="s">
         <v>1216</v>
       </c>
-    </row>
-    <row r="1401" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1401" t="s">
+      <c r="D1403">
+        <v>6</v>
+      </c>
+      <c r="E1403" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1404" t="s">
         <v>66</v>
       </c>
-      <c r="B1401" t="s">
+      <c r="B1404" t="s">
         <v>1218</v>
       </c>
-    </row>
-    <row r="1402" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1402" t="s">
+      <c r="D1404">
+        <v>6</v>
+      </c>
+      <c r="E1404" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1405" t="s">
         <v>67</v>
       </c>
-      <c r="B1402" t="s">
+      <c r="B1405" t="s">
         <v>1217</v>
       </c>
-    </row>
-    <row r="1403" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1403" t="s">
+      <c r="D1405">
+        <v>6</v>
+      </c>
+      <c r="E1405" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1406" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1404" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1404" t="s">
+    <row r="1407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1407" t="s">
         <v>460</v>
       </c>
-      <c r="B1404" t="s">
+      <c r="B1407" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="1405" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1405" t="s">
+    <row r="1408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1408" t="s">
         <v>68</v>
       </c>
-      <c r="B1405" t="s">
+      <c r="B1408" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="1406" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1406" t="s">
+      <c r="D1408">
+        <v>6</v>
+      </c>
+      <c r="E1408" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1409" t="s">
         <v>643</v>
       </c>
-      <c r="B1406" t="s">
+      <c r="B1409" t="s">
         <v>1211</v>
       </c>
     </row>
-    <row r="1407" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1407" t="s">
+    <row r="1410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1410" t="s">
         <v>68</v>
       </c>
-      <c r="B1407" t="s">
+      <c r="B1410" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="1408" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1408" t="s">
+      <c r="D1410">
+        <v>6</v>
+      </c>
+      <c r="E1410" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1411" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1409" t="s">
+    <row r="1412" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1412" t="s">
         <v>460</v>
       </c>
-      <c r="B1409" t="s">
+      <c r="B1412" t="s">
         <v>1213</v>
       </c>
     </row>
-    <row r="1410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1410" t="s">
+    <row r="1413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1413" t="s">
         <v>66</v>
       </c>
-      <c r="B1410" t="s">
+      <c r="B1413" t="s">
         <v>1214</v>
       </c>
-    </row>
-    <row r="1411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1411" t="s">
+      <c r="D1413">
+        <v>6</v>
+      </c>
+      <c r="E1413" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1414" t="s">
         <v>68</v>
       </c>
-      <c r="B1411" t="s">
+      <c r="B1414" t="s">
         <v>1215</v>
       </c>
-    </row>
-    <row r="1412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1412" t="s">
+      <c r="D1414">
+        <v>6</v>
+      </c>
+      <c r="E1414" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1415" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1423" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1416" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1420" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1420" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D1420">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1421" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1421" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1422" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1422" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D1422">
+        <v>6</v>
+      </c>
+      <c r="E1422" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1423" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1424" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1424" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D1424">
+        <v>6</v>
+      </c>
+      <c r="E1424" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1425" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1426" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1428" t="s">
         <v>133</v>
       </c>
-      <c r="B1423" t="s">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="1424" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1424" t="s">
-        <v>460</v>
-      </c>
-      <c r="B1424" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="1425" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1425" t="s">
+      <c r="B1428" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D1428">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1429" t="s">
         <v>66</v>
       </c>
-      <c r="B1425" t="s">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="1426" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1426" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="1427" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1427" t="s">
+      <c r="B1429" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D1429">
+        <v>6</v>
+      </c>
+      <c r="E1429" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1430" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1430" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1431" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1433" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1433" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D1433">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1434" t="s">
         <v>66</v>
       </c>
-      <c r="B1427" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="1428" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1428" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="1429" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1429" t="s">
+      <c r="B1434" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D1434">
+        <v>6</v>
+      </c>
+      <c r="E1434" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1435" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1431" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1431" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1431" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="1432" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1432" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1432" t="s">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="1433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1433" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1433" t="s">
-        <v>1189</v>
-      </c>
-    </row>
-    <row r="1434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1434" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="1438" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1438" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1438" t="s">
         <v>133</v>
       </c>
       <c r="B1438" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="1439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1438">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1439" t="s">
         <v>66</v>
       </c>
       <c r="B1439" t="s">
         <v>1190</v>
       </c>
-    </row>
-    <row r="1440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1439">
+        <v>6</v>
+      </c>
+      <c r="E1439" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1440" t="s">
         <v>11</v>
       </c>
       <c r="B1440" t="s">
         <v>1191</v>
       </c>
-    </row>
-    <row r="1441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1440">
+        <v>6</v>
+      </c>
+      <c r="E1440" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1441" t="s">
-        <v>66</v>
+        <v>460</v>
       </c>
       <c r="B1441" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="1442" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1442" t="s">
-        <v>134</v>
+        <v>1049</v>
       </c>
       <c r="B1442" t="s">
         <v>1197</v>
       </c>
     </row>
-    <row r="1443" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1443" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1444" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1444" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D1444">
+        <v>6</v>
+      </c>
+      <c r="E1444" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1445" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1445" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1446" t="s">
         <v>11</v>
       </c>
-      <c r="B1443" t="s">
+      <c r="B1446" t="s">
         <v>1198</v>
       </c>
-    </row>
-    <row r="1444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1444" t="s">
+      <c r="D1446">
+        <v>6</v>
+      </c>
+      <c r="E1446" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1447" t="s">
         <v>134</v>
       </c>
-      <c r="B1444" t="s">
+      <c r="B1447" t="s">
         <v>1200</v>
       </c>
     </row>
-    <row r="1445" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1445" t="s">
+    <row r="1448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1448" t="s">
         <v>11</v>
       </c>
-      <c r="B1445" t="s">
+      <c r="B1448" t="s">
         <v>1194</v>
       </c>
-    </row>
-    <row r="1446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1446" t="s">
+      <c r="D1448">
+        <v>6</v>
+      </c>
+      <c r="E1448" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1449" t="s">
         <v>134</v>
       </c>
-      <c r="B1446" t="s">
+      <c r="B1449" t="s">
         <v>1195</v>
       </c>
     </row>
-    <row r="1447" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1447" t="s">
+    <row r="1450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1450" t="s">
         <v>11</v>
       </c>
-      <c r="B1447" t="s">
+      <c r="B1450" t="s">
         <v>1193</v>
       </c>
-    </row>
-    <row r="1448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1448" t="s">
+      <c r="D1450">
+        <v>6</v>
+      </c>
+      <c r="E1450" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1451" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1450" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1450" t="s">
+    <row r="1453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1453" t="s">
         <v>133</v>
       </c>
-      <c r="B1450" t="s">
+      <c r="B1453" t="s">
         <v>1197</v>
       </c>
-    </row>
-    <row r="1451" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1451" t="s">
+      <c r="D1453">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1454" t="s">
         <v>66</v>
       </c>
-      <c r="B1451" t="s">
+      <c r="B1454" t="s">
         <v>1199</v>
       </c>
-    </row>
-    <row r="1452" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1452" t="s">
+      <c r="D1454">
+        <v>6</v>
+      </c>
+      <c r="E1454" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1455" t="s">
         <v>1049</v>
       </c>
-      <c r="B1452" t="s">
+      <c r="B1455" t="s">
         <v>1060</v>
       </c>
     </row>
-    <row r="1453" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1453" t="s">
+    <row r="1456" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1456" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1455" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1455" t="s">
+    <row r="1458" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1458" t="s">
         <v>133</v>
       </c>
-      <c r="B1455" t="s">
+      <c r="B1458" t="s">
         <v>1200</v>
       </c>
-    </row>
-    <row r="1456" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1456" t="s">
+      <c r="D1458">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1459" t="s">
         <v>66</v>
       </c>
-      <c r="B1456" t="s">
+      <c r="B1459" t="s">
         <v>1201</v>
       </c>
-    </row>
-    <row r="1457" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1457" t="s">
+      <c r="D1459">
+        <v>6</v>
+      </c>
+      <c r="E1459" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1460" t="s">
         <v>1049</v>
       </c>
-      <c r="B1457" t="s">
+      <c r="B1460" t="s">
         <v>1060</v>
       </c>
     </row>
-    <row r="1458" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1458" t="s">
+    <row r="1461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1461" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1460" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1460" t="s">
+    <row r="1463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1463" t="s">
         <v>133</v>
       </c>
-      <c r="B1460" t="s">
+      <c r="B1463" t="s">
         <v>1195</v>
       </c>
-    </row>
-    <row r="1461" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1461" t="s">
+      <c r="D1463">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1464" t="s">
         <v>66</v>
       </c>
-      <c r="B1461" t="s">
+      <c r="B1464" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="1462" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1462" t="s">
+      <c r="D1464">
+        <v>6</v>
+      </c>
+      <c r="E1464" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1465" t="s">
         <v>1049</v>
       </c>
-      <c r="B1462" t="s">
+      <c r="B1465" t="s">
         <v>1059</v>
       </c>
     </row>
-    <row r="1463" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1463" t="s">
+    <row r="1466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1466" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1466" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1466" t="s">
+    <row r="1469" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1469" t="s">
         <v>133</v>
       </c>
-      <c r="B1466" t="s">
+      <c r="B1469" t="s">
         <v>1202</v>
       </c>
-    </row>
-    <row r="1467" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1467" t="s">
+      <c r="D1469">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1470" t="s">
         <v>460</v>
       </c>
-      <c r="B1467" t="s">
+      <c r="B1470" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="1468" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1468" t="s">
+    <row r="1471" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1471" t="s">
         <v>67</v>
       </c>
-      <c r="B1468" t="s">
+      <c r="B1471" t="s">
         <v>1203</v>
       </c>
-    </row>
-    <row r="1469" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1469" t="s">
+      <c r="D1471">
+        <v>6</v>
+      </c>
+      <c r="E1471" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1472" t="s">
         <v>643</v>
       </c>
-      <c r="B1469" t="s">
+      <c r="B1472" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="1470" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1470" t="s">
+    <row r="1473" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1473" t="s">
         <v>68</v>
       </c>
-      <c r="B1470" t="s">
+      <c r="B1473" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="1471" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1471" t="s">
+      <c r="D1473">
+        <v>6</v>
+      </c>
+      <c r="E1473" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1474" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="1472" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1472" t="s">
+    <row r="1475" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1475" t="s">
         <v>11</v>
       </c>
-      <c r="B1472" t="s">
+      <c r="B1475" t="s">
         <v>1205</v>
       </c>
-    </row>
-    <row r="1473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1473" t="s">
+      <c r="D1475">
+        <v>6</v>
+      </c>
+      <c r="E1475" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1476" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1474" t="s">
+    <row r="1477" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1477" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1483" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1483" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D1483">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1484" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1484" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D1484">
+        <v>6</v>
+      </c>
+      <c r="E1484" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1485" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1487" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1487" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D1487">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1488" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1488" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D1488">
+        <v>6</v>
+      </c>
+      <c r="E1488" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1489" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1489" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1490" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1492" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1492" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D1492">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1493" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1493" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D1493">
+        <v>6</v>
+      </c>
+      <c r="E1493" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1494" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1496" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1496" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D1496">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1497" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1497" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D1497">
+        <v>6</v>
+      </c>
+      <c r="E1497" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1498" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1500" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1500" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D1500">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1501" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1501" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D1501">
+        <v>6</v>
+      </c>
+      <c r="E1501" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1502" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1504" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1504" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D1504">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1505" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1505" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D1505">
+        <v>6</v>
+      </c>
+      <c r="E1505" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1506" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1514" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1514" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D1514">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1515" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1515" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D1515">
+        <v>6</v>
+      </c>
+      <c r="E1515" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1516" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1518" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1518" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D1518">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1519" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1519" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D1519">
+        <v>6</v>
+      </c>
+      <c r="E1519" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1520" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1520" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1521" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1523" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1523" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D1523">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1524" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1524" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D1524">
+        <v>6</v>
+      </c>
+      <c r="E1524" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1525" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1527" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1527" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D1527">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1528" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1528" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D1528">
+        <v>6</v>
+      </c>
+      <c r="E1528" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1529" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1531" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1531" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D1531">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1532" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1532" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D1532">
+        <v>6</v>
+      </c>
+      <c r="E1532" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1533" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1535" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1535" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D1535">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1536" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1536" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D1536">
+        <v>6</v>
+      </c>
+      <c r="E1536" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1537" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1542" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1542" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D1542">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1543" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1543" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D1543">
+        <v>6</v>
+      </c>
+      <c r="E1543" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1544" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1544" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1545" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1545" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D1545">
+        <v>6</v>
+      </c>
+      <c r="E1545" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1546" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1547" t="s">
         <v>135</v>
       </c>
     </row>
@@ -19453,113 +22525,369 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1368:H1384 A1386 A1387:H1387 C1388:H1388 A1388 C1409:H1410 A1414 C1414:H1414 C1416:H1416 A1416 A1417:H1419 A1420 C1420:H1420 A1440:B1440 A1415:H1415 A1426:H1426 A1425 A1428:H1431 A1426:B1427 C1424:H1427 A1431:B1432 C1429:H1432 A1433:H1439 A1439:A1441 C1437:H1441 A1442:H1048576 A1421:H1424 C1404:H1405 A1403:H1403 A1389:H1399 A1406:H1408 A1408:B1410 A1404:B1406 A1411:H1413 A1409:A1412 A1400:A1402 C1400:H1402">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1387:H1387 C1388:H1388 A1388 A1440:B1440 A1431:B1432 C1429:H1432 A1439:A1441 C1437:H1441 A1404:B1406 B1441:B1442 E1378:H1380 A1378:D1378 A1385:A1386 A1380:H1384 A1368:H1377 A1378:A1381 B1379 A1386:B1386 A1389:H1389 A1400:A1405 C1400:H1405 A1390 C1390:H1390 A1391:H1391 A1393:H1403 A1392 C1392:H1392 A1406:H1431 A1433:H1439 A1484 C1484:H1484 A1485:H1492 A1494:H1495 A1493 C1493:H1493 A1499:H1500 C1496:H1498 A1496:B1496 A1498:B1498 A1497 A1502:H1503 A1501 C1501:H1501 A1507:H1513 A1504:B1504 A1506:B1506 A1505 A1538:H1542 A1514:B1514 A1515 A1525:B1527 A1529:B1531 A1533:B1535 A1537:B1537 A1516:B1518 A1524 A1528 A1532 A1536 A1520:B1523 A1519 A1544:H1544 A1543 C1543:H1543 A1546:H1048576 A1545 C1545:H1545 A1442:H1483 C1504:H1506 C1514:H1537">
+    <cfRule type="expression" dxfId="9" priority="81">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="8" priority="82">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="7" priority="83">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="6" priority="84">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="5" priority="85">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="4" priority="86">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="3" priority="87">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="2" priority="88">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="1" priority="89">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="0" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="47" priority="10" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="127" priority="90" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="11" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="126" priority="91" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="12" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="125" priority="92" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="124" priority="93" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1385:H1385">
-    <cfRule type="expression" dxfId="29" priority="37">
+  <conditionalFormatting sqref="E1385:H1385">
+    <cfRule type="expression" dxfId="109" priority="117">
       <formula>LEFT($A1386, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="38">
+    <cfRule type="expression" dxfId="108" priority="118">
       <formula>$A1386="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="39">
+    <cfRule type="expression" dxfId="107" priority="119">
       <formula>$A1386="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="40">
+    <cfRule type="expression" dxfId="106" priority="120">
       <formula>$A1386="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="41">
+    <cfRule type="expression" dxfId="105" priority="121">
       <formula>$A1386="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="42">
+    <cfRule type="expression" dxfId="104" priority="122">
       <formula>$A1386="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="43">
+    <cfRule type="expression" dxfId="103" priority="123">
       <formula>$A1386="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="44">
+    <cfRule type="expression" dxfId="102" priority="124">
       <formula>$A1386="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="45">
+    <cfRule type="expression" dxfId="101" priority="125">
       <formula>$A1386="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="46">
+    <cfRule type="expression" dxfId="100" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1386:H1386">
-    <cfRule type="expression" dxfId="19" priority="57">
+    <cfRule type="expression" dxfId="99" priority="137">
       <formula>LEFT(#REF!, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="58">
+    <cfRule type="expression" dxfId="98" priority="138">
       <formula>#REF!="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="59">
+    <cfRule type="expression" dxfId="97" priority="139">
       <formula>#REF!="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="60">
+    <cfRule type="expression" dxfId="96" priority="140">
       <formula>#REF!="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="61">
+    <cfRule type="expression" dxfId="95" priority="141">
       <formula>#REF!="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="62">
+    <cfRule type="expression" dxfId="94" priority="142">
       <formula>#REF!="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="63">
+    <cfRule type="expression" dxfId="93" priority="143">
       <formula>#REF!="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="64">
+    <cfRule type="expression" dxfId="92" priority="144">
       <formula>#REF!="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="65">
+    <cfRule type="expression" dxfId="91" priority="145">
       <formula>#REF!="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="66">
+    <cfRule type="expression" dxfId="90" priority="146">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1379:D1379">
+    <cfRule type="expression" dxfId="89" priority="61">
+      <formula>LEFT($A1380, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="62">
+      <formula>$A1380="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="63">
+      <formula>$A1380="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="64">
+      <formula>$A1380="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="65">
+      <formula>$A1380="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="66">
+      <formula>$A1380="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="67">
+      <formula>$A1380="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="68">
+      <formula>$A1380="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="69">
+      <formula>$A1380="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="70">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1380:D1380">
+    <cfRule type="expression" dxfId="79" priority="71">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="72">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="73">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="74">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="75">
+      <formula>#REF!="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="76">
+      <formula>#REF!="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="77">
+      <formula>#REF!="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="78">
+      <formula>#REF!="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="79">
+      <formula>#REF!="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="80">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1384:D1384">
+    <cfRule type="expression" dxfId="69" priority="41">
+      <formula>LEFT($A1385, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="42">
+      <formula>$A1385="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="43">
+      <formula>$A1385="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="44">
+      <formula>$A1385="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="45">
+      <formula>$A1385="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="46">
+      <formula>$A1385="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="47">
+      <formula>$A1385="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="48">
+      <formula>$A1385="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="49">
+      <formula>$A1385="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="50">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1385:D1385">
+    <cfRule type="expression" dxfId="59" priority="51">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="52">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="53">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="54">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="55">
+      <formula>#REF!="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="56">
+      <formula>#REF!="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="57">
+      <formula>#REF!="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="58">
+      <formula>#REF!="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="59">
+      <formula>#REF!="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="60">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1378:H1378">
+    <cfRule type="expression" dxfId="49" priority="21">
+      <formula>LEFT($A1379, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="22">
+      <formula>$A1379="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="23">
+      <formula>$A1379="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="24">
+      <formula>$A1379="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="25">
+      <formula>$A1379="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="26">
+      <formula>$A1379="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="27">
+      <formula>$A1379="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="28">
+      <formula>$A1379="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="29">
+      <formula>$A1379="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="30">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1379:H1379">
+    <cfRule type="expression" dxfId="39" priority="31">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="32">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="33">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="34">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="35">
+      <formula>#REF!="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="36">
+      <formula>#REF!="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="37">
+      <formula>#REF!="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="38">
+      <formula>#REF!="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="39">
+      <formula>#REF!="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="40">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1377:D1377">
+    <cfRule type="expression" dxfId="29" priority="1">
+      <formula>LEFT($A1378, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="2">
+      <formula>$A1378="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="3">
+      <formula>$A1378="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="4">
+      <formula>$A1378="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="5">
+      <formula>$A1378="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="6">
+      <formula>$A1378="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="7">
+      <formula>$A1378="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="8">
+      <formula>$A1378="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="9">
+      <formula>$A1378="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1378:D1378">
+    <cfRule type="expression" dxfId="19" priority="11">
+      <formula>LEFT(#REF!, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="12">
+      <formula>#REF!="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>#REF!="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="14">
+      <formula>#REF!="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>#REF!="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>#REF!="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>#REF!="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>#REF!="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="19">
+      <formula>#REF!="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19671,48 +22999,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="43" priority="1">
+    <cfRule type="expression" dxfId="123" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="2">
+    <cfRule type="expression" dxfId="122" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="3">
+    <cfRule type="expression" dxfId="121" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="4">
+    <cfRule type="expression" dxfId="120" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="5">
+    <cfRule type="expression" dxfId="119" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="6">
+    <cfRule type="expression" dxfId="118" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="7">
+    <cfRule type="expression" dxfId="117" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="8">
+    <cfRule type="expression" dxfId="116" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="9">
+    <cfRule type="expression" dxfId="115" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="26">
+    <cfRule type="expression" dxfId="114" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="113" priority="13" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="112" priority="22" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="111" priority="24" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="110" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added IDs to day 6 lines
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6E0401-ED53-47E5-BB16-D25F35CAEC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC98E284-2A90-4B81-AA21-EB1C6FE9E81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3593" uniqueCount="1343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3635" uniqueCount="1384">
   <si>
     <t>Context</t>
   </si>
@@ -4066,6 +4066,129 @@
   </si>
   <si>
     <t>Alright, you can find any free room really, or just sleep out here. Whatever works.</t>
+  </si>
+  <si>
+    <t>h_6_arrive_at_door</t>
+  </si>
+  <si>
+    <t>p_6_twins_through_peephole</t>
+  </si>
+  <si>
+    <t>j_6_let_twins_in</t>
+  </si>
+  <si>
+    <t>h_6_stop_being_silent</t>
+  </si>
+  <si>
+    <t>h_6_im_hal</t>
+  </si>
+  <si>
+    <t>s_6_groan_introduction</t>
+  </si>
+  <si>
+    <t>h_6_who_we_are_start</t>
+  </si>
+  <si>
+    <t>none_5_mins_later</t>
+  </si>
+  <si>
+    <t>h_6_who_we_are_end</t>
+  </si>
+  <si>
+    <t>b_6_this_kid_can_talk</t>
+  </si>
+  <si>
+    <t>h_6_we_want_to_crash</t>
+  </si>
+  <si>
+    <t>h_6_idk_what_we_can_do</t>
+  </si>
+  <si>
+    <t>h_6_me_and_sal_are_good</t>
+  </si>
+  <si>
+    <t>h_6_skills</t>
+  </si>
+  <si>
+    <t>b_6_t_no_resources</t>
+  </si>
+  <si>
+    <t>j_6_t_conservative</t>
+  </si>
+  <si>
+    <t>b_6_j_surprised</t>
+  </si>
+  <si>
+    <t>j_6_t_they_are_dying</t>
+  </si>
+  <si>
+    <t>v_6_t_let_twins_in</t>
+  </si>
+  <si>
+    <t>v_6_t_keep_twins_out</t>
+  </si>
+  <si>
+    <t>p_6_t_sorry_but_stay_out</t>
+  </si>
+  <si>
+    <t>h_6_p_bargaining</t>
+  </si>
+  <si>
+    <t>p_6_t_sorry_no</t>
+  </si>
+  <si>
+    <t>h_6_s_get_up</t>
+  </si>
+  <si>
+    <t>s_6_groans</t>
+  </si>
+  <si>
+    <t>h_6_s_i_know_bro_lets_go</t>
+  </si>
+  <si>
+    <t>j_6_p_shouldve_let_them_in</t>
+  </si>
+  <si>
+    <t>p_6_going_to_open_door</t>
+  </si>
+  <si>
+    <t>h_6_p_thanks_so_much</t>
+  </si>
+  <si>
+    <t>s_6_groan_and_get_up</t>
+  </si>
+  <si>
+    <t>none_30_mins_pass</t>
+  </si>
+  <si>
+    <t>p_6_t_what_happened</t>
+  </si>
+  <si>
+    <t>s_6_p_shrapnel</t>
+  </si>
+  <si>
+    <t>b_6_t_where</t>
+  </si>
+  <si>
+    <t>j_6_t_where</t>
+  </si>
+  <si>
+    <t>v_6_t_where</t>
+  </si>
+  <si>
+    <t>p_6_t_where</t>
+  </si>
+  <si>
+    <t>s_6_pain</t>
+  </si>
+  <si>
+    <t>h_6_down_south</t>
+  </si>
+  <si>
+    <t>h_6_want_to_sleep</t>
+  </si>
+  <si>
+    <t>p_6_t_go_to_room</t>
   </si>
 </sst>
 </file>
@@ -7644,8 +7767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H1735"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1635" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1661" sqref="B1661:C1661"/>
+    <sheetView tabSelected="1" topLeftCell="A1632" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1662" sqref="E1662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22156,57 +22279,78 @@
         <v>135</v>
       </c>
     </row>
-    <row r="1553" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1553" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1553" t="s">
         <v>133</v>
       </c>
       <c r="B1553" t="s">
         <v>1288</v>
       </c>
-    </row>
-    <row r="1554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1553">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1554" t="s">
         <v>69</v>
       </c>
       <c r="B1554" t="s">
         <v>1289</v>
       </c>
-    </row>
-    <row r="1555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1554">
+        <v>6</v>
+      </c>
+      <c r="E1554" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1555" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1557" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1557" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1557" t="s">
         <v>133</v>
       </c>
       <c r="B1557" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="1558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1557">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1558" t="s">
         <v>11</v>
       </c>
       <c r="B1558" t="s">
         <v>1298</v>
       </c>
-    </row>
-    <row r="1559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1558">
+        <v>6</v>
+      </c>
+      <c r="E1558" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1559" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1561" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1561" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1561" t="s">
         <v>133</v>
       </c>
       <c r="B1561" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="1562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1561">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1562" t="s">
         <v>457</v>
       </c>
@@ -22214,86 +22358,131 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1563" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1563" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1563" t="s">
         <v>66</v>
       </c>
       <c r="B1563" t="s">
         <v>1299</v>
       </c>
-    </row>
-    <row r="1564" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1563">
+        <v>6</v>
+      </c>
+      <c r="E1563" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1564" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1565" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1565" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1565" t="s">
         <v>69</v>
       </c>
       <c r="B1565" t="s">
         <v>1300</v>
       </c>
-    </row>
-    <row r="1566" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1565">
+        <v>6</v>
+      </c>
+      <c r="E1565" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1566" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1567" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1567" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1567" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1569" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1569" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1569" t="s">
         <v>133</v>
       </c>
       <c r="B1569" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="1570" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1569">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1570" t="s">
         <v>69</v>
       </c>
       <c r="B1570" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="1571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1570">
+        <v>6</v>
+      </c>
+      <c r="E1570" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1571" t="s">
         <v>70</v>
       </c>
       <c r="B1571" t="s">
         <v>1302</v>
       </c>
-    </row>
-    <row r="1572" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1571">
+        <v>6</v>
+      </c>
+      <c r="E1571" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1572" t="s">
         <v>69</v>
       </c>
       <c r="B1572" t="s">
         <v>1303</v>
       </c>
-    </row>
-    <row r="1573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1572">
+        <v>6</v>
+      </c>
+      <c r="E1572" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1573" t="s">
         <v>5</v>
       </c>
       <c r="B1573" t="s">
         <v>1304</v>
       </c>
-    </row>
-    <row r="1574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1573">
+        <v>6</v>
+      </c>
+      <c r="E1573" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1574" t="s">
         <v>69</v>
       </c>
       <c r="B1574" t="s">
         <v>1305</v>
       </c>
-    </row>
-    <row r="1575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1574">
+        <v>6</v>
+      </c>
+      <c r="E1574" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1575" t="s">
         <v>457</v>
       </c>
@@ -22301,125 +22490,176 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1576" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1576" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1576" t="s">
         <v>67</v>
       </c>
       <c r="B1576" t="s">
         <v>1306</v>
       </c>
-    </row>
-    <row r="1577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1576">
+        <v>6</v>
+      </c>
+      <c r="E1576" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1577" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1578" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1578" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1578" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1581" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1581" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1581" t="s">
         <v>133</v>
       </c>
       <c r="B1581" t="s">
         <v>1307</v>
       </c>
-    </row>
-    <row r="1582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1581">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1582" t="s">
         <v>69</v>
       </c>
       <c r="B1582" t="s">
         <v>1308</v>
       </c>
-    </row>
-    <row r="1583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1582">
+        <v>6</v>
+      </c>
+      <c r="E1582" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1583" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1586" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1586" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1586" t="s">
         <v>133</v>
       </c>
       <c r="B1586" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="1587" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1586">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1587" t="s">
         <v>69</v>
       </c>
       <c r="B1587" t="s">
         <v>1309</v>
       </c>
-    </row>
-    <row r="1588" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1587">
+        <v>6</v>
+      </c>
+      <c r="E1587" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1588" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1591" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1591" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1591" t="s">
         <v>133</v>
       </c>
       <c r="B1591" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="1592" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1591">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1592" t="s">
         <v>69</v>
       </c>
       <c r="B1592" t="s">
         <v>1311</v>
       </c>
-    </row>
-    <row r="1593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1592">
+        <v>6</v>
+      </c>
+      <c r="E1592" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1593" t="s">
         <v>69</v>
       </c>
       <c r="B1593" t="s">
         <v>1312</v>
       </c>
-    </row>
-    <row r="1594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1593">
+        <v>6</v>
+      </c>
+      <c r="E1593" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1594" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1597" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1597" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1597" t="s">
         <v>133</v>
       </c>
       <c r="B1597" t="s">
         <v>1313</v>
       </c>
-    </row>
-    <row r="1598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1597">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1598" t="s">
         <v>67</v>
       </c>
       <c r="B1598" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="1599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1598">
+        <v>6</v>
+      </c>
+      <c r="E1598" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1599" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1601" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1601" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1601" t="s">
         <v>133</v>
       </c>
       <c r="B1601" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="1602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1601">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1602" t="s">
         <v>457</v>
       </c>
@@ -22427,54 +22667,75 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1603" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1603" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1603" t="s">
         <v>66</v>
       </c>
       <c r="B1603" t="s">
         <v>1317</v>
       </c>
-    </row>
-    <row r="1604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1603">
+        <v>6</v>
+      </c>
+      <c r="E1603" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1604" t="s">
         <v>67</v>
       </c>
       <c r="B1604" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="1605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1604">
+        <v>6</v>
+      </c>
+      <c r="E1604" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1605" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="1606" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1606" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1606" t="s">
         <v>66</v>
       </c>
       <c r="B1606" t="s">
         <v>1319</v>
       </c>
-    </row>
-    <row r="1607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1606">
+        <v>6</v>
+      </c>
+      <c r="E1606" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1607" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1608" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1608" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1608" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1611" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1611" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1611" t="s">
         <v>133</v>
       </c>
       <c r="B1611" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="1612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1611">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1612" t="s">
         <v>457</v>
       </c>
@@ -22482,94 +22743,145 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="1613" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1613" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1613" t="s">
         <v>68</v>
       </c>
       <c r="B1613" t="s">
         <v>1321</v>
       </c>
-    </row>
-    <row r="1614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1613">
+        <v>6</v>
+      </c>
+      <c r="E1613" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1614" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="1615" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1615" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1615" t="s">
         <v>68</v>
       </c>
       <c r="B1615" t="s">
         <v>1322</v>
       </c>
-    </row>
-    <row r="1616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1615">
+        <v>6</v>
+      </c>
+      <c r="E1615" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1616" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1617" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1617" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1617" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1620" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1620" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1620" t="s">
         <v>133</v>
       </c>
       <c r="B1620" t="s">
         <v>1323</v>
       </c>
-    </row>
-    <row r="1621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1620">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1621" t="s">
         <v>11</v>
       </c>
       <c r="B1621" t="s">
         <v>1324</v>
       </c>
-    </row>
-    <row r="1622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1621">
+        <v>6</v>
+      </c>
+      <c r="E1621" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1622" t="s">
         <v>69</v>
       </c>
       <c r="B1622" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="1623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1622">
+        <v>6</v>
+      </c>
+      <c r="E1622" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1623" t="s">
         <v>11</v>
       </c>
       <c r="B1623" t="s">
         <v>1326</v>
       </c>
-    </row>
-    <row r="1624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1623">
+        <v>6</v>
+      </c>
+      <c r="E1623" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1624" t="s">
         <v>69</v>
       </c>
       <c r="B1624" t="s">
         <v>1327</v>
       </c>
-    </row>
-    <row r="1625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1624">
+        <v>6</v>
+      </c>
+      <c r="E1624" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1625" t="s">
         <v>70</v>
       </c>
       <c r="B1625" t="s">
         <v>1328</v>
       </c>
-    </row>
-    <row r="1626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1625">
+        <v>6</v>
+      </c>
+      <c r="E1625" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1626" t="s">
         <v>69</v>
       </c>
       <c r="B1626" t="s">
         <v>1329</v>
       </c>
-    </row>
-    <row r="1627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1626">
+        <v>6</v>
+      </c>
+      <c r="E1626" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1627" t="s">
         <v>457</v>
       </c>
@@ -22577,41 +22889,56 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1628" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1628" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1628" t="s">
         <v>66</v>
       </c>
       <c r="B1628" t="s">
         <v>1330</v>
       </c>
-    </row>
-    <row r="1629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1628">
+        <v>6</v>
+      </c>
+      <c r="E1628" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1629" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1630" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1630" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1630" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="1634" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1634" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1634" t="s">
         <v>133</v>
       </c>
       <c r="B1634" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="1635" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1634">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1635" t="s">
         <v>11</v>
       </c>
       <c r="B1635" t="s">
         <v>1332</v>
       </c>
-    </row>
-    <row r="1636" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1635">
+        <v>6</v>
+      </c>
+      <c r="E1635" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1636" t="s">
         <v>457</v>
       </c>
@@ -22619,60 +22946,96 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1637" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1637" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1637" t="s">
         <v>67</v>
       </c>
       <c r="B1637" t="s">
         <v>1100</v>
       </c>
-    </row>
-    <row r="1638" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1637">
+        <v>6</v>
+      </c>
+      <c r="E1637" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1638" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1639" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1639" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1639" t="s">
         <v>69</v>
       </c>
       <c r="B1639" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="1640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1639">
+        <v>6</v>
+      </c>
+      <c r="E1639" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1640" t="s">
         <v>70</v>
       </c>
       <c r="B1640" t="s">
         <v>1334</v>
       </c>
-    </row>
-    <row r="1641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1640">
+        <v>6</v>
+      </c>
+      <c r="E1640" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1641" t="s">
         <v>5</v>
       </c>
       <c r="B1641" t="s">
         <v>1335</v>
       </c>
-    </row>
-    <row r="1642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1641">
+        <v>6</v>
+      </c>
+      <c r="E1641" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1642" t="s">
         <v>11</v>
       </c>
       <c r="B1642" t="s">
         <v>1336</v>
       </c>
-    </row>
-    <row r="1643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1642">
+        <v>6</v>
+      </c>
+      <c r="E1642" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1643" t="s">
         <v>70</v>
       </c>
       <c r="B1643" t="s">
         <v>1337</v>
       </c>
-    </row>
-    <row r="1644" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1643">
+        <v>6</v>
+      </c>
+      <c r="E1643" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1644" t="s">
         <v>457</v>
       </c>
@@ -22680,15 +23043,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1645" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1645" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1645" t="s">
         <v>66</v>
       </c>
       <c r="B1645" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="1646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1645">
+        <v>6</v>
+      </c>
+      <c r="E1645" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1646" t="s">
         <v>639</v>
       </c>
@@ -22696,15 +23065,21 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1647" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1647" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1647" t="s">
         <v>67</v>
       </c>
       <c r="B1647" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="1648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1647">
+        <v>6</v>
+      </c>
+      <c r="E1647" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1648" t="s">
         <v>639</v>
       </c>
@@ -22712,65 +23087,101 @@
         <v>68</v>
       </c>
     </row>
-    <row r="1649" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1649" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1649" t="s">
         <v>68</v>
       </c>
       <c r="B1649" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="1650" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1649">
+        <v>6</v>
+      </c>
+      <c r="E1649" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1650" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="1651" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1651" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1651" t="s">
         <v>11</v>
       </c>
       <c r="B1651" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="1652" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1651">
+        <v>6</v>
+      </c>
+      <c r="E1651" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1652" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1653" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1653" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1653" t="s">
         <v>70</v>
       </c>
       <c r="B1653" t="s">
         <v>1339</v>
       </c>
-    </row>
-    <row r="1654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1653">
+        <v>6</v>
+      </c>
+      <c r="E1653" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1654" t="s">
         <v>69</v>
       </c>
       <c r="B1654" t="s">
         <v>1340</v>
       </c>
-    </row>
-    <row r="1655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1654">
+        <v>6</v>
+      </c>
+      <c r="E1654" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1655" t="s">
         <v>69</v>
       </c>
       <c r="B1655" t="s">
         <v>1341</v>
       </c>
-    </row>
-    <row r="1656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1655">
+        <v>6</v>
+      </c>
+      <c r="E1655" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1656" t="s">
         <v>11</v>
       </c>
       <c r="B1656" t="s">
         <v>1342</v>
       </c>
-    </row>
-    <row r="1657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1656">
+        <v>6</v>
+      </c>
+      <c r="E1656" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1657" t="s">
         <v>135</v>
       </c>
@@ -23285,7 +23696,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1387:H1387 C1388:H1388 A1388 A1440:B1440 A1431:B1432 C1429:H1432 A1439:A1441 C1437:H1441 A1404:B1406 B1441:B1442 E1378:H1380 A1378:D1378 A1385:A1386 A1380:H1384 A1368:H1377 A1378:A1381 B1379 A1386:B1386 A1389:H1389 A1400:A1405 C1400:H1405 A1390 C1390:H1390 A1391:H1391 A1393:H1403 A1392 C1392:H1392 A1406:H1431 A1433:H1439 A1484 C1484:H1484 A1485:H1492 A1494:H1495 A1493 C1493:H1493 A1499:H1500 C1496:H1498 A1496:B1496 A1498:B1498 A1497 A1502:H1503 A1501 C1501:H1501 A1507:H1513 A1504:B1504 A1506:B1506 A1505 A1514:B1514 A1515 A1525:B1527 A1529:B1531 A1533:B1535 A1537:B1537 A1516:B1518 A1524 A1528 A1532 A1536 A1520:B1523 A1519 A1442:H1483 C1504:H1506 C1514:H1537 A1538:H1542 A1543 C1543:H1543 A1544:H1557 A1559:H1562 A1558 C1558:H1558 A1564:H1564 A1563 C1563:H1563 A1565 C1565:H1565 A1566:H1569 A1571:H1571 A1570 C1570:H1570 A1573:H1573 A1572 C1572:H1572 A1575:H1575 A1574 C1574:H1574 A1576 C1576:H1576 A1577:H1581 A1583:H1585 A1582 C1582:H1582 A1589:H1590 C1586:H1588 A1586:B1586 A1588:B1588 A1587 C1591:H1593 A1591:B1591 A1592:A1594 A1594:H1597 A1598 C1598:H1598 A1599:H1602 A1605:H1605 A1603:A1604 C1603:H1604 A1606 C1606:H1606 A1607:H1620 A1627:H1627 A1621:A1626 C1621:H1626 A1628 C1628:H1628 A1629:H1634 A1636:H1636 A1635 C1635:H1635 A1638:H1638 A1637 C1637:H1637 A1644:H1644 A1639:A1643 C1639:H1643 A1652:H1652 B1646 B1648 C1645:H1651 B1650 A1645:A1651 A1657:H1048576 A1653:A1656 C1653:H1656">
+  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1387:H1387 C1388:H1388 A1388 A1440:B1440 A1431:B1432 C1429:H1432 A1439:A1441 C1437:H1441 A1404:B1406 B1441:B1442 E1378:H1380 A1378:D1378 A1385:A1386 A1380:H1384 A1368:H1377 A1378:A1381 B1379 A1386:B1386 A1389:H1389 A1400:A1405 C1400:H1405 A1390 C1390:H1390 A1391:H1391 A1393:H1403 A1392 C1392:H1392 A1406:H1431 A1433:H1439 A1484 C1484:H1484 A1485:H1492 A1494:H1495 A1493 C1493:H1493 A1499:H1500 C1496:H1498 A1496:B1496 A1498:B1498 A1497 A1502:H1503 A1501 C1501:H1501 A1507:H1513 A1504:B1504 A1506:B1506 A1505 A1514:B1514 A1515 A1525:B1527 A1529:B1531 A1533:B1535 A1537:B1537 A1516:B1518 A1524 A1528 A1532 A1536 A1520:B1523 A1519 A1442:H1483 C1504:H1506 C1514:H1537 A1538:H1542 A1543 C1543:H1543 A1544:H1557 A1559:H1562 A1558 C1558:H1558 A1564:H1564 A1563 C1563:H1563 A1565 C1565:H1565 A1566:H1569 A1571:H1571 A1570 C1570:H1570 A1573:H1573 A1572 C1572:H1572 A1575:H1575 A1574 C1574:H1574 A1576 C1576:H1576 A1577:H1581 A1583:H1585 A1582 C1582:H1582 A1589:H1590 C1586:H1588 A1586:B1586 A1588:B1588 A1587 C1591:H1593 A1591:B1591 A1592:A1594 A1594:H1597 A1598 C1598:H1598 A1599:H1602 A1605:H1605 A1603:A1604 C1603:H1604 A1606 C1606:H1606 A1607:H1620 A1627:H1627 A1621:A1626 C1621:H1626 A1628 C1628:H1628 A1629:H1634 A1636:H1636 A1635 C1635:H1635 A1638:H1638 A1637 C1637:H1637 A1644:H1644 A1639:A1643 C1639:H1643 A1652:H1652 B1646 B1648 B1650 A1645:A1651 A1657:H1048576 A1653:A1656 C1653:H1656 C1645:H1651">
     <cfRule type="expression" dxfId="9" priority="81">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Day 7 Jessica scavenging
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849B08EF-4B05-45E9-A668-EABC60DA1C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372E9DD0-A25A-484A-87B0-33E8C3144491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3819" uniqueCount="1441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="1463">
   <si>
     <t>Context</t>
   </si>
@@ -4266,18 +4266,12 @@
     <t>Send twins</t>
   </si>
   <si>
-    <t>Send twins with shotgun</t>
-  </si>
-  <si>
     <t>Thanks. I'm a pretty good shot. Maybe we'll hunt an animal.</t>
   </si>
   <si>
     <t>Let's focus on getting you sealed up before we go running around the woods!</t>
   </si>
   <si>
-    <t>Send twins without shotgun</t>
-  </si>
-  <si>
     <t>I'm on death's door. Who's gonna defend me? Who will defend Hal?</t>
   </si>
   <si>
@@ -4360,6 +4354,78 @@
   </si>
   <si>
     <t>You should've let me go.</t>
+  </si>
+  <si>
+    <t>I can't! I don't know if you heard the radio, but I did - there might be people fighting out there!</t>
+  </si>
+  <si>
+    <t>They will shoot me!</t>
+  </si>
+  <si>
+    <t>j_7_worried</t>
+  </si>
+  <si>
+    <t>j_7_dont_send_me</t>
+  </si>
+  <si>
+    <t>Please keep it this way!</t>
+  </si>
+  <si>
+    <t>j_7_relief</t>
+  </si>
+  <si>
+    <t>Will you let me take the gun?</t>
+  </si>
+  <si>
+    <t>j_7_wants_gun</t>
+  </si>
+  <si>
+    <t>We will see what happens. I'll try to get some medicine, at least we actually need it.</t>
+  </si>
+  <si>
+    <t>j_7_will_try_to_find_meds</t>
+  </si>
+  <si>
+    <t>Sending Jessica without shotgun</t>
+  </si>
+  <si>
+    <t>Sending Jessica with shotgun</t>
+  </si>
+  <si>
+    <t>Whatever happens is your fault.</t>
+  </si>
+  <si>
+    <t>j_7_speechless</t>
+  </si>
+  <si>
+    <t>j_7_your_fault</t>
+  </si>
+  <si>
+    <t>Sending twins without shotgun</t>
+  </si>
+  <si>
+    <t>Sending twins with shotgun</t>
+  </si>
+  <si>
+    <t>She isn't coming back. It's been too long.</t>
+  </si>
+  <si>
+    <t>h_7_jessica_died</t>
+  </si>
+  <si>
+    <t>v_7_jessica_died</t>
+  </si>
+  <si>
+    <t>b_7_jessica_died</t>
+  </si>
+  <si>
+    <t>p_7_jessica_died</t>
+  </si>
+  <si>
+    <t>I don't think she made it... maybe I should've listened to her.</t>
+  </si>
+  <si>
+    <t>*i wonder what happened to her, dont think she will come back*</t>
   </si>
 </sst>
 </file>
@@ -4417,7 +4483,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="128">
+  <dxfs count="192">
     <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
@@ -4457,6 +4523,1606 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -7936,10 +9602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H1873"/>
+  <dimension ref="A1:H2004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1833" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1848" sqref="B1848"/>
+    <sheetView tabSelected="1" topLeftCell="A1902" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1926" sqref="C1926"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24234,15 +25900,15 @@
     </row>
     <row r="1809" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1809" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B1809" t="s">
-        <v>1032</v>
+        <v>640</v>
       </c>
     </row>
     <row r="1810" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1810" t="s">
-        <v>640</v>
+        <v>1036</v>
+      </c>
+      <c r="B1810" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="1811" spans="1:2" x14ac:dyDescent="0.25">
@@ -24255,7 +25921,7 @@
         <v>133</v>
       </c>
       <c r="B1814" t="s">
-        <v>1409</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1815" spans="1:2" x14ac:dyDescent="0.25">
@@ -24263,7 +25929,7 @@
         <v>70</v>
       </c>
       <c r="B1815" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1816" spans="1:2" x14ac:dyDescent="0.25">
@@ -24271,7 +25937,7 @@
         <v>69</v>
       </c>
       <c r="B1816" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1817" spans="1:2" x14ac:dyDescent="0.25">
@@ -24284,7 +25950,7 @@
         <v>133</v>
       </c>
       <c r="B1820" t="s">
-        <v>1412</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1821" spans="1:2" x14ac:dyDescent="0.25">
@@ -24292,7 +25958,7 @@
         <v>70</v>
       </c>
       <c r="B1821" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1822" spans="1:2" x14ac:dyDescent="0.25">
@@ -24300,7 +25966,7 @@
         <v>69</v>
       </c>
       <c r="B1822" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1823" spans="1:2" x14ac:dyDescent="0.25">
@@ -24321,7 +25987,7 @@
         <v>133</v>
       </c>
       <c r="B1829" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1830" spans="1:2" x14ac:dyDescent="0.25">
@@ -24329,7 +25995,7 @@
         <v>69</v>
       </c>
       <c r="B1830" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1831" spans="1:2" x14ac:dyDescent="0.25">
@@ -24337,7 +26003,7 @@
         <v>70</v>
       </c>
       <c r="B1831" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1832" spans="1:2" x14ac:dyDescent="0.25">
@@ -24345,7 +26011,7 @@
         <v>69</v>
       </c>
       <c r="B1832" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1833" spans="1:2" x14ac:dyDescent="0.25">
@@ -24353,7 +26019,7 @@
         <v>69</v>
       </c>
       <c r="B1833" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1834" spans="1:2" x14ac:dyDescent="0.25">
@@ -24366,7 +26032,7 @@
         <v>99</v>
       </c>
       <c r="B1836" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1837" spans="1:2" x14ac:dyDescent="0.25">
@@ -24374,7 +26040,7 @@
         <v>133</v>
       </c>
       <c r="B1837" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1838" spans="1:2" x14ac:dyDescent="0.25">
@@ -24382,7 +26048,7 @@
         <v>70</v>
       </c>
       <c r="B1838" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1839" spans="1:2" x14ac:dyDescent="0.25">
@@ -24390,7 +26056,7 @@
         <v>11</v>
       </c>
       <c r="B1839" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1840" spans="1:2" x14ac:dyDescent="0.25">
@@ -24398,7 +26064,7 @@
         <v>70</v>
       </c>
       <c r="B1840" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1841" spans="1:2" x14ac:dyDescent="0.25">
@@ -24406,7 +26072,7 @@
         <v>70</v>
       </c>
       <c r="B1841" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1842" spans="1:2" x14ac:dyDescent="0.25">
@@ -24422,7 +26088,7 @@
         <v>66</v>
       </c>
       <c r="B1843" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1844" spans="1:2" x14ac:dyDescent="0.25">
@@ -24438,7 +26104,7 @@
         <v>67</v>
       </c>
       <c r="B1845" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1846" spans="1:2" x14ac:dyDescent="0.25">
@@ -24446,7 +26112,7 @@
         <v>67</v>
       </c>
       <c r="B1846" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1847" spans="1:2" x14ac:dyDescent="0.25">
@@ -24480,7 +26146,7 @@
         <v>133</v>
       </c>
       <c r="B1853" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1854" spans="1:2" x14ac:dyDescent="0.25">
@@ -24488,7 +26154,7 @@
         <v>70</v>
       </c>
       <c r="B1854" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1855" spans="1:2" x14ac:dyDescent="0.25">
@@ -24496,7 +26162,7 @@
         <v>69</v>
       </c>
       <c r="B1855" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1856" spans="1:2" x14ac:dyDescent="0.25">
@@ -24504,7 +26170,7 @@
         <v>70</v>
       </c>
       <c r="B1856" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1857" spans="1:2" x14ac:dyDescent="0.25">
@@ -24512,7 +26178,7 @@
         <v>69</v>
       </c>
       <c r="B1857" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1858" spans="1:2" x14ac:dyDescent="0.25">
@@ -24528,7 +26194,7 @@
         <v>69</v>
       </c>
       <c r="B1859" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1860" spans="1:2" x14ac:dyDescent="0.25">
@@ -24544,7 +26210,7 @@
         <v>69</v>
       </c>
       <c r="B1861" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1862" spans="1:2" x14ac:dyDescent="0.25">
@@ -24568,7 +26234,7 @@
         <v>66</v>
       </c>
       <c r="B1864" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1865" spans="1:2" x14ac:dyDescent="0.25">
@@ -24576,7 +26242,7 @@
         <v>69</v>
       </c>
       <c r="B1865" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1866" spans="1:2" x14ac:dyDescent="0.25">
@@ -24592,7 +26258,7 @@
         <v>67</v>
       </c>
       <c r="B1867" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1868" spans="1:2" x14ac:dyDescent="0.25">
@@ -24600,7 +26266,7 @@
         <v>69</v>
       </c>
       <c r="B1868" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1869" spans="1:2" x14ac:dyDescent="0.25">
@@ -24616,7 +26282,7 @@
         <v>68</v>
       </c>
       <c r="B1870" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1871" spans="1:2" x14ac:dyDescent="0.25">
@@ -24624,7 +26290,7 @@
         <v>69</v>
       </c>
       <c r="B1871" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1872" spans="1:2" x14ac:dyDescent="0.25">
@@ -24632,486 +26298,788 @@
         <v>640</v>
       </c>
     </row>
-    <row r="1873" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1873" t="s">
         <v>135</v>
       </c>
     </row>
+    <row r="1879" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1879" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1879" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D1879">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1880" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1880" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D1880">
+        <v>7</v>
+      </c>
+      <c r="E1880" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1881" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1883" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1883" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D1883">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1884" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1884" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D1884">
+        <v>7</v>
+      </c>
+      <c r="E1884" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1885" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1887" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1887" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D1887">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1888" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1888" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D1888">
+        <v>7</v>
+      </c>
+      <c r="E1888" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1889" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1892" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1892" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1892">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1893" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1893" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1894" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1894" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D1894">
+        <v>7</v>
+      </c>
+      <c r="E1894" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1895" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1896" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B1896" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1897" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1900" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1900" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D1900">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1901" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1901" t="s">
+        <v>682</v>
+      </c>
+      <c r="D1901">
+        <v>7</v>
+      </c>
+      <c r="E1901" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1902" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1902" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D1902">
+        <v>7</v>
+      </c>
+      <c r="E1902" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1903" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1906" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1906" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D1906">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1907" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1907" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D1907">
+        <v>7</v>
+      </c>
+      <c r="E1907" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1908" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1912" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1912" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D1912">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1913" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1913" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1913" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1914" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1914" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D1914">
+        <v>7</v>
+      </c>
+      <c r="E1914" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1915" t="s">
+        <v>639</v>
+      </c>
+      <c r="B1915" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1916" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1916" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D1916">
+        <v>7</v>
+      </c>
+      <c r="E1916" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1917" t="s">
+        <v>639</v>
+      </c>
+      <c r="B1917" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1918" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1918" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D1918">
+        <v>7</v>
+      </c>
+      <c r="E1918" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1919" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1920" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1920" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D1920">
+        <v>7</v>
+      </c>
+      <c r="E1920" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1921" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1922" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1922" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1923" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B1923" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1924" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1925" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1942" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1942" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D1942">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1943" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1943" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D1943">
+        <v>7</v>
+      </c>
+      <c r="E1943" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1944" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1946" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1946" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D1946">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1947" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1947" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D1947">
+        <v>7</v>
+      </c>
+      <c r="E1947" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1948" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B1948" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1949" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1951" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1951" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D1951">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1952" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1952" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D1952">
+        <v>7</v>
+      </c>
+      <c r="E1952" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1953" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1955" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1955" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D1955">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1956" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1956" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D1956">
+        <v>7</v>
+      </c>
+      <c r="E1956" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1957" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1959" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1959" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D1959">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1960" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1960" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D1960">
+        <v>7</v>
+      </c>
+      <c r="E1960" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1961" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1963" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1963" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D1963">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1964" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1964" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D1964">
+        <v>7</v>
+      </c>
+      <c r="E1964" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1965" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1973" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1973" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1973" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D1973">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1974" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1974" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1974" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D1974">
+        <v>7</v>
+      </c>
+      <c r="E1974" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="1975" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1975" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1977" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1977" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1977" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D1977">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1978" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1978" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D1978">
+        <v>7</v>
+      </c>
+      <c r="E1978" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="1979" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1979" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B1979" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="1980" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1980" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1982" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1982" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1982" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D1982">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1983" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1983" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1983" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D1983">
+        <v>7</v>
+      </c>
+      <c r="E1983" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="1984" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1984" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1986" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1986" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1986" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D1986">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1987" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1987" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1987" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D1987">
+        <v>7</v>
+      </c>
+      <c r="E1987" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1988" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1990" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1990" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D1990">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1991" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1991" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D1991">
+        <v>7</v>
+      </c>
+      <c r="E1991" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1992" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1994" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1994" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D1994">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1995" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1995" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D1995">
+        <v>7</v>
+      </c>
+      <c r="E1995" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1996" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1999" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1999" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D1999">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2000" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2000" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D2000">
+        <v>7</v>
+      </c>
+      <c r="E2000" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2001" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2001" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2002" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2002" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D2002">
+        <v>7</v>
+      </c>
+      <c r="E2002" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2003" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2004" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H1260 A1261:A1263 C1261:H1263 A1264:H1266 A1267 C1267:H1267 A1268:H1279 A1280 C1280:H1280 A1281:H1281 A1282 C1282:H1282 A1283:H1283 A1284 C1284:H1284 A1285:H1285 A1286:A1287 C1286:H1287 A1288:H1305 A1306 C1306:H1306 A1307:H1323 C1324:H1324 A1324:A1326 A1325:H1325 C1326:H1326 A1327:H1338 A1339 C1339:H1339 A1340:H1346 A1347 C1347:H1347 A1348:H1351 A1352:A1353 C1352:H1353 A1354:H1361 A1362 C1362:H1362 A1363:H1363 A1364 C1364:H1364 A1365:H1366 A1367 C1367:H1367 A1387:H1387 C1388:H1388 A1388 A1440:B1440 A1431:B1432 C1429:H1432 A1439:A1441 C1437:H1441 A1404:B1406 B1441:B1442 E1378:H1380 A1378:D1378 A1385:A1386 A1380:H1384 A1368:H1377 A1378:A1381 B1379 A1386:B1386 A1389:H1389 A1400:A1405 C1400:H1405 A1390 C1390:H1390 A1391:H1391 A1393:H1403 A1392 C1392:H1392 A1406:H1431 A1433:H1439 A1484 C1484:H1484 A1485:H1492 A1494:H1495 A1493 C1493:H1493 A1499:H1500 C1496:H1498 A1496:B1496 A1498:B1498 A1497 A1502:H1503 A1501 C1501:H1501 A1507:H1513 A1504:B1504 A1506:B1506 A1505 A1514:B1514 A1515 A1525:B1527 A1529:B1531 A1533:B1535 A1537:B1537 A1516:B1518 A1524 A1528 A1532 A1536 A1520:B1523 A1519 A1442:H1483 C1504:H1506 C1514:H1537 A1538:H1542 A1543 C1543:H1543 A1544:H1557 A1559:H1562 A1558 C1558:H1558 A1564:H1564 A1563 C1563:H1563 A1565 C1565:H1565 A1566:H1569 A1571:H1571 A1570 C1570:H1570 A1573:H1573 A1572 C1572:H1572 A1575:H1575 A1574 C1574:H1574 A1576 C1576:H1576 A1577:H1581 A1583:H1585 A1582 C1582:H1582 A1589:H1590 C1586:H1588 A1586:B1586 A1588:B1588 A1587 C1591:H1593 A1591:B1591 A1592:A1594 A1594:H1597 A1598 C1598:H1598 A1599:H1602 A1605:H1605 A1603:A1604 C1603:H1604 A1606 C1606:H1606 A1607:H1620 A1627:H1627 A1621:A1626 C1621:H1626 A1628 C1628:H1628 A1629:H1634 A1636:H1636 A1635 C1635:H1635 A1638:H1638 A1637 C1637:H1637 A1644:H1644 A1639:A1643 C1639:H1643 A1652:H1652 B1646 B1648 B1650 A1645:A1651 A1653:A1656 C1653:H1656 C1645:H1651 A1657:H1751 A1752 C1752:H1752 A1753:H1759 A1762:H1762 A1760:A1761 A1764:H1764 A1763 C1763:H1763 A1767:H1767 A1765:A1766 C1765:H1766 A1769:H1770 A1768 C1768:H1768 A1772:H1776 A1771 C1771:H1771 C1777:H1780 A1780:B1780 A1777:A1779 A1781:H1787 A1789:H1789 A1788 C1788:H1788 A1791:H1792 A1790 C1790:H1790 A1793 C1793:H1793 C1797:H1799 A1798:B1798 A1799 A1794:H1796 A1795:A1797 A1800:H1807 A1808 C1808:H1808 A1809:H1814 A1817:H1819 A1815:A1816 C1815:H1816 C1820:H1823 A1820:B1820 A1823:B1823 A1821:A1823 A1824:H1829 A1830:A1833 C1830:H1833 A1834:H1839 A1840:A1841 C1840:H1841 A1858:H1858 A1860:H1861 C1849:H1862 A1853:H1853 A1863:H1048576 A1849:A1862 A1842:H1845 A1847:H1848 A1846 C1846:H1846">
-    <cfRule type="expression" dxfId="127" priority="81">
-      <formula>LEFT($A1, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="82">
-      <formula>$A1="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="83">
-      <formula>$A1="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="124" priority="84">
-      <formula>$A1="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="123" priority="85">
-      <formula>$A1="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="122" priority="86">
-      <formula>$A1="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="87">
-      <formula>$A1="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="88">
-      <formula>$A1="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="89">
-      <formula>$A1="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="94">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="117" priority="90" operator="containsText" text="Final">
-      <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="91" operator="containsText" text="Draft">
-      <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="92" operator="containsText" text="Placeholder">
-      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="93" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1385:H1385 C1760:H1760">
-    <cfRule type="expression" dxfId="113" priority="117">
-      <formula>LEFT($A1386, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="118">
-      <formula>$A1386="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="119">
-      <formula>$A1386="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="120">
-      <formula>$A1386="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="121">
-      <formula>$A1386="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="122">
-      <formula>$A1386="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="123">
-      <formula>$A1386="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="124">
-      <formula>$A1386="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="125">
-      <formula>$A1386="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="126">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1386:H1386 B1761:H1761">
-    <cfRule type="expression" dxfId="103" priority="137">
-      <formula>LEFT(#REF!, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="138">
-      <formula>#REF!="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="139">
-      <formula>#REF!="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="140">
-      <formula>#REF!="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="99" priority="141">
-      <formula>#REF!="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="142">
-      <formula>#REF!="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="143">
-      <formula>#REF!="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="144">
-      <formula>#REF!="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="95" priority="145">
-      <formula>#REF!="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="146">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1379:D1379">
-    <cfRule type="expression" dxfId="93" priority="61">
-      <formula>LEFT($A1380, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="92" priority="62">
-      <formula>$A1380="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="63">
-      <formula>$A1380="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="64">
-      <formula>$A1380="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="65">
-      <formula>$A1380="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="66">
-      <formula>$A1380="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="67">
-      <formula>$A1380="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="68">
-      <formula>$A1380="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="69">
-      <formula>$A1380="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="70">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1380:D1380">
-    <cfRule type="expression" dxfId="83" priority="71">
-      <formula>LEFT(#REF!, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="72">
-      <formula>#REF!="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="73">
-      <formula>#REF!="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="74">
-      <formula>#REF!="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75">
-      <formula>#REF!="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="76">
-      <formula>#REF!="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="77">
-      <formula>#REF!="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="78">
-      <formula>#REF!="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="79">
-      <formula>#REF!="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="80">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1384:D1384">
-    <cfRule type="expression" dxfId="73" priority="41">
-      <formula>LEFT($A1385, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="42">
-      <formula>$A1385="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="43">
-      <formula>$A1385="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="44">
-      <formula>$A1385="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="45">
-      <formula>$A1385="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="46">
-      <formula>$A1385="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="47">
-      <formula>$A1385="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="48">
-      <formula>$A1385="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="49">
-      <formula>$A1385="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="50">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1385:D1385">
-    <cfRule type="expression" dxfId="63" priority="51">
-      <formula>LEFT(#REF!, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="52">
-      <formula>#REF!="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="53">
-      <formula>#REF!="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="54">
-      <formula>#REF!="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="55">
-      <formula>#REF!="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="56">
-      <formula>#REF!="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="57">
-      <formula>#REF!="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="58">
-      <formula>#REF!="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="59">
-      <formula>#REF!="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="60">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1378:H1378">
-    <cfRule type="expression" dxfId="53" priority="21">
-      <formula>LEFT($A1379, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="22">
-      <formula>$A1379="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="23">
-      <formula>$A1379="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="24">
-      <formula>$A1379="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="25">
-      <formula>$A1379="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="26">
-      <formula>$A1379="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="27">
-      <formula>$A1379="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="28">
-      <formula>$A1379="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="29">
-      <formula>$A1379="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="30">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1379:H1379">
-    <cfRule type="expression" dxfId="43" priority="31">
-      <formula>LEFT(#REF!, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="32">
-      <formula>#REF!="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="33">
-      <formula>#REF!="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="34">
-      <formula>#REF!="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="35">
-      <formula>#REF!="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="36">
-      <formula>#REF!="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="37">
-      <formula>#REF!="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="38">
-      <formula>#REF!="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="39">
-      <formula>#REF!="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="40">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1377:D1377">
-    <cfRule type="expression" dxfId="33" priority="1">
-      <formula>LEFT($A1378, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="2">
-      <formula>$A1378="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="3">
-      <formula>$A1378="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="4">
-      <formula>$A1378="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="5">
-      <formula>$A1378="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="6">
-      <formula>$A1378="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="7">
-      <formula>$A1378="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="8">
-      <formula>$A1378="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="9">
-      <formula>$A1378="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="10">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1378:D1378">
-    <cfRule type="expression" dxfId="23" priority="11">
-      <formula>LEFT(#REF!, 2)="//"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="12">
-      <formula>#REF!="CHOICE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="13">
-      <formula>#REF!="CONVERSATION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14">
-      <formula>#REF!="END"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="15">
-      <formula>#REF!="GOTO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="16">
-      <formula>#REF!="IF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="17">
-      <formula>#REF!="ELIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
-      <formula>#REF!="ELSE"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="19">
-      <formula>#REF!="ENDIF"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="20">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A79F56-0C3E-4AB0-8A5A-02F26E99BBD1}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>457</v>
-      </c>
-      <c r="B6" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
-        <v>644</v>
-      </c>
-    </row>
-  </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
     <cfRule type="expression" dxfId="13" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
@@ -25140,21 +27108,174 @@
     <cfRule type="expression" dxfId="5" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="26">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="1" priority="12" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A79F56-0C3E-4AB0-8A5A-02F26E99BBD1}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>457</v>
+      </c>
+      <c r="B6" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>644</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:H1048576">
+    <cfRule type="expression" dxfId="47" priority="1">
+      <formula>LEFT($A1, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="2">
+      <formula>$A1="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="3">
+      <formula>$A1="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="4">
+      <formula>$A1="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="5">
+      <formula>$A1="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="6">
+      <formula>$A1="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="7">
+      <formula>$A1="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="8">
+      <formula>$A1="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="9">
+      <formula>$A1="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="26">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="containsText" dxfId="37" priority="13" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="22" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="24" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Day 7 afternoon complete
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3367AD37-AE17-4F57-B57B-0331330CACC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C465D8-2C26-496A-B64B-48764490E84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4167" uniqueCount="1581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4250" uniqueCount="1626">
   <si>
     <t>Context</t>
   </si>
@@ -4780,6 +4780,141 @@
   </si>
   <si>
     <t>MakeOCDecision</t>
+  </si>
+  <si>
+    <t>Twins OC vouch</t>
+  </si>
+  <si>
+    <t>You can't just kick us out? We just got here and my brother here is still hurt! That's not fair at all!</t>
+  </si>
+  <si>
+    <t>We are useful. I know we are young, but I am a great shot and Hal here can patch anyone up. Saved me from dying.</t>
+  </si>
+  <si>
+    <t>Besides, what does *she* do? Just sit around and eat up all of your food? Why not kick her out!</t>
+  </si>
+  <si>
+    <t>Watch your mouth. You talk too much.</t>
+  </si>
+  <si>
+    <t>b_7_oc_vouch_stop</t>
+  </si>
+  <si>
+    <t>s_7_b_weve_all_made_it_far</t>
+  </si>
+  <si>
+    <t>b_7_s_oc_vouch_dont_care</t>
+  </si>
+  <si>
+    <t>b_7_oc_vouch_kick_jessica</t>
+  </si>
+  <si>
+    <t>j_7_b_shocked</t>
+  </si>
+  <si>
+    <t>b_7_oc_vouch_jessica_useless</t>
+  </si>
+  <si>
+    <t>b_7_oc_vouch_life_death_taxes</t>
+  </si>
+  <si>
+    <t>j_7_oc_vouch_garbage_answer</t>
+  </si>
+  <si>
+    <t>v_7_oc_vouch_car</t>
+  </si>
+  <si>
+    <t>v_7_oc_vouch_nocar</t>
+  </si>
+  <si>
+    <t>v_7_oc_vouch_jessica_sucks</t>
+  </si>
+  <si>
+    <t>j_7_v_oc_vouch_suspicious</t>
+  </si>
+  <si>
+    <t>h_7_oc_vouch_what</t>
+  </si>
+  <si>
+    <t>s_7_oc_vouch_we_are_useful</t>
+  </si>
+  <si>
+    <t>h_7_oc_vouch_jessica_sucks</t>
+  </si>
+  <si>
+    <t>j_7_h_oc_vouch_sassy</t>
+  </si>
+  <si>
+    <t>p_7_oc_intro</t>
+  </si>
+  <si>
+    <t>p_7_oc_someone_has_to_go</t>
+  </si>
+  <si>
+    <t>Twins kicked out</t>
+  </si>
+  <si>
+    <t>Good luck. I hope you rot.</t>
+  </si>
+  <si>
+    <t>I'll die out there! I can't believe you are doing this to me!</t>
+  </si>
+  <si>
+    <t>*hopefully i see you at the border*</t>
+  </si>
+  <si>
+    <t>*thanks for letting me stay through the storm at least*</t>
+  </si>
+  <si>
+    <t>I can't believe you. We trusted you!</t>
+  </si>
+  <si>
+    <t>Hey, hey... it's alright.</t>
+  </si>
+  <si>
+    <t>Thanks for letting us stay for a bit. I'm feeling better</t>
+  </si>
+  <si>
+    <t>Let's get back on the road. Just another adventure, right?</t>
+  </si>
+  <si>
+    <t>Just another adventure.</t>
+  </si>
+  <si>
+    <t>Maybe we'll belong somewhere some day.</t>
+  </si>
+  <si>
+    <t>b_7_kicked_out</t>
+  </si>
+  <si>
+    <t>j_7_kicked_out</t>
+  </si>
+  <si>
+    <t>v_7_kicked_out_car</t>
+  </si>
+  <si>
+    <t>v_7_kicked_out_nocar</t>
+  </si>
+  <si>
+    <t>h_7_kicked_out_cant_believe</t>
+  </si>
+  <si>
+    <t>s_7_kicked_out_its_alright</t>
+  </si>
+  <si>
+    <t>s_7_kicked_out_thanks</t>
+  </si>
+  <si>
+    <t>h_7_kicked_out_speechless</t>
+  </si>
+  <si>
+    <t>s_7_kicked_out_adventure</t>
+  </si>
+  <si>
+    <t>h_7_kicked_out_adventure</t>
+  </si>
+  <si>
+    <t>h_7_kicked_out_soul_crushing</t>
   </si>
 </sst>
 </file>
@@ -4838,46 +4973,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <gradientFill degree="90">
@@ -5438,6 +5533,46 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5756,10 +5891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H2097"/>
+  <dimension ref="A1:H2139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2045" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2064" sqref="E2064"/>
+    <sheetView tabSelected="1" topLeftCell="A2111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2138" sqref="E2138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23798,6 +23933,12 @@
       <c r="B2034" t="s">
         <v>1546</v>
       </c>
+      <c r="D2034">
+        <v>7</v>
+      </c>
+      <c r="E2034" t="s">
+        <v>1602</v>
+      </c>
     </row>
     <row r="2035" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2035" t="s">
@@ -23806,6 +23947,12 @@
       <c r="B2035" t="s">
         <v>809</v>
       </c>
+      <c r="D2035">
+        <v>7</v>
+      </c>
+      <c r="E2035" t="s">
+        <v>1603</v>
+      </c>
     </row>
     <row r="2036" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2036" t="s">
@@ -23994,7 +24141,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2066" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2066" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2066" t="s">
         <v>133</v>
       </c>
@@ -24005,7 +24152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2067" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2067" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2067" t="s">
         <v>67</v>
       </c>
@@ -24015,8 +24162,11 @@
       <c r="D2067">
         <v>7</v>
       </c>
-    </row>
-    <row r="2068" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2067" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2068" t="s">
         <v>70</v>
       </c>
@@ -24026,8 +24176,11 @@
       <c r="D2068">
         <v>7</v>
       </c>
-    </row>
-    <row r="2069" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2068" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2069" t="s">
         <v>67</v>
       </c>
@@ -24037,8 +24190,11 @@
       <c r="D2069">
         <v>7</v>
       </c>
-    </row>
-    <row r="2070" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2069" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2070" t="s">
         <v>457</v>
       </c>
@@ -24046,7 +24202,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2071" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2071" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2071" t="s">
         <v>67</v>
       </c>
@@ -24056,8 +24212,11 @@
       <c r="D2071">
         <v>7</v>
       </c>
-    </row>
-    <row r="2072" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2071" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="2072" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2072" t="s">
         <v>66</v>
       </c>
@@ -24067,8 +24226,11 @@
       <c r="D2072">
         <v>7</v>
       </c>
-    </row>
-    <row r="2073" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2072" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="2073" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2073" t="s">
         <v>67</v>
       </c>
@@ -24078,8 +24240,11 @@
       <c r="D2073">
         <v>7</v>
       </c>
-    </row>
-    <row r="2074" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2073" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="2074" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2074" t="s">
         <v>67</v>
       </c>
@@ -24089,18 +24254,21 @@
       <c r="D2074">
         <v>7</v>
       </c>
-    </row>
-    <row r="2075" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2074" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="2075" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2075" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="2076" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2076" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2076" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2079" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2079" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2079" t="s">
         <v>133</v>
       </c>
@@ -24111,7 +24279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2080" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2080" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2080" t="s">
         <v>66</v>
       </c>
@@ -24121,13 +24289,16 @@
       <c r="D2080">
         <v>7</v>
       </c>
-    </row>
-    <row r="2081" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2080" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="2081" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2081" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2084" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2084" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2084" t="s">
         <v>133</v>
       </c>
@@ -24138,7 +24309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2085" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2085" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2085" t="s">
         <v>457</v>
       </c>
@@ -24146,7 +24317,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="2086" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2086" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2086" t="s">
         <v>68</v>
       </c>
@@ -24156,13 +24327,16 @@
       <c r="D2086">
         <v>7</v>
       </c>
-    </row>
-    <row r="2087" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2086" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2087" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="2088" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2088" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2088" t="s">
         <v>68</v>
       </c>
@@ -24172,13 +24346,16 @@
       <c r="D2088">
         <v>7</v>
       </c>
-    </row>
-    <row r="2089" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2088" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2089" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="2090" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2090" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2090" t="s">
         <v>457</v>
       </c>
@@ -24186,7 +24363,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2091" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2091" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2091" t="s">
         <v>68</v>
       </c>
@@ -24196,8 +24373,11 @@
       <c r="D2091">
         <v>7</v>
       </c>
-    </row>
-    <row r="2092" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2091" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2092" t="s">
         <v>66</v>
       </c>
@@ -24207,67 +24387,400 @@
       <c r="D2092">
         <v>7</v>
       </c>
-    </row>
-    <row r="2093" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2092" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2093" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="2094" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2094" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2094" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2097" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2097" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2097" t="s">
         <v>133</v>
+      </c>
+      <c r="B2097" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D2097">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2098" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2098" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D2098">
+        <v>7</v>
+      </c>
+      <c r="E2098" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2099" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2099" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D2099">
+        <v>7</v>
+      </c>
+      <c r="E2099" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="2100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2100" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2100" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2101" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2101" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D2101">
+        <v>7</v>
+      </c>
+      <c r="E2101" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2102" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2102" t="s">
+        <v>1585</v>
+      </c>
+      <c r="D2102">
+        <v>7</v>
+      </c>
+      <c r="E2102" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="2103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2103" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2104" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2111" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2111" t="s">
+        <v>866</v>
+      </c>
+      <c r="D2111">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2112" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2112" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D2112">
+        <v>7</v>
+      </c>
+      <c r="E2112" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="2113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2113" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2116" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2116" t="s">
+        <v>876</v>
+      </c>
+      <c r="D2116">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2117" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2117" t="s">
+        <v>1606</v>
+      </c>
+      <c r="D2117">
+        <v>7</v>
+      </c>
+      <c r="E2117" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2118" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2121" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2121" t="s">
+        <v>873</v>
+      </c>
+      <c r="D2121">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2122" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2122" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2123" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2123" t="s">
+        <v>1607</v>
+      </c>
+      <c r="D2123">
+        <v>7</v>
+      </c>
+      <c r="E2123" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2124" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2125" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2125" t="s">
+        <v>1608</v>
+      </c>
+      <c r="D2125">
+        <v>7</v>
+      </c>
+      <c r="E2125" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2126" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2127" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2130" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2130" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D2130">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2131" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2131" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D2131">
+        <v>7</v>
+      </c>
+      <c r="E2131" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2132" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2132" t="s">
+        <v>1610</v>
+      </c>
+      <c r="D2132">
+        <v>7</v>
+      </c>
+      <c r="E2132" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2133" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2133" t="s">
+        <v>1611</v>
+      </c>
+      <c r="D2133">
+        <v>7</v>
+      </c>
+      <c r="E2133" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2134" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2134" t="s">
+        <v>682</v>
+      </c>
+      <c r="D2134">
+        <v>7</v>
+      </c>
+      <c r="E2134" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2135" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2135" t="s">
+        <v>1612</v>
+      </c>
+      <c r="D2135">
+        <v>7</v>
+      </c>
+      <c r="E2135" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2136" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2136" t="s">
+        <v>1613</v>
+      </c>
+      <c r="D2136">
+        <v>7</v>
+      </c>
+      <c r="E2136" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2137" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2137" t="s">
+        <v>682</v>
+      </c>
+      <c r="D2137">
+        <v>7</v>
+      </c>
+      <c r="E2137" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2138" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2138" t="s">
+        <v>1614</v>
+      </c>
+      <c r="D2138">
+        <v>7</v>
+      </c>
+      <c r="E2138" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2139" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1957:H1959 A1956 C1956:H1956 A1961:H1964 A1960 C1960:H1960 A1966:H1968 A1965 C1965:H1965 A1969 C1969:H1969 A1970:H1973 A1977:H1995 A1974:A1976 A1997:H1999 A1996 C1996:H1996 A2000 C2000:H2000 A2001:H2003 A2004:A2007 C1974:H1976 C2004:H2006 A2007:H2033 C2034:H2035 A2034:A2035 A2036:H2040 A2042:H2044 A2041 C2041:H2041 A2046:H2049 A2045 C2045:H2045 A2051:H2051 A2050 C2050:H2050 A2053:H2056 A2052 C2052:H2052 A2058:H2060 A2057 C2057:H2057 A2061 C2061:H2061 A2062:H2066 A2070:H2070 A2067:A2069 C2067:H2069 A2073:H2073 A2071:A2072 C2071:H2072 C2074:H2075 A2074:A2075 A2076:H2079 A2080 C2080:H2080 A2081:H2085 A2087:H2087 A2086 C2086:H2086 A2089:H2090 A2088 C2088:H2088 A2091:A2092 C2091:H2092 A2093:H1048576 A1:H51 A53:H1955">
-    <cfRule type="expression" dxfId="27" priority="1">
+  <conditionalFormatting sqref="A1957:H1959 A1956 C1956:H1956 A1961:H1964 A1960 C1960:H1960 A1966:H1968 A1965 C1965:H1965 A1969 C1969:H1969 A1970:H1973 A1977:H1995 A1974:A1976 A1997:H1999 A1996 C1996:H1996 A2000 C2000:H2000 A2001:H2003 A2004:A2007 C1974:H1976 C2004:H2006 A2007:H2033 C2034:H2035 A2034:A2035 A2036:H2040 A2042:H2044 A2041 C2041:H2041 A2046:H2049 A2045 C2045:H2045 A2051:H2051 A2050 C2050:H2050 A2053:H2056 A2052 C2052:H2052 A2058:H2060 A2057 C2057:H2057 A2061 C2061:H2061 A2062:H2066 A2070:H2070 A2067:A2069 C2067:H2069 A2073:H2073 A2071:A2072 C2071:H2072 C2074:H2075 A2074:A2075 A2076:H2079 A2080 C2080:H2080 A2081:H2085 A2087:H2087 A2086 C2086:H2086 A2089:H2090 A2088 C2088:H2088 A2091:A2092 C2091:H2092 A1:H51 A53:H1955 A2093:H2097 A2100:H2100 A2098:A2099 C2098:H2099 A2101:A2102 C2101:H2102 A2103:H2111 C2121:H2127 A2124:B2124 A2123 A2126:B2127 A2125 A2121:B2122 A2128:H2130 A2113:H2116 A2112 C2112:H2112 A2118:H2120 A2117 C2117:H2117 A2139:H1048576 A2131:A2138 C2131:H2138">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G51 F53:G1048576">
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24379,48 +24892,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="26">
+    <cfRule type="expression" dxfId="14" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="11" priority="24" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="10" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Day 7 night written
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C465D8-2C26-496A-B64B-48764490E84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10248D26-F4E3-449D-831F-BD323B7E26D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4250" uniqueCount="1626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4463" uniqueCount="1681">
   <si>
     <t>Context</t>
   </si>
@@ -4915,6 +4915,171 @@
   </si>
   <si>
     <t>h_7_kicked_out_soul_crushing</t>
+  </si>
+  <si>
+    <t>Raiders arriving</t>
+  </si>
+  <si>
+    <t>HEY! WE KNOW YOU'RE IN THERE! OPEN UP!</t>
+  </si>
+  <si>
+    <t>OPEN UP OR WE ARE BUSTING OUR WAY IN!</t>
+  </si>
+  <si>
+    <t>WE WON'T HURT YOU! OPEN THE GODDAMN DOOR.</t>
+  </si>
+  <si>
+    <t>Oh shit.</t>
+  </si>
+  <si>
+    <t>That is a lot of people. At least five. They have guns.</t>
+  </si>
+  <si>
+    <t>WE CAN SEE YOU PUSSIES IN THERE.</t>
+  </si>
+  <si>
+    <t>OPEN THE FUCKING DOOR AND FIND OUT.</t>
+  </si>
+  <si>
+    <t>I WANT TO KILL YOU FOR ASKING SO MANY QUESTIONS.</t>
+  </si>
+  <si>
+    <t>WE WILL COME IN WHETHER YOU OPEN THIS DOOR OR NOT. IF YOU LET US IN, WE MIGHT NOT KILL YOU ALL.</t>
+  </si>
+  <si>
+    <t>*shoots bullets through door*</t>
+  </si>
+  <si>
+    <t>AH!</t>
+  </si>
+  <si>
+    <t>Holy shit.</t>
+  </si>
+  <si>
+    <t>Bobs opinion of raiders</t>
+  </si>
+  <si>
+    <t>Jessicas opinion of raiders</t>
+  </si>
+  <si>
+    <t>Violets opinion of raiders</t>
+  </si>
+  <si>
+    <t>Barricade the fucking door. If you let them in, we are dead.</t>
+  </si>
+  <si>
+    <t>Um.. oh god. Maybe you should let them in? Maybe they will just leave...</t>
+  </si>
+  <si>
+    <t>Shut the fuck up. Do not let them in.</t>
+  </si>
+  <si>
+    <t>(curling fists) ...</t>
+  </si>
+  <si>
+    <t>Hals opinion of raiders</t>
+  </si>
+  <si>
+    <t>Sals opinion of raiders</t>
+  </si>
+  <si>
+    <t>These fuckers better get ready. We aren't going down without a fight.</t>
+  </si>
+  <si>
+    <t>*whispering* I hope your door is strong.</t>
+  </si>
+  <si>
+    <t>Keep raiders out</t>
+  </si>
+  <si>
+    <t>Let raiders in</t>
+  </si>
+  <si>
+    <t>Get the fuck out of here.</t>
+  </si>
+  <si>
+    <t>YOU ASKED FOR IT.</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>*slamming sounds*</t>
+  </si>
+  <si>
+    <t>(muffled) Back up guys...</t>
+  </si>
+  <si>
+    <t>Shots ring out.</t>
+  </si>
+  <si>
+    <t>You are hit.</t>
+  </si>
+  <si>
+    <t>Shit, you're bleeding.</t>
+  </si>
+  <si>
+    <t>Put some pressure on that.</t>
+  </si>
+  <si>
+    <t>HOW DO YOU FUCKING LIKE THAT?</t>
+  </si>
+  <si>
+    <t>More shots ring out, hitting nothing.</t>
+  </si>
+  <si>
+    <t>WE WILL BE BACK YOU ASSHOLE. YOU'RE DEAD!</t>
+  </si>
+  <si>
+    <t>Okay, I'll open the door.</t>
+  </si>
+  <si>
+    <t>DON'T-</t>
+  </si>
+  <si>
+    <t>HEY!</t>
+  </si>
+  <si>
+    <t>*yelling*</t>
+  </si>
+  <si>
+    <t>STOP!</t>
+  </si>
+  <si>
+    <t>The raiders come inside.</t>
+  </si>
+  <si>
+    <t>Good. You did the right thing, huh?</t>
+  </si>
+  <si>
+    <t>Yells echo as the raiders drag everyone out.</t>
+  </si>
+  <si>
+    <t>We'll get rid of all your little problems. Little revolutionary scum, all of them.</t>
+  </si>
+  <si>
+    <t>Glory to Brasnia.</t>
+  </si>
+  <si>
+    <t>The raiders leave and close the door behind them.</t>
+  </si>
+  <si>
+    <t>Execute party members</t>
+  </si>
+  <si>
+    <t>You hear pleading and crying.</t>
+  </si>
+  <si>
+    <t>You hear nothing but the car starting up and driving away.</t>
+  </si>
+  <si>
+    <t>You hear nothing but the wind.</t>
+  </si>
+  <si>
+    <t>Day7Over</t>
+  </si>
+  <si>
+    <t>I love not implementing Ors</t>
   </si>
 </sst>
 </file>
@@ -4973,6 +5138,46 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <gradientFill degree="90">
@@ -5533,46 +5738,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5891,10 +6056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
-  <dimension ref="A1:H2139"/>
+  <dimension ref="A1:H2303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2138" sqref="E2138"/>
+    <sheetView tabSelected="1" topLeftCell="A2272" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2290" sqref="B2290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24736,51 +24901,989 @@
         <v>135</v>
       </c>
     </row>
+    <row r="2150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2150" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2150" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D2150">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2151" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2151" t="s">
+        <v>1627</v>
+      </c>
+      <c r="D2151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2152" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2152" t="s">
+        <v>1628</v>
+      </c>
+      <c r="D2152">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2153" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2153" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2154" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2154" t="s">
+        <v>1630</v>
+      </c>
+      <c r="D2154">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2155" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2156" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2156" t="s">
+        <v>1629</v>
+      </c>
+      <c r="D2156">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2157" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2160" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2160" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2160">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2161" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2161" t="s">
+        <v>1631</v>
+      </c>
+      <c r="D2161">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2162" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2165" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2165" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2165">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2166" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2166" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D2166">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2167" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2170" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2170" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2170">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2171" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2171" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D2171">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2172" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2175" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2175" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D2175">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2176" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2176" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D2176">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2177" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2180" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2180" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2180">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2181" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2181" t="s">
+        <v>1635</v>
+      </c>
+      <c r="D2181">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2182" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2185" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2185" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D2185">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2186" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2186" t="s">
+        <v>1636</v>
+      </c>
+      <c r="D2186">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2187" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2187" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2188" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2188" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D2188">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2189" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2190" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2190" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2191" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2191" t="s">
+        <v>1638</v>
+      </c>
+      <c r="D2191">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2192" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2193" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2196" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2196" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2197" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2197" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2198" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2200" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2200" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2201" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2201" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2202" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2202" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2203" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2203" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2204" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2205" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2208" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2208" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2209" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2209" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2210" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2213" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2213" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2214" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2214" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2215" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2218" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2218" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2219" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2219" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2220" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2224" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2224" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2225" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2225" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2226" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2226" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2227" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B2227" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2228" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2228" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2229" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2229" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2230" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2230" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2231" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2231" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2232" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2232" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2233" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2233" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2234" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2234" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2235" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2236" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2236" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2237" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2237" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2238" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2238" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2239" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2243" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2243" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2244" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2244" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2245" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2245" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2246" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2246" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2247" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2248" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2248" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2249" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2249" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2250" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2251" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2251" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2252" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2252" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2253" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2254" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2254" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2255" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2255" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2256" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2257" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2257" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2258" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2258" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2259" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2259" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2260" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2260" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2261" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2261" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2262" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2262" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2263" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2263" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2264" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2264" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2265" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2265" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2266" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2266" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2267" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2267" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2268" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2268" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2269" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2269" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2270" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2270" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2271" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2272" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2272" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2273" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2273" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2274" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2274" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2275" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2275" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2276" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B2276" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2277" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2277" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2278" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B2278" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2279" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2279" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2280" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B2280" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2281" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2281" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2282" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B2282" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2283" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2284" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B2284" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2285" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2291" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2291" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2292" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2292" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2293" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2293" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2294" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2294" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2295" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2295" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2296" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2297" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2297" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2298" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2299" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B2299" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2300" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2302" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2302" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2303" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1957:H1959 A1956 C1956:H1956 A1961:H1964 A1960 C1960:H1960 A1966:H1968 A1965 C1965:H1965 A1969 C1969:H1969 A1970:H1973 A1977:H1995 A1974:A1976 A1997:H1999 A1996 C1996:H1996 A2000 C2000:H2000 A2001:H2003 A2004:A2007 C1974:H1976 C2004:H2006 A2007:H2033 C2034:H2035 A2034:A2035 A2036:H2040 A2042:H2044 A2041 C2041:H2041 A2046:H2049 A2045 C2045:H2045 A2051:H2051 A2050 C2050:H2050 A2053:H2056 A2052 C2052:H2052 A2058:H2060 A2057 C2057:H2057 A2061 C2061:H2061 A2062:H2066 A2070:H2070 A2067:A2069 C2067:H2069 A2073:H2073 A2071:A2072 C2071:H2072 C2074:H2075 A2074:A2075 A2076:H2079 A2080 C2080:H2080 A2081:H2085 A2087:H2087 A2086 C2086:H2086 A2089:H2090 A2088 C2088:H2088 A2091:A2092 C2091:H2092 A1:H51 A53:H1955 A2093:H2097 A2100:H2100 A2098:A2099 C2098:H2099 A2101:A2102 C2101:H2102 A2103:H2111 C2121:H2127 A2124:B2124 A2123 A2126:B2127 A2125 A2121:B2122 A2128:H2130 A2113:H2116 A2112 C2112:H2112 A2118:H2120 A2117 C2117:H2117 A2139:H1048576 A2131:A2138 C2131:H2138">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="A1957:H1959 A1956 C1956:H1956 A1961:H1964 A1960 C1960:H1960 A1966:H1968 A1965 C1965:H1965 A1969 C1969:H1969 A1970:H1973 A1977:H1995 A1974:A1976 A1997:H1999 A1996 C1996:H1996 A2000 C2000:H2000 A2001:H2003 A2004:A2007 C1974:H1976 C2004:H2006 A2007:H2033 C2034:H2035 A2034:A2035 A2036:H2040 A2042:H2044 A2041 C2041:H2041 A2046:H2049 A2045 C2045:H2045 A2051:H2051 A2050 C2050:H2050 A2053:H2056 A2052 C2052:H2052 A2058:H2060 A2057 C2057:H2057 A2061 C2061:H2061 A2062:H2066 A2070:H2070 A2067:A2069 C2067:H2069 A2073:H2073 A2071:A2072 C2071:H2072 C2074:H2075 A2074:A2075 A2076:H2079 A2080 C2080:H2080 A2081:H2085 A2087:H2087 A2086 C2086:H2086 A2089:H2090 A2088 C2088:H2088 A2091:A2092 C2091:H2092 A1:H51 A53:H1955 A2093:H2097 A2100:H2100 A2098:A2099 C2098:H2099 A2101:A2102 C2101:H2102 A2103:H2111 C2121:H2127 A2124:B2124 A2123 A2126:B2127 A2125 A2121:B2122 A2128:H2130 A2113:H2116 A2112 C2112:H2112 A2118:H2120 A2117 C2117:H2117 A2139:H2150 A2131:A2138 C2131:H2138 A2153:H2155 A2151:A2152 C2151:H2152 A2156 C2156:H2156 A2157:H2160 A2162:H2164 A2161 C2161:H2161 C2165:H2167 A2165:B2165 A2167:B2167 A2166 A2168:H2170 A2172:H2175 A2171 C2171:H2171 A2177:H2180 A2176 C2176:H2176 A2182:H2185 A2181 C2181:H2181 A2186 C2186:H2186 A2187:H2187 A2189:H2190 A2188 C2188:H2188 A2191 C2191:H2191 A2200:H2202 C2199:H2199 C2203:H2205 A2198:B2200 A2192:H2198 A2201:A2205 A2204:B2210 A2206:H2213 A2215:H2218 A2214 C2214:H2214 A2219 C2219:H2219 A2220:H2224 A2225 C2225:H2225 C2229:H2229 A2230:H2231 A2232 C2232:H2232 A2233:H2235 A2239:H2242 C2236:H2238 A2243:B2243 A2244 C2243:H2253 A2254:H2256 A2245:B2256 A2236:A2239 A2228:A2230 A2226:H2228 A2257:A2258 C2257:H2258 A2259:H2260 A2262:H2262 A2261 C2261:H2261 A2265:H2265 C2263:H2264 A2263:B2263 A2264 A2268:H2268 C2266:H2267 A2266:B2266 A2267 C2269:H2270 A2269:B2269 A2270 A2271:H2271 A2274:H2274 A2272:A2273 C2272:H2273 C2275:H2287 A2287:B2287 A2285:B2285 A2275:B2282 A2283:A2286 B2284 A2288:H1048576">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="25" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G51 F53:G1048576">
-    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24892,48 +25995,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="26">
+    <cfRule type="expression" dxfId="4" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="1" priority="24" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="0" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
importing day 6 and 7
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DF0E8E-233B-475A-9FAF-FC72CDE48BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9115100C-BA29-478F-82BD-7401381DF0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4543" uniqueCount="1730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4542" uniqueCount="1729">
   <si>
     <t>Context</t>
   </si>
@@ -5206,9 +5206,6 @@
   </si>
   <si>
     <t>Day 1 peephole</t>
-  </si>
-  <si>
-    <t>Sending Jessica to scavenge or not</t>
   </si>
   <si>
     <t>NOT Sending Jessica to scavange</t>
@@ -6205,8 +6202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H2488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1504" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1523" sqref="B1523"/>
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B320" sqref="B320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9291,14 +9288,6 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B317" t="s">
-        <v>1723</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
         <v>135</v>
       </c>
     </row>
@@ -9307,7 +9296,7 @@
         <v>133</v>
       </c>
       <c r="B321" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D321">
         <v>2</v>
@@ -9343,7 +9332,7 @@
         <v>133</v>
       </c>
       <c r="B328" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D328">
         <v>2</v>
@@ -9566,7 +9555,7 @@
         <v>133</v>
       </c>
       <c r="B354" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.25">
@@ -12778,12 +12767,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="718" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A718" t="s">
+        <v>638</v>
+      </c>
+    </row>
     <row r="719" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
         <v>456</v>
       </c>
       <c r="B719" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="720" spans="1:6" x14ac:dyDescent="0.25">
@@ -13083,7 +13077,7 @@
         <v>456</v>
       </c>
       <c r="B795" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="796" spans="1:6" x14ac:dyDescent="0.25">
@@ -17553,7 +17547,7 @@
         <v>71</v>
       </c>
       <c r="B1287" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="D1287">
         <v>5</v>
@@ -26403,7 +26397,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H719 H720:H727 A720:G726 A728:H978 A979:B979 A980:H981 A991:H1287 A1289:H1289 A1296:H1048576 A1288:B1288">
+  <conditionalFormatting sqref="A720:G726 H720:H727 A728:H978 A979:B979 A980:H981 A991:H1287 A1288:B1288 A1289:H1289 A1296:H1048576 A1:H719">
     <cfRule type="expression" dxfId="27" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
@@ -26435,7 +26429,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G726 F728:G978 F980:G981 F1296:G1048576 F991:G1287 F1289:G1289">
+  <conditionalFormatting sqref="F1:G726 F728:G978 F980:G981 F991:G1287 F1289:G1289 F1296:G1048576">
     <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Various flow elements implemented
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF62AFA-D4F6-4806-8027-FB14C5EAA18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBADB61-B599-4F07-94DE-56599C9C15F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4582" uniqueCount="1733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4585" uniqueCount="1734">
   <si>
     <t>Context</t>
   </si>
@@ -5236,6 +5236,9 @@
   </si>
   <si>
     <t>DoorOptions</t>
+  </si>
+  <si>
+    <t>Advance</t>
   </si>
 </sst>
 </file>
@@ -6214,8 +6217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H2488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1441" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1460" sqref="B1460"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7581,6 +7584,19 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>133</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>135</v>
       </c>
     </row>
@@ -26808,23 +26824,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -27063,32 +27062,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27105,4 +27096,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tweaked a day 4 convo
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBADB61-B599-4F07-94DE-56599C9C15F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44047C7-740F-46B9-AB74-514505819023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4585" uniqueCount="1734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4583" uniqueCount="1737">
   <si>
     <t>Context</t>
   </si>
@@ -5239,6 +5239,15 @@
   </si>
   <si>
     <t>Advance</t>
+  </si>
+  <si>
+    <t>//CHOICE</t>
+  </si>
+  <si>
+    <t>//Player</t>
+  </si>
+  <si>
+    <t>I'm sure, we're not letting anyone inside.</t>
   </si>
 </sst>
 </file>
@@ -5297,46 +5306,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <gradientFill degree="90">
@@ -5897,6 +5866,46 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -6217,8 +6226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H2488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A952" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B970" sqref="B970"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13384,14 +13393,6 @@
     </row>
     <row r="806" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B806" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="807" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A807" t="s">
         <v>135</v>
       </c>
     </row>
@@ -14505,7 +14506,7 @@
     </row>
     <row r="948" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A948" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B948" t="s">
         <v>66</v>
@@ -14549,7 +14550,7 @@
     </row>
     <row r="952" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A952" t="s">
-        <v>134</v>
+        <v>1734</v>
       </c>
       <c r="B952" t="s">
         <v>709</v>
@@ -14557,7 +14558,7 @@
     </row>
     <row r="953" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A953" t="s">
-        <v>11</v>
+        <v>1735</v>
       </c>
       <c r="B953" t="s">
         <v>717</v>
@@ -14574,7 +14575,7 @@
     </row>
     <row r="954" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A954" t="s">
-        <v>134</v>
+        <v>1734</v>
       </c>
       <c r="B954" t="s">
         <v>719</v>
@@ -14585,7 +14586,7 @@
         <v>11</v>
       </c>
       <c r="B955" t="s">
-        <v>718</v>
+        <v>1736</v>
       </c>
       <c r="D955">
         <v>4</v>
@@ -26621,48 +26622,48 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26774,48 +26775,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="26">
+    <cfRule type="expression" dxfId="14" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="11" priority="24" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="10" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26824,6 +26825,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -27062,24 +27080,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27096,29 +27122,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed one of the lines that would pop up even with a character dead
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21073FF7-5F1E-49B6-BE63-ECFDC4FCCA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B0D966-98B3-4F1C-8369-C0857F738F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Lines" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4598" uniqueCount="1739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4599" uniqueCount="1740">
   <si>
     <t>Context</t>
   </si>
@@ -5254,6 +5254,9 @@
   </si>
   <si>
     <t>TutDad_LookForKeys</t>
+  </si>
+  <si>
+    <t>!bobdead</t>
   </si>
 </sst>
 </file>
@@ -6232,8 +6235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H2488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F210" sqref="F210"/>
+    <sheetView tabSelected="1" topLeftCell="A1062" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1091" sqref="B1091"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10843,7 +10846,7 @@
         <v>456</v>
       </c>
       <c r="B483" t="s">
-        <v>66</v>
+        <v>491</v>
       </c>
     </row>
     <row r="484" spans="1:6" x14ac:dyDescent="0.25">
@@ -11889,7 +11892,10 @@
     </row>
     <row r="607" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>460</v>
+        <v>636</v>
+      </c>
+      <c r="B607" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="608" spans="1:6" x14ac:dyDescent="0.25">
@@ -13037,7 +13043,7 @@
         <v>456</v>
       </c>
       <c r="B729" t="s">
-        <v>67</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="730" spans="1:6" x14ac:dyDescent="0.25">
@@ -26903,6 +26909,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -27141,24 +27164,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27175,29 +27206,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed missing door links
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21073FF7-5F1E-49B6-BE63-ECFDC4FCCA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE83809A-ADB9-4905-8846-3A5817AD9C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4598" uniqueCount="1739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4600" uniqueCount="1739">
   <si>
     <t>Context</t>
   </si>
@@ -6232,8 +6232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H2488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F210" sqref="F210"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7581,6 +7581,9 @@
       <c r="A136" t="s">
         <v>134</v>
       </c>
+      <c r="B136" t="s">
+        <v>1730</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E137" t="s">
@@ -7590,6 +7593,9 @@
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>134</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1729</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -26903,6 +26909,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -27141,24 +27164,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27175,29 +27206,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Jessica ghost lines are fixed now
</commit_message>
<xml_diff>
--- a/Lines.xlsx
+++ b/Lines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC45587B-9AE9-4484-9A90-2C6C6EBF3DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4852633-4100-455A-B958-F597EB0DB8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5720E99C-D5EB-444B-A102-DF29F8B30E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Lines" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4575" uniqueCount="1745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4592" uniqueCount="1745">
   <si>
     <t>Context</t>
   </si>
@@ -5329,7 +5329,267 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="72">
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
@@ -5369,6 +5629,826 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="2"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBECD0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFECC6F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -6250,8 +7330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1AC0A-1CB8-418F-B007-6C69A37E9EC1}">
   <dimension ref="A1:H2493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2409" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2429" sqref="B2429"/>
+    <sheetView tabSelected="1" topLeftCell="A677" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B905" sqref="B905"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14088,289 +15168,270 @@
         <v>135</v>
       </c>
     </row>
+    <row r="892" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>133</v>
+      </c>
+      <c r="B892" t="s">
+        <v>691</v>
+      </c>
+      <c r="D892">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="893" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>456</v>
+      </c>
+      <c r="B893" t="s">
+        <v>491</v>
+      </c>
+    </row>
     <row r="894" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="B894" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D894">
         <v>4</v>
       </c>
+      <c r="E894" t="s">
+        <v>735</v>
+      </c>
+      <c r="F894" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="895" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
-        <v>456</v>
+        <v>67</v>
       </c>
       <c r="B895" t="s">
-        <v>491</v>
+        <v>693</v>
+      </c>
+      <c r="D895">
+        <v>4</v>
+      </c>
+      <c r="E895" t="s">
+        <v>736</v>
+      </c>
+      <c r="F895" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="896" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
-        <v>66</v>
-      </c>
-      <c r="B896" t="s">
-        <v>692</v>
-      </c>
-      <c r="D896">
-        <v>4</v>
-      </c>
-      <c r="E896" t="s">
-        <v>735</v>
-      </c>
-      <c r="F896" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="897" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
-        <v>67</v>
+        <v>456</v>
       </c>
       <c r="B897" t="s">
-        <v>693</v>
-      </c>
-      <c r="D897">
-        <v>4</v>
-      </c>
-      <c r="E897" t="s">
-        <v>736</v>
-      </c>
-      <c r="F897" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="898" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
-        <v>637</v>
+        <v>134</v>
+      </c>
+      <c r="B898" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="899" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="B899" t="s">
-        <v>696</v>
+        <v>694</v>
+      </c>
+      <c r="D899">
+        <v>4</v>
+      </c>
+      <c r="E899" t="s">
+        <v>737</v>
+      </c>
+      <c r="F899" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="900" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
-        <v>11</v>
-      </c>
-      <c r="B900" t="s">
-        <v>694</v>
-      </c>
-      <c r="D900">
-        <v>4</v>
-      </c>
-      <c r="E900" t="s">
-        <v>737</v>
-      </c>
-      <c r="F900" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="901" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
-        <v>134</v>
-      </c>
-      <c r="B901" t="s">
-        <v>695</v>
+        <v>460</v>
       </c>
     </row>
     <row r="902" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
-        <v>11</v>
-      </c>
-      <c r="B902" t="s">
-        <v>695</v>
-      </c>
-      <c r="D902">
-        <v>4</v>
-      </c>
-      <c r="E902" t="s">
-        <v>738</v>
-      </c>
-      <c r="F902" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
     </row>
     <row r="903" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A903" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="905" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A905" t="s">
-        <v>133</v>
-      </c>
-      <c r="B905" t="s">
-        <v>696</v>
-      </c>
-      <c r="D905">
+        <v>11</v>
+      </c>
+      <c r="B903" t="s">
+        <v>694</v>
+      </c>
+      <c r="D903">
         <v>4</v>
       </c>
-    </row>
-    <row r="906" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A906" t="s">
-        <v>66</v>
-      </c>
-      <c r="B906" t="s">
-        <v>1284</v>
-      </c>
-      <c r="D906">
-        <v>4</v>
-      </c>
-      <c r="E906" t="s">
-        <v>739</v>
-      </c>
-      <c r="F906" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="907" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A907" t="s">
-        <v>135</v>
+      <c r="E903" t="s">
+        <v>737</v>
+      </c>
+      <c r="F903" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="904" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="908" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
+        <v>134</v>
+      </c>
+      <c r="B908" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="909" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B909" t="s">
-        <v>705</v>
+        <v>695</v>
       </c>
       <c r="D909">
         <v>4</v>
       </c>
+      <c r="E909" t="s">
+        <v>738</v>
+      </c>
+      <c r="F909" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="910" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
-        <v>456</v>
-      </c>
-      <c r="B910" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="911" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A911" t="s">
-        <v>67</v>
-      </c>
-      <c r="B911" t="s">
-        <v>706</v>
-      </c>
-      <c r="D911">
-        <v>4</v>
-      </c>
-      <c r="E911" t="s">
-        <v>740</v>
-      </c>
-      <c r="F911" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="912" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A912" t="s">
-        <v>637</v>
+        <v>133</v>
+      </c>
+      <c r="B912" t="s">
+        <v>696</v>
+      </c>
+      <c r="D912">
+        <v>4</v>
       </c>
     </row>
     <row r="913" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A913" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="B913" t="s">
-        <v>66</v>
+        <v>1284</v>
+      </c>
+      <c r="D913">
+        <v>4</v>
+      </c>
+      <c r="E913" t="s">
+        <v>739</v>
+      </c>
+      <c r="F913" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="914" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A914" t="s">
-        <v>66</v>
-      </c>
-      <c r="B914" t="s">
-        <v>707</v>
-      </c>
-      <c r="D914">
-        <v>4</v>
-      </c>
-      <c r="E914" t="s">
-        <v>741</v>
-      </c>
-      <c r="F914" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="915" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A915" t="s">
-        <v>637</v>
+        <v>135</v>
       </c>
     </row>
     <row r="916" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A916" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="917" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>133</v>
+      </c>
+      <c r="B916" t="s">
+        <v>705</v>
+      </c>
+      <c r="D916">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="917" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A917" t="s">
+        <v>456</v>
+      </c>
+      <c r="B917" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="918" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A918" t="s">
+        <v>67</v>
+      </c>
+      <c r="B918" t="s">
+        <v>706</v>
+      </c>
+      <c r="D918">
+        <v>4</v>
+      </c>
+      <c r="E918" t="s">
+        <v>740</v>
+      </c>
+      <c r="F918" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="919" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A919" t="s">
-        <v>133</v>
-      </c>
-      <c r="B919" t="s">
-        <v>695</v>
-      </c>
-      <c r="D919">
-        <v>4</v>
+        <v>637</v>
       </c>
     </row>
     <row r="920" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A920" t="s">
-        <v>11</v>
+        <v>456</v>
       </c>
       <c r="B920" t="s">
-        <v>697</v>
-      </c>
-      <c r="D920">
-        <v>4</v>
-      </c>
-      <c r="E920" t="s">
-        <v>742</v>
-      </c>
-      <c r="F920" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="921" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="B921" t="s">
-        <v>67</v>
+        <v>707</v>
+      </c>
+      <c r="D921">
+        <v>4</v>
+      </c>
+      <c r="E921" t="s">
+        <v>741</v>
+      </c>
+      <c r="F921" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="922" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
-        <v>67</v>
-      </c>
-      <c r="B922" t="s">
-        <v>698</v>
-      </c>
-      <c r="D922">
-        <v>4</v>
-      </c>
-      <c r="E922" t="s">
-        <v>743</v>
-      </c>
-      <c r="F922" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="923" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A923" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="924" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A924" t="s">
         <v>135</v>
       </c>
     </row>
@@ -14379,7 +15440,7 @@
         <v>133</v>
       </c>
       <c r="B926" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D926">
         <v>4</v>
@@ -14387,16 +15448,16 @@
     </row>
     <row r="927" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A927" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="B927" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D927">
         <v>4</v>
       </c>
       <c r="E927" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F927" t="s">
         <v>2</v>
@@ -14404,164 +15465,161 @@
     </row>
     <row r="928" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A928" t="s">
-        <v>135</v>
+        <v>456</v>
+      </c>
+      <c r="B928" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="929" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A929" t="s">
+        <v>67</v>
+      </c>
+      <c r="B929" t="s">
+        <v>698</v>
+      </c>
+      <c r="D929">
+        <v>4</v>
+      </c>
+      <c r="E929" t="s">
+        <v>743</v>
+      </c>
+      <c r="F929" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="930" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A930" t="s">
-        <v>133</v>
-      </c>
-      <c r="B930" t="s">
-        <v>701</v>
-      </c>
-      <c r="D930">
-        <v>4</v>
+        <v>637</v>
       </c>
     </row>
     <row r="931" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A931" t="s">
-        <v>68</v>
-      </c>
-      <c r="B931" t="s">
-        <v>700</v>
-      </c>
-      <c r="D931">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="933" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A933" t="s">
+        <v>133</v>
+      </c>
+      <c r="B933" t="s">
+        <v>699</v>
+      </c>
+      <c r="D933">
         <v>4</v>
-      </c>
-      <c r="E931" t="s">
-        <v>745</v>
-      </c>
-      <c r="F931" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="932" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A932" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="934" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A934" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="B934" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D934">
         <v>4</v>
       </c>
+      <c r="E934" t="s">
+        <v>744</v>
+      </c>
+      <c r="F934" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="935" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A935" t="s">
-        <v>68</v>
-      </c>
-      <c r="B935" t="s">
-        <v>704</v>
-      </c>
-      <c r="D935">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="937" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A937" t="s">
+        <v>133</v>
+      </c>
+      <c r="B937" t="s">
+        <v>701</v>
+      </c>
+      <c r="D937">
         <v>4</v>
-      </c>
-      <c r="E935" t="s">
-        <v>746</v>
-      </c>
-      <c r="F935" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="936" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A936" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="938" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A938" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="B938" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D938">
         <v>4</v>
       </c>
+      <c r="E938" t="s">
+        <v>745</v>
+      </c>
+      <c r="F938" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="939" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A939" t="s">
-        <v>68</v>
-      </c>
-      <c r="B939" t="s">
-        <v>704</v>
-      </c>
-      <c r="D939">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="941" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A941" t="s">
+        <v>133</v>
+      </c>
+      <c r="B941" t="s">
+        <v>702</v>
+      </c>
+      <c r="D941">
         <v>4</v>
-      </c>
-      <c r="E939" t="s">
-        <v>747</v>
-      </c>
-      <c r="F939" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="940" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A940" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="942" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A942" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="B942" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D942">
         <v>4</v>
       </c>
+      <c r="E942" t="s">
+        <v>746</v>
+      </c>
+      <c r="F942" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="943" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A943" t="s">
-        <v>134</v>
-      </c>
-      <c r="B943" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="944" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A944" t="s">
-        <v>11</v>
-      </c>
-      <c r="B944" t="s">
-        <v>217</v>
-      </c>
-      <c r="D944">
-        <v>4</v>
-      </c>
-      <c r="E944" t="s">
-        <v>711</v>
-      </c>
-      <c r="F944" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="945" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A945" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B945" t="s">
-        <v>710</v>
+        <v>703</v>
+      </c>
+      <c r="D945">
+        <v>4</v>
       </c>
     </row>
     <row r="946" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A946" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B946" t="s">
-        <v>227</v>
+        <v>704</v>
       </c>
       <c r="D946">
         <v>4</v>
       </c>
       <c r="E946" t="s">
-        <v>712</v>
+        <v>747</v>
       </c>
       <c r="F946" t="s">
         <v>2</v>
@@ -14577,7 +15635,7 @@
         <v>133</v>
       </c>
       <c r="B949" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D949">
         <v>4</v>
@@ -14585,24 +15643,24 @@
     </row>
     <row r="950" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A950" t="s">
-        <v>456</v>
+        <v>134</v>
       </c>
       <c r="B950" t="s">
-        <v>67</v>
+        <v>709</v>
       </c>
     </row>
     <row r="951" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A951" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B951" t="s">
-        <v>713</v>
+        <v>217</v>
       </c>
       <c r="D951">
         <v>4</v>
       </c>
       <c r="E951" t="s">
-        <v>748</v>
+        <v>711</v>
       </c>
       <c r="F951" t="s">
         <v>2</v>
@@ -14610,73 +15668,65 @@
     </row>
     <row r="952" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A952" t="s">
-        <v>637</v>
+        <v>134</v>
+      </c>
+      <c r="B952" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="953" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A953" t="s">
-        <v>456</v>
+        <v>11</v>
       </c>
       <c r="B953" t="s">
-        <v>66</v>
+        <v>227</v>
+      </c>
+      <c r="D953">
+        <v>4</v>
+      </c>
+      <c r="E953" t="s">
+        <v>712</v>
+      </c>
+      <c r="F953" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="954" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A954" t="s">
-        <v>66</v>
-      </c>
-      <c r="B954" t="s">
-        <v>714</v>
-      </c>
-      <c r="D954">
-        <v>4</v>
-      </c>
-      <c r="E954" t="s">
-        <v>749</v>
-      </c>
-      <c r="F954" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="955" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A955" t="s">
-        <v>66</v>
-      </c>
-      <c r="B955" t="s">
-        <v>715</v>
-      </c>
-      <c r="D955">
-        <v>4</v>
-      </c>
-      <c r="E955" t="s">
-        <v>750</v>
+        <v>135</v>
       </c>
     </row>
     <row r="956" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A956" t="s">
-        <v>637</v>
+        <v>133</v>
+      </c>
+      <c r="B956" t="s">
+        <v>709</v>
+      </c>
+      <c r="D956">
+        <v>4</v>
       </c>
     </row>
     <row r="957" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A957" t="s">
-        <v>1731</v>
+        <v>456</v>
       </c>
       <c r="B957" t="s">
-        <v>708</v>
+        <v>67</v>
       </c>
     </row>
     <row r="958" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A958" t="s">
-        <v>1732</v>
+        <v>67</v>
       </c>
       <c r="B958" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="D958">
         <v>4</v>
       </c>
       <c r="E958" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="F958" t="s">
         <v>2</v>
@@ -14684,90 +15734,101 @@
     </row>
     <row r="959" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A959" t="s">
-        <v>1731</v>
-      </c>
-      <c r="B959" t="s">
-        <v>718</v>
+        <v>637</v>
       </c>
     </row>
     <row r="960" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A960" t="s">
-        <v>11</v>
+        <v>456</v>
       </c>
       <c r="B960" t="s">
-        <v>1733</v>
-      </c>
-      <c r="D960">
-        <v>4</v>
-      </c>
-      <c r="E960" t="s">
-        <v>609</v>
-      </c>
-      <c r="F960" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="961" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A961" t="s">
-        <v>135</v>
+        <v>66</v>
+      </c>
+      <c r="B961" t="s">
+        <v>714</v>
+      </c>
+      <c r="D961">
+        <v>4</v>
+      </c>
+      <c r="E961" t="s">
+        <v>749</v>
+      </c>
+      <c r="F961" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="962" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A962" t="s">
+        <v>66</v>
+      </c>
+      <c r="B962" t="s">
+        <v>715</v>
+      </c>
+      <c r="D962">
+        <v>4</v>
+      </c>
+      <c r="E962" t="s">
+        <v>750</v>
       </c>
     </row>
     <row r="963" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A963" t="s">
-        <v>133</v>
-      </c>
-      <c r="B963" t="s">
-        <v>718</v>
-      </c>
-      <c r="D963">
-        <v>4</v>
+        <v>637</v>
       </c>
     </row>
     <row r="964" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A964" t="s">
-        <v>66</v>
+        <v>1731</v>
       </c>
       <c r="B964" t="s">
-        <v>720</v>
-      </c>
-      <c r="D964">
-        <v>4</v>
-      </c>
-      <c r="E964" t="s">
-        <v>752</v>
-      </c>
-      <c r="F964" t="s">
-        <v>2</v>
+        <v>708</v>
       </c>
     </row>
     <row r="965" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A965" t="s">
-        <v>456</v>
+        <v>1732</v>
       </c>
       <c r="B965" t="s">
-        <v>690</v>
+        <v>716</v>
+      </c>
+      <c r="D965">
+        <v>4</v>
+      </c>
+      <c r="E965" t="s">
+        <v>751</v>
+      </c>
+      <c r="F965" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="966" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A966" t="s">
-        <v>67</v>
+        <v>1731</v>
       </c>
       <c r="B966" t="s">
-        <v>719</v>
-      </c>
-      <c r="D966">
-        <v>4</v>
-      </c>
-      <c r="E966" t="s">
-        <v>753</v>
-      </c>
-      <c r="F966" t="s">
-        <v>2</v>
+        <v>718</v>
       </c>
     </row>
     <row r="967" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A967" t="s">
-        <v>637</v>
+        <v>11</v>
+      </c>
+      <c r="B967" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D967">
+        <v>4</v>
+      </c>
+      <c r="E967" t="s">
+        <v>609</v>
+      </c>
+      <c r="F967" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="968" spans="1:6" x14ac:dyDescent="0.25">
@@ -14780,7 +15841,7 @@
         <v>133</v>
       </c>
       <c r="B970" t="s">
-        <v>710</v>
+        <v>718</v>
       </c>
       <c r="D970">
         <v>4</v>
@@ -14788,27 +15849,27 @@
     </row>
     <row r="971" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A971" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="B971" t="s">
-        <v>690</v>
+        <v>720</v>
+      </c>
+      <c r="D971">
+        <v>4</v>
+      </c>
+      <c r="E971" t="s">
+        <v>752</v>
+      </c>
+      <c r="F971" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="972" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A972" t="s">
-        <v>67</v>
+        <v>456</v>
       </c>
       <c r="B972" t="s">
-        <v>721</v>
-      </c>
-      <c r="D972">
-        <v>4</v>
-      </c>
-      <c r="E972" t="s">
-        <v>754</v>
-      </c>
-      <c r="F972" t="s">
-        <v>2</v>
+        <v>690</v>
       </c>
     </row>
     <row r="973" spans="1:6" x14ac:dyDescent="0.25">
@@ -14816,13 +15877,13 @@
         <v>67</v>
       </c>
       <c r="B973" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="D973">
         <v>4</v>
       </c>
       <c r="E973" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F973" t="s">
         <v>2</v>
@@ -14835,122 +15896,185 @@
     </row>
     <row r="975" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A975" t="s">
-        <v>68</v>
-      </c>
-      <c r="B975" t="s">
-        <v>722</v>
-      </c>
-      <c r="D975">
-        <v>4</v>
-      </c>
-      <c r="E975" t="s">
-        <v>756</v>
-      </c>
-      <c r="F975" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="976" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A976" t="s">
-        <v>456</v>
-      </c>
-      <c r="B976" t="s">
-        <v>724</v>
+        <v>135</v>
       </c>
     </row>
     <row r="977" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A977" t="s">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="B977" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
       <c r="D977">
         <v>4</v>
       </c>
-      <c r="E977" t="s">
-        <v>757</v>
-      </c>
-      <c r="F977" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="978" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A978" t="s">
-        <v>67</v>
+        <v>456</v>
       </c>
       <c r="B978" t="s">
-        <v>725</v>
-      </c>
-      <c r="D978">
-        <v>4</v>
-      </c>
-      <c r="E978" t="s">
-        <v>758</v>
+        <v>690</v>
       </c>
     </row>
     <row r="979" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A979" t="s">
-        <v>637</v>
+        <v>67</v>
+      </c>
+      <c r="B979" t="s">
+        <v>721</v>
+      </c>
+      <c r="D979">
+        <v>4</v>
+      </c>
+      <c r="E979" t="s">
+        <v>754</v>
+      </c>
+      <c r="F979" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="980" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A980" t="s">
-        <v>456</v>
+        <v>67</v>
       </c>
       <c r="B980" t="s">
-        <v>66</v>
+        <v>728</v>
+      </c>
+      <c r="D980">
+        <v>4</v>
+      </c>
+      <c r="E980" t="s">
+        <v>755</v>
+      </c>
+      <c r="F980" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="981" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A981" t="s">
-        <v>66</v>
-      </c>
-      <c r="B981" t="s">
-        <v>723</v>
-      </c>
-      <c r="D981">
-        <v>4</v>
-      </c>
-      <c r="E981" t="s">
-        <v>757</v>
-      </c>
-      <c r="F981" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="982" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A982" t="s">
-        <v>637</v>
+        <v>68</v>
+      </c>
+      <c r="B982" t="s">
+        <v>722</v>
+      </c>
+      <c r="D982">
+        <v>4</v>
+      </c>
+      <c r="E982" t="s">
+        <v>756</v>
+      </c>
+      <c r="F982" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="983" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A983" t="s">
-        <v>726</v>
+        <v>456</v>
       </c>
       <c r="B983" t="s">
-        <v>727</v>
-      </c>
-      <c r="D983">
-        <v>4</v>
-      </c>
-      <c r="E983" t="s">
-        <v>759</v>
-      </c>
-      <c r="F983" t="s">
-        <v>2</v>
+        <v>724</v>
       </c>
     </row>
     <row r="984" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A984" t="s">
-        <v>1031</v>
+        <v>66</v>
       </c>
       <c r="B984" t="s">
-        <v>729</v>
+        <v>723</v>
+      </c>
+      <c r="D984">
+        <v>4</v>
+      </c>
+      <c r="E984" t="s">
+        <v>757</v>
+      </c>
+      <c r="F984" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="985" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A985" t="s">
+        <v>67</v>
+      </c>
+      <c r="B985" t="s">
+        <v>725</v>
+      </c>
+      <c r="D985">
+        <v>4</v>
+      </c>
+      <c r="E985" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="986" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A986" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="987" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A987" t="s">
+        <v>456</v>
+      </c>
+      <c r="B987" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="988" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A988" t="s">
+        <v>66</v>
+      </c>
+      <c r="B988" t="s">
+        <v>723</v>
+      </c>
+      <c r="D988">
+        <v>4</v>
+      </c>
+      <c r="E988" t="s">
+        <v>757</v>
+      </c>
+      <c r="F988" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="989" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A989" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="990" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A990" t="s">
+        <v>726</v>
+      </c>
+      <c r="B990" t="s">
+        <v>727</v>
+      </c>
+      <c r="D990">
+        <v>4</v>
+      </c>
+      <c r="E990" t="s">
+        <v>759</v>
+      </c>
+      <c r="F990" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="991" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A991" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B991" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="992" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A992" t="s">
         <v>135</v>
       </c>
     </row>
@@ -17623,163 +18747,87 @@
     </row>
     <row r="1277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1277" t="s">
-        <v>134</v>
+        <v>456</v>
       </c>
       <c r="B1277" t="s">
-        <v>907</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1278" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="B1278" t="s">
-        <v>909</v>
-      </c>
-      <c r="D1278">
-        <v>5</v>
-      </c>
-      <c r="E1278" t="s">
-        <v>998</v>
-      </c>
-      <c r="F1278" t="s">
-        <v>2</v>
+        <v>907</v>
       </c>
     </row>
     <row r="1279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1279" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="B1279" t="s">
-        <v>908</v>
+        <v>909</v>
+      </c>
+      <c r="D1279">
+        <v>5</v>
+      </c>
+      <c r="E1279" t="s">
+        <v>998</v>
+      </c>
+      <c r="F1279" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1280" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1280" t="s">
-        <v>910</v>
-      </c>
-      <c r="D1280">
-        <v>5</v>
-      </c>
-      <c r="E1280" t="s">
-        <v>999</v>
-      </c>
-      <c r="F1280" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="1281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1281" t="s">
-        <v>135</v>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1282" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="1283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1283" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B1283" t="s">
-        <v>907</v>
-      </c>
-      <c r="D1283">
-        <v>5</v>
+        <v>909</v>
       </c>
     </row>
     <row r="1284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1284" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="B1284" t="s">
-        <v>1284</v>
-      </c>
-      <c r="D1284">
-        <v>5</v>
-      </c>
-      <c r="E1284" t="s">
-        <v>1000</v>
-      </c>
-      <c r="F1284" t="s">
-        <v>2</v>
+        <v>908</v>
       </c>
     </row>
     <row r="1285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1285" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="1287" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1287" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1287" t="s">
-        <v>908</v>
-      </c>
-      <c r="D1287">
+        <v>11</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>910</v>
+      </c>
+      <c r="D1285">
         <v>5</v>
       </c>
-    </row>
-    <row r="1288" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1288" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1288" t="s">
-        <v>911</v>
-      </c>
-      <c r="D1288">
-        <v>5</v>
-      </c>
-      <c r="E1288" t="s">
+      <c r="E1285" t="s">
         <v>999</v>
       </c>
-      <c r="F1288" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1289" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1289" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="1291" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1291" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1291" t="s">
-        <v>912</v>
-      </c>
-      <c r="D1291">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="1292" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1292" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1292" t="s">
-        <v>1725</v>
-      </c>
-      <c r="D1292">
-        <v>5</v>
-      </c>
-      <c r="E1292" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F1292" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1293" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1293" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B1293" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="1294" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1294" t="s">
+      <c r="F1285" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1286" t="s">
         <v>135</v>
       </c>
     </row>
@@ -17788,7 +18836,7 @@
         <v>133</v>
       </c>
       <c r="B1301" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="D1301">
         <v>5</v>
@@ -17796,16 +18844,16 @@
     </row>
     <row r="1302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1302" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B1302" t="s">
-        <v>922</v>
+        <v>1284</v>
       </c>
       <c r="D1302">
         <v>5</v>
       </c>
       <c r="E1302" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="F1302" t="s">
         <v>2</v>
@@ -17821,7 +18869,7 @@
         <v>133</v>
       </c>
       <c r="B1305" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="D1305">
         <v>5</v>
@@ -17829,16 +18877,16 @@
     </row>
     <row r="1306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1306" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="B1306" t="s">
-        <v>923</v>
+        <v>911</v>
       </c>
       <c r="D1306">
         <v>5</v>
       </c>
       <c r="E1306" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
       <c r="F1306" t="s">
         <v>2</v>
@@ -17851,10 +18899,10 @@
     </row>
     <row r="1309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1309" t="s">
-        <v>915</v>
+        <v>133</v>
       </c>
       <c r="B1309" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="D1309">
         <v>5</v>
@@ -17862,183 +18910,142 @@
     </row>
     <row r="1310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1310" t="s">
-        <v>918</v>
+        <v>71</v>
       </c>
       <c r="B1310" t="s">
-        <v>917</v>
+        <v>1725</v>
+      </c>
+      <c r="D1310">
+        <v>5</v>
       </c>
       <c r="E1310" t="s">
-        <v>1005</v>
+        <v>1003</v>
+      </c>
+      <c r="F1310" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1311" t="s">
-        <v>456</v>
+        <v>1031</v>
       </c>
       <c r="B1311" t="s">
-        <v>67</v>
+        <v>916</v>
       </c>
     </row>
     <row r="1312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1312" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1312" t="s">
-        <v>919</v>
-      </c>
-      <c r="D1312">
-        <v>5</v>
-      </c>
-      <c r="E1312" t="s">
-        <v>1006</v>
-      </c>
-      <c r="F1312" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1313" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1313" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="1314" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1314" t="s">
-        <v>456</v>
-      </c>
-      <c r="B1314" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="1315" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1315" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1315" t="s">
-        <v>919</v>
-      </c>
-      <c r="D1315">
-        <v>5</v>
-      </c>
-      <c r="E1315" t="s">
-        <v>1007</v>
-      </c>
-      <c r="F1315" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1316" t="s">
-        <v>637</v>
+        <v>133</v>
+      </c>
+      <c r="B1316" t="s">
+        <v>913</v>
+      </c>
+      <c r="D1316">
+        <v>5</v>
       </c>
     </row>
     <row r="1317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1317" t="s">
-        <v>456</v>
+        <v>71</v>
       </c>
       <c r="B1317" t="s">
-        <v>68</v>
+        <v>922</v>
+      </c>
+      <c r="D1317">
+        <v>5</v>
+      </c>
+      <c r="E1317" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F1317" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1318" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1318" t="s">
-        <v>920</v>
-      </c>
-      <c r="D1318">
-        <v>5</v>
-      </c>
-      <c r="E1318" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F1318" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1319" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1319" t="s">
-        <v>637</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1320" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="B1320" t="s">
-        <v>921</v>
+        <v>914</v>
       </c>
       <c r="D1320">
         <v>5</v>
       </c>
-      <c r="E1320" t="s">
-        <v>1009</v>
-      </c>
-      <c r="F1320" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="1321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1321" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1321" t="s">
+        <v>923</v>
+      </c>
+      <c r="D1321">
+        <v>5</v>
+      </c>
+      <c r="E1321" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F1321" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1322" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="1323" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1323" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1323" t="s">
-        <v>928</v>
-      </c>
-      <c r="D1323">
-        <v>5</v>
       </c>
     </row>
     <row r="1324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1324" t="s">
-        <v>134</v>
+        <v>915</v>
       </c>
       <c r="B1324" t="s">
-        <v>931</v>
+        <v>916</v>
+      </c>
+      <c r="D1324">
+        <v>5</v>
       </c>
     </row>
     <row r="1325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1325" t="s">
-        <v>11</v>
+        <v>918</v>
       </c>
       <c r="B1325" t="s">
-        <v>222</v>
-      </c>
-      <c r="D1325">
-        <v>5</v>
+        <v>917</v>
       </c>
       <c r="E1325" t="s">
-        <v>930</v>
-      </c>
-      <c r="F1325" t="s">
-        <v>2</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="1326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1326" t="s">
-        <v>134</v>
+        <v>456</v>
       </c>
       <c r="B1326" t="s">
-        <v>932</v>
+        <v>67</v>
       </c>
     </row>
     <row r="1327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1327" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B1327" t="s">
-        <v>227</v>
+        <v>919</v>
       </c>
       <c r="D1327">
         <v>5</v>
       </c>
       <c r="E1327" t="s">
-        <v>929</v>
+        <v>1006</v>
       </c>
       <c r="F1327" t="s">
         <v>2</v>
@@ -18046,70 +19053,81 @@
     </row>
     <row r="1328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1328" t="s">
-        <v>135</v>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1329" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1329" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="1330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1330" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="B1330" t="s">
-        <v>931</v>
+        <v>919</v>
       </c>
       <c r="D1330">
         <v>5</v>
       </c>
+      <c r="E1330" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F1330" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="1331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1331" t="s">
-        <v>456</v>
-      </c>
-      <c r="B1331" t="s">
-        <v>68</v>
+        <v>637</v>
       </c>
     </row>
     <row r="1332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1332" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1332" t="s">
         <v>68</v>
-      </c>
-      <c r="B1332" t="s">
-        <v>933</v>
-      </c>
-      <c r="D1332">
-        <v>5</v>
-      </c>
-      <c r="E1332" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F1332" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="1333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1333" t="s">
-        <v>637</v>
+        <v>68</v>
+      </c>
+      <c r="B1333" t="s">
+        <v>920</v>
+      </c>
+      <c r="D1333">
+        <v>5</v>
+      </c>
+      <c r="E1333" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F1333" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1334" t="s">
-        <v>456</v>
-      </c>
-      <c r="B1334" t="s">
-        <v>67</v>
+        <v>637</v>
       </c>
     </row>
     <row r="1335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1335" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B1335" t="s">
-        <v>934</v>
+        <v>921</v>
       </c>
       <c r="D1335">
         <v>5</v>
       </c>
       <c r="E1335" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="F1335" t="s">
         <v>2</v>
@@ -18117,45 +19135,43 @@
     </row>
     <row r="1336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1336" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="1337" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1337" t="s">
-        <v>456</v>
-      </c>
-      <c r="B1337" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1338" t="s">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="B1338" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="D1338">
         <v>5</v>
       </c>
-      <c r="E1338" t="s">
-        <v>1012</v>
-      </c>
-      <c r="F1338" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="1339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1339" t="s">
-        <v>637</v>
+        <v>134</v>
+      </c>
+      <c r="B1339" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="1340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1340" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="B1340" t="s">
-        <v>935</v>
+        <v>222</v>
+      </c>
+      <c r="D1340">
+        <v>5</v>
+      </c>
+      <c r="E1340" t="s">
+        <v>930</v>
+      </c>
+      <c r="F1340" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1341" spans="1:6" x14ac:dyDescent="0.25">
@@ -18163,7 +19179,7 @@
         <v>134</v>
       </c>
       <c r="B1341" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
     </row>
     <row r="1342" spans="1:6" x14ac:dyDescent="0.25">
@@ -18171,13 +19187,13 @@
         <v>11</v>
       </c>
       <c r="B1342" t="s">
-        <v>716</v>
+        <v>227</v>
       </c>
       <c r="D1342">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1342" t="s">
-        <v>751</v>
+        <v>929</v>
       </c>
       <c r="F1342" t="s">
         <v>2</v>
@@ -18185,139 +19201,138 @@
     </row>
     <row r="1343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1343" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1343" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="1344" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1344" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1344" t="s">
-        <v>717</v>
-      </c>
-      <c r="D1344">
-        <v>4</v>
-      </c>
-      <c r="E1344" t="s">
-        <v>609</v>
-      </c>
-      <c r="F1344" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1345" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="B1345" t="s">
+        <v>931</v>
+      </c>
+      <c r="D1345">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1346" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1346" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="1347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1347" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="B1347" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="D1347">
         <v>5</v>
       </c>
+      <c r="E1347" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F1347" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="1348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1348" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1348" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1348">
-        <v>5</v>
-      </c>
-      <c r="E1348" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F1348" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="1349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1349" t="s">
-        <v>135</v>
+        <v>456</v>
+      </c>
+      <c r="B1349" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1350" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1350" t="s">
+        <v>934</v>
+      </c>
+      <c r="D1350">
+        <v>5</v>
+      </c>
+      <c r="E1350" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F1350" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1351" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1351" t="s">
-        <v>932</v>
-      </c>
-      <c r="D1351">
-        <v>5</v>
+        <v>637</v>
       </c>
     </row>
     <row r="1352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1352" t="s">
-        <v>71</v>
+        <v>456</v>
       </c>
       <c r="B1352" t="s">
-        <v>938</v>
-      </c>
-      <c r="E1352" t="s">
-        <v>1014</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1353" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="B1353" t="s">
-        <v>67</v>
+        <v>936</v>
+      </c>
+      <c r="D1353">
+        <v>5</v>
+      </c>
+      <c r="E1353" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F1353" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1354" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1354" t="s">
-        <v>939</v>
-      </c>
-      <c r="D1354">
-        <v>5</v>
-      </c>
-      <c r="E1354" t="s">
-        <v>1015</v>
-      </c>
-      <c r="F1354" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="1355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1355" t="s">
-        <v>637</v>
+        <v>71</v>
+      </c>
+      <c r="B1355" t="s">
+        <v>935</v>
       </c>
     </row>
     <row r="1356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1356" t="s">
-        <v>456</v>
+        <v>134</v>
       </c>
       <c r="B1356" t="s">
-        <v>68</v>
+        <v>928</v>
       </c>
     </row>
     <row r="1357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1357" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="B1357" t="s">
-        <v>940</v>
+        <v>716</v>
       </c>
       <c r="D1357">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1357" t="s">
-        <v>1016</v>
+        <v>751</v>
       </c>
       <c r="F1357" t="s">
         <v>2</v>
@@ -18325,80 +19340,57 @@
     </row>
     <row r="1358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1358" t="s">
-        <v>637</v>
+        <v>134</v>
+      </c>
+      <c r="B1358" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="1359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1359" t="s">
-        <v>456</v>
+        <v>11</v>
       </c>
       <c r="B1359" t="s">
-        <v>66</v>
+        <v>717</v>
+      </c>
+      <c r="D1359">
+        <v>4</v>
+      </c>
+      <c r="E1359" t="s">
+        <v>609</v>
+      </c>
+      <c r="F1359" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1360" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1360" t="s">
-        <v>941</v>
-      </c>
-      <c r="D1360">
-        <v>5</v>
-      </c>
-      <c r="E1360" t="s">
-        <v>1017</v>
-      </c>
-      <c r="F1360" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1361" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1361" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1361" t="s">
-        <v>942</v>
-      </c>
-      <c r="D1361">
-        <v>5</v>
-      </c>
-      <c r="E1361" t="s">
-        <v>1018</v>
-      </c>
-      <c r="F1361" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1362" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="B1362" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="D1362">
         <v>5</v>
       </c>
-      <c r="E1362" t="s">
-        <v>1001</v>
-      </c>
-      <c r="F1362" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="1363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1363" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B1363" t="s">
-        <v>944</v>
+        <v>288</v>
       </c>
       <c r="D1363">
         <v>5</v>
       </c>
       <c r="E1363" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
       <c r="F1363" t="s">
         <v>2</v>
@@ -18406,80 +19398,51 @@
     </row>
     <row r="1364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1364" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1364" t="s">
-        <v>945</v>
-      </c>
-      <c r="D1364">
-        <v>5</v>
-      </c>
-      <c r="E1364" t="s">
-        <v>1020</v>
-      </c>
-      <c r="F1364" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1365" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1365" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1365" t="s">
-        <v>946</v>
-      </c>
-      <c r="D1365">
-        <v>5</v>
-      </c>
-      <c r="E1365" t="s">
-        <v>1021</v>
-      </c>
-      <c r="F1365" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1366" t="s">
-        <v>637</v>
+        <v>133</v>
+      </c>
+      <c r="B1366" t="s">
+        <v>932</v>
+      </c>
+      <c r="D1366">
+        <v>5</v>
       </c>
     </row>
     <row r="1367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1367" t="s">
-        <v>456</v>
+        <v>71</v>
       </c>
       <c r="B1367" t="s">
-        <v>67</v>
+        <v>938</v>
+      </c>
+      <c r="E1367" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="1368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1368" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1368" t="s">
         <v>67</v>
-      </c>
-      <c r="B1368" t="s">
-        <v>947</v>
-      </c>
-      <c r="D1368">
-        <v>5</v>
-      </c>
-      <c r="E1368" t="s">
-        <v>1022</v>
-      </c>
-      <c r="F1368" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="1369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1369" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B1369" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="D1369">
         <v>5</v>
       </c>
       <c r="E1369" t="s">
-        <v>1001</v>
+        <v>1015</v>
       </c>
       <c r="F1369" t="s">
         <v>2</v>
@@ -18487,50 +19450,29 @@
     </row>
     <row r="1370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1370" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1370" t="s">
-        <v>944</v>
-      </c>
-      <c r="D1370">
-        <v>5</v>
-      </c>
-      <c r="E1370" t="s">
-        <v>1019</v>
-      </c>
-      <c r="F1370" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
     </row>
     <row r="1371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1371" t="s">
-        <v>11</v>
+        <v>456</v>
       </c>
       <c r="B1371" t="s">
-        <v>945</v>
-      </c>
-      <c r="D1371">
-        <v>5</v>
-      </c>
-      <c r="E1371" t="s">
-        <v>1020</v>
-      </c>
-      <c r="F1371" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="1372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1372" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B1372" t="s">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="D1372">
         <v>5</v>
       </c>
       <c r="E1372" t="s">
-        <v>1021</v>
+        <v>1016</v>
       </c>
       <c r="F1372" t="s">
         <v>2</v>
@@ -18543,6 +19485,219 @@
     </row>
     <row r="1374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1374" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1374" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1375" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1375" t="s">
+        <v>941</v>
+      </c>
+      <c r="D1375">
+        <v>5</v>
+      </c>
+      <c r="E1375" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F1375" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1376" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1376" t="s">
+        <v>942</v>
+      </c>
+      <c r="D1376">
+        <v>5</v>
+      </c>
+      <c r="E1376" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F1376" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1377" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1377" t="s">
+        <v>943</v>
+      </c>
+      <c r="D1377">
+        <v>5</v>
+      </c>
+      <c r="E1377" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F1377" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1378" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1378" t="s">
+        <v>944</v>
+      </c>
+      <c r="D1378">
+        <v>5</v>
+      </c>
+      <c r="E1378" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F1378" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1379" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1379" t="s">
+        <v>945</v>
+      </c>
+      <c r="D1379">
+        <v>5</v>
+      </c>
+      <c r="E1379" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F1379" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1380" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1380" t="s">
+        <v>946</v>
+      </c>
+      <c r="D1380">
+        <v>5</v>
+      </c>
+      <c r="E1380" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F1380" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1381" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1382" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1382" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1383" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1383" t="s">
+        <v>947</v>
+      </c>
+      <c r="D1383">
+        <v>5</v>
+      </c>
+      <c r="E1383" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F1383" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1384" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1384" t="s">
+        <v>943</v>
+      </c>
+      <c r="D1384">
+        <v>5</v>
+      </c>
+      <c r="E1384" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F1384" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1385" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1385" t="s">
+        <v>944</v>
+      </c>
+      <c r="D1385">
+        <v>5</v>
+      </c>
+      <c r="E1385" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F1385" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1386" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>945</v>
+      </c>
+      <c r="D1386">
+        <v>5</v>
+      </c>
+      <c r="E1386" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F1386" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1387" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1387" t="s">
+        <v>946</v>
+      </c>
+      <c r="D1387">
+        <v>5</v>
+      </c>
+      <c r="E1387" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F1387" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1388" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1389" t="s">
         <v>135</v>
       </c>
     </row>
@@ -26619,50 +27774,192 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:H604 A605:B605 A606:H614 A620:H1048576">
-    <cfRule type="expression" dxfId="27" priority="1">
+  <conditionalFormatting sqref="A1:H604 A605:B605 A606:H614 A620:H896 A898:H899 A897:B897 A1277:B1277 A1278:H1279 A1281 A1284:H1286 A908:H1276 A1301:H1048576 A900:A901">
+    <cfRule type="expression" dxfId="71" priority="45">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="70" priority="46">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="69" priority="47">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="68" priority="48">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="67" priority="49">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="66" priority="50">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="65" priority="51">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="64" priority="52">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="63" priority="53">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="62" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G604 F606:G614 F620:G1048576">
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Final">
+  <conditionalFormatting sqref="F1:G604 F606:G614 F620:G896 F898:G899 F1278:G1279 F1301:G1048576 F1284:G1286 F908:G1276">
+    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="60" priority="55" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1280:B1280">
+    <cfRule type="expression" dxfId="57" priority="35">
+      <formula>LEFT($A1280, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="36">
+      <formula>$A1280="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="37">
+      <formula>$A1280="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="38">
+      <formula>$A1280="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="39">
+      <formula>$A1280="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="40">
+      <formula>$A1280="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="41">
+      <formula>$A1280="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="42">
+      <formula>$A1280="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="43">
+      <formula>$A1280="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="44">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1282:B1283">
+    <cfRule type="expression" dxfId="47" priority="25">
+      <formula>LEFT($A1282, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="26">
+      <formula>$A1282="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="27">
+      <formula>$A1282="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="28">
+      <formula>$A1282="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="29">
+      <formula>$A1282="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="30">
+      <formula>$A1282="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="31">
+      <formula>$A1282="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="32">
+      <formula>$A1282="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>$A1282="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A902:H903">
+    <cfRule type="expression" dxfId="23" priority="11">
+      <formula>LEFT($A902, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="12">
+      <formula>$A902="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="13">
+      <formula>$A902="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="14">
+      <formula>$A902="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="15">
+      <formula>$A902="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="16">
+      <formula>$A902="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="17">
+      <formula>$A902="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>$A902="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="19">
+      <formula>$A902="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="24">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F902:G903">
+    <cfRule type="containsText" dxfId="13" priority="20" operator="containsText" text="Final">
+      <formula>NOT(ISERROR(SEARCH("Final",F902)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="21" operator="containsText" text="Draft">
+      <formula>NOT(ISERROR(SEARCH("Draft",F902)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="22" operator="containsText" text="Placeholder">
+      <formula>NOT(ISERROR(SEARCH("Placeholder",F902)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",F902)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A904">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>LEFT($A904, 2)="//"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="2">
+      <formula>$A904="CHOICE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>$A904="CONVERSATION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>$A904="END"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$A904="GOTO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$A904="IF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>$A904="ELIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>$A904="ELSE"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>$A904="ENDIF"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26773,48 +28070,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="37" priority="1">
       <formula>LEFT($A1, 2)="//"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="36" priority="2">
       <formula>$A1="CHOICE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="35" priority="3">
       <formula>$A1="CONVERSATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="34" priority="4">
       <formula>$A1="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="33" priority="5">
       <formula>$A1="GOTO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="32" priority="6">
       <formula>$A1="IF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="31" priority="7">
       <formula>$A1="ELIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>$A1="ELSE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>$A1="ENDIF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="26">
+    <cfRule type="expression" dxfId="28" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Final">
+    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="Final">
       <formula>NOT(ISERROR(SEARCH("Final",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="Draft">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Draft">
       <formula>NOT(ISERROR(SEARCH("Draft",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="24" operator="containsText" text="Placeholder">
+    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Placeholder">
       <formula>NOT(ISERROR(SEARCH("Placeholder",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26823,6 +28120,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7FA1DABE19A7441B0DD9ECFD97FA9FD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="050f4f45281d41711b3fd526c487e384">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb09cb51-d096-4c65-98ba-548d51d18e12" xmlns:ns4="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70a97b6bbbcf4d804a06f93a6796394b" ns3:_="" ns4:_="">
     <xsd:import namespace="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
@@ -27061,24 +28375,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
+    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fb09cb51-d096-4c65-98ba-548d51d18e12" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E80BA8F-CFA8-4AE9-922C-12206892D807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27095,29 +28417,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA71395-BCBD-4A1E-9A2D-93EE87AC2E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0615C31A-2D0B-447F-BD43-7D2425502AF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb09cb51-d096-4c65-98ba-548d51d18e12"/>
-    <ds:schemaRef ds:uri="4ea2eb1a-06eb-46a9-9e36-de3faac4ce52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>